<commit_message>
Add ranking data for 2025-09-22
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -20,6 +20,7 @@
     <sheet name="2025-09-01" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="2025-09-08" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="2025-09-15" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="2025-09-22" sheetId="15" state="visible" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -4674,22 +4675,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第127話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第135話	ムラ塚先生の憂鬱</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>不徳のギルド</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>河添太一</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第９８話：コインの裏表</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第６９話『岩鬼停止』②</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第40話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第32話：思考を奪う②</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第64話 更衣室の戦いが始まった（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第125話　四騎戦の打ち上げです！</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第38話</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>六志麻あさ 業務用餅 kisui</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第７１話</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第35話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第11話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>美人女上司滝沢さん</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>やんBARU(著者)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第203話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>蜘蛛ですが、なにか？</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第76話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>久遠まこと(著者) 石のやっさん(原作)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第30話</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンの幼なじみ</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>久真やすひさ(著者)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第57話</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>番外編①</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第128話　レムと話してみる（中編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第５２話　暴走を止める器用貧乏（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>不純な彼女達は懺悔しない</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>ポロロッカ(著者)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第31話</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第304話</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第２３食　巨大ヘビモンスターさん、パクパクですわ！（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第139話 よくわからないけれどズゥゥゥンときたみたいです（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>望まぬ不死の冒険者</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>中曽根ハイジ（漫画） 丘野 優（原作） じゃいあん（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第60話　異国の観光客</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第73話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第47話 魔導具師とつながれたもの④</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第41話　奴は帰りたい（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第52話②　最強の武器を手に入れてみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第33話 独身貴族は見積もりを誤る（4）</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第72話(後編) ダリエルの照らした道</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>三吉汐美(著者)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第17話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第84話</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>拷問149</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第82話その3</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第４２話　勇者、六邪神将相手に舐めプしてたら、ピンチになる（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>はぐはぐ(著者)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第85話</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第１９話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第87話　その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>バーサス</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第28話　工場（1）</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>セレビィ量産型(著者)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第22話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>塔の管理をしてみよう</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第92話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>ライブダンジョン！</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第89話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第2話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>異世界でも無難に生きたい症候群</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第31話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第1話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>女子高生の無駄づかい</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>ビーノ(著者)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第135話　きずな</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>路地裏で拾った女の子がバッドエンド後の乙女ゲームのヒロインだった件</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>カボチャマスク(原作) 樋乃えなが(作画) へいろー(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第2話</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>三部べべ(漫画) ねうしとら(原作)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>隣の席のヤンキー清水さんが髪を黒く染めてきた</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>底花(原作) 真田若楓(漫画) ハム(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第11話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第12話　最弱貴族、悪役令嬢と出会う（２）</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>丈(著者)</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第127話</t>
+          <t>211撃目</t>
         </is>
       </c>
     </row>
@@ -4699,17 +5741,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>生徒会にも穴はある！</t>
+          <t>異種族レビュアーズ</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>むちまろ</t>
+          <t>天原(原作) masha(作画)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第135話	ムラ塚先生の憂鬱</t>
+          <t>第87話</t>
         </is>
       </c>
     </row>
@@ -4719,17 +5761,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>不徳のギルド</t>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>河添太一</t>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第９８話：コインの裏表</t>
+          <t>第71話</t>
         </is>
       </c>
     </row>
@@ -4739,17 +5781,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>異世界おじさん</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第６９話『岩鬼停止』②</t>
+          <t>コミックス第14巻発売告知</t>
         </is>
       </c>
     </row>
@@ -4759,17 +5801,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第40話②</t>
+          <t>第32話：思考を奪う③</t>
         </is>
       </c>
     </row>
@@ -4779,17 +5821,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>zunta(作画) はらわたさいぞう(原作)</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第32話：思考を奪う②</t>
+          <t>第６９話『岩鬼停止』③</t>
         </is>
       </c>
     </row>
@@ -4799,17 +5841,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第64話 更衣室の戦いが始まった（２）</t>
+          <t>第5話 前編</t>
         </is>
       </c>
     </row>
@@ -4819,17 +5861,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>須河篤志(著者)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第125話　四騎戦の打ち上げです！</t>
+          <t>第15話後半</t>
         </is>
       </c>
     </row>
@@ -4839,17 +5881,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>六志麻あさ 業務用餅 kisui</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第38話</t>
+          <t>第７２話</t>
         </is>
       </c>
     </row>
@@ -4859,17 +5901,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+          <t>美人女上司滝沢さん</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>六志麻あさ 業務用餅 kisui</t>
+          <t>やんBARU(著者)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第７１話</t>
+          <t>第203話</t>
         </is>
       </c>
     </row>
@@ -4879,17 +5921,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第35話①</t>
+          <t>第126話　王家の立場</t>
         </is>
       </c>
     </row>
@@ -4899,17 +5941,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第11話-1</t>
+          <t>第64話 更衣室の戦いが始まった（２）</t>
         </is>
       </c>
     </row>
@@ -4919,17 +5961,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>美人女上司滝沢さん</t>
+          <t>帰ってください！ 阿久津さん</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>やんBARU(著者)</t>
+          <t>長岡太一(著者)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第203話</t>
+          <t>第196話</t>
         </is>
       </c>
     </row>
@@ -4939,17 +5981,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>蜘蛛ですが、なにか？</t>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第76話その1</t>
+          <t>第78話その2</t>
         </is>
       </c>
     </row>
@@ -4959,17 +6001,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>久遠まこと(著者) 石のやっさん(原作)</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第30話</t>
+          <t>第128話　レムと話してみる（後編）</t>
         </is>
       </c>
     </row>
@@ -4979,17 +6021,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ダンジョンの幼なじみ</t>
+          <t>ダークサモナーとデキている</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>久真やすひさ(著者)</t>
+          <t>車王(著者)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第57話</t>
+          <t>第76話</t>
         </is>
       </c>
     </row>
@@ -4999,17 +6041,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+          <t>蜘蛛ですが、なにか？</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>番外編①</t>
+          <t>第76話その1</t>
         </is>
       </c>
     </row>
@@ -5019,17 +6061,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>異世界魔王と召喚少女の奴隷魔術</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第128話　レムと話してみる（中編）</t>
+          <t>第５２話　暴走を止める器用貧乏（４）</t>
         </is>
       </c>
     </row>
@@ -5039,17 +6081,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第５２話　暴走を止める器用貧乏（３）</t>
+          <t>第48話前編</t>
         </is>
       </c>
     </row>
@@ -5059,17 +6101,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>不純な彼女達は懺悔しない</t>
+          <t>淫獄団地</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ポロロッカ(著者)</t>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第31話</t>
+          <t>第50話（後編）</t>
         </is>
       </c>
     </row>
@@ -5079,17 +6121,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>異世界のんびり農家</t>
+          <t>Ｓ級ギルドを追放されたけど、実は俺だけドラゴンの言葉がわかるので、気付いたときには竜騎士の頂点を極めてました。</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+          <t>ひそな(漫画) 三木なずな(原作) 白狼(キャラクター原案)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第304話</t>
+          <t>第39話-2</t>
         </is>
       </c>
     </row>
@@ -5099,17 +6141,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+          <t>異世界のんびり農家</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>島知宏 音速炒飯 有都あらゆる</t>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第２３食　巨大ヘビモンスターさん、パクパクですわ！（４）</t>
+          <t>第305話</t>
         </is>
       </c>
     </row>
@@ -5119,17 +6161,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第139話 よくわからないけれどズゥゥゥンときたみたいです（１）</t>
+          <t>第80話　先に行く</t>
         </is>
       </c>
     </row>
@@ -5139,17 +6181,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>望まぬ不死の冒険者</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>中曽根ハイジ（漫画） 丘野 優（原作） じゃいあん（キャラクター原案）</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第60話　異国の観光客</t>
+          <t>第73話②</t>
         </is>
       </c>
     </row>
@@ -5159,17 +6201,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>戸崎さんは僕にだけ冷たい</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>saku(著者)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第73話①</t>
+          <t>第29話-1</t>
         </is>
       </c>
     </row>
@@ -5179,17 +6221,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+          <t>濁る瞳で何を願う ハイセルク戦記</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+          <t>トルトネン 創-taro 斎藤八呑</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第47話 魔導具師とつながれたもの④</t>
+          <t>第34話 ダンデューグ城へようこそ</t>
         </is>
       </c>
     </row>
@@ -5199,17 +6241,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+          <t>ニチアサ好きのオタクが悪役生徒に転生した結果、破滅フラグが崩壊していく件について</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+          <t>烏丸英（原作） どんぐりす（漫画）</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第41話　奴は帰りたい（後編）</t>
+          <t>第14話（後編）急襲…事件の始まり</t>
         </is>
       </c>
     </row>
@@ -5219,17 +6261,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第52話②　最強の武器を手に入れてみた</t>
+          <t>第31話</t>
         </is>
       </c>
     </row>
@@ -5239,17 +6281,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>君のラブを見せてくれ！</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>リムコロ(著者)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第33話 独身貴族は見積もりを誤る（4）</t>
+          <t>コミックス第⑤巻発売告知</t>
         </is>
       </c>
     </row>
@@ -5259,17 +6301,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第72話(後編) ダリエルの照らした道</t>
+          <t>第34話 独身貴族は礼の品を贈る（1）</t>
         </is>
       </c>
     </row>
@@ -5279,17 +6321,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>アイドル辞めるけど結婚してくれますか!?</t>
+          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>三吉汐美(著者)</t>
+          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第17話前半</t>
+          <t>第110話：王女に贈る子守歌</t>
         </is>
       </c>
     </row>
@@ -5299,17 +6341,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>くらいあの子としたいこと</t>
+          <t>「おかえり、パパ」</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>碇マナツ(著者)</t>
+          <t>蝉丸</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第84話</t>
+          <t>第28話　帰宅</t>
         </is>
       </c>
     </row>
@@ -5319,17 +6361,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>拷問149</t>
+          <t>第139話 よくわからないけれどズゥゥゥンときたみたいです（２）</t>
         </is>
       </c>
     </row>
@@ -5339,17 +6381,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>聖者無双</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第82話その3</t>
+          <t>第92話　龍と精霊の信仰（後半）</t>
         </is>
       </c>
     </row>
@@ -5369,7 +6411,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第４２話　勇者、六邪神将相手に舐めプしてたら、ピンチになる（２）</t>
+          <t>第４２話　勇者、六邪神将相手に舐めプしてたら、ピンチになる（３）</t>
         </is>
       </c>
     </row>
@@ -5379,17 +6421,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>サーシャちゃんとクラスメイトオタクくん</t>
+          <t>ライドンキング</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>はぐはぐ(著者)</t>
+          <t>馬場康誌</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第85話</t>
+          <t>第83話 大統領と龍の闇卵（前編）</t>
         </is>
       </c>
     </row>
@@ -5399,17 +6441,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>板垣恵介 林たかあき</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第１９話①</t>
+          <t>第54話 イバラの帰り道</t>
         </is>
       </c>
     </row>
@@ -5419,17 +6461,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第87話　その2</t>
+          <t>第6話-2：火蓮の剣</t>
         </is>
       </c>
     </row>
@@ -5439,17 +6481,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>バーサス</t>
+          <t>小林さんちのメイドラゴン</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+          <t>クール教信者</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第28話　工場（1）</t>
+          <t>第150話</t>
         </is>
       </c>
     </row>
@@ -5459,17 +6501,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>三枝さんはメガネ先輩と恋を描く</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>セレビィ量産型(著者)</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第22話前半</t>
+          <t>第82話その4</t>
         </is>
       </c>
     </row>
@@ -5479,17 +6521,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>塔の管理をしてみよう</t>
+          <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+          <t>丈(著者)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第92話後編</t>
+          <t>第127話</t>
         </is>
       </c>
     </row>
@@ -5499,17 +6541,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ライブダンジョン！</t>
+          <t>ダメ人間の愛しかた</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+          <t>岩葉(著者)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第89話前半</t>
+          <t>第20話前編　ダメ人間と3人暮らしの彼女</t>
         </is>
       </c>
     </row>
@@ -5519,17 +6561,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+          <t>漫画/すたひろ 原作/Y.A</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第2話後編</t>
+          <t>chapter70【37話①】</t>
         </is>
       </c>
     </row>
@@ -5539,17 +6581,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>異世界でも無難に生きたい症候群</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第31話③</t>
+          <t>第87話　その3</t>
         </is>
       </c>
     </row>
@@ -5559,17 +6601,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+          <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+          <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第1話後半</t>
+          <t>第5話②「4人で遊園地！」</t>
         </is>
       </c>
     </row>
@@ -5579,17 +6621,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>女子高生の無駄づかい</t>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ビーノ(著者)</t>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第135話　きずな</t>
+          <t>第6話　美少女二人（後編）</t>
         </is>
       </c>
     </row>
@@ -5599,17 +6641,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>路地裏で拾った女の子がバッドエンド後の乙女ゲームのヒロインだった件</t>
+          <t>生徒会役員共</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>カボチャマスク(原作) 樋乃えなが(作画) へいろー(キャラクター原案)</t>
+          <t>氏家ト全</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第2話</t>
+          <t>#414</t>
         </is>
       </c>
     </row>
@@ -5619,17 +6661,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
+          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>三部べべ(漫画) ねうしとら(原作)</t>
+          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第25話-2</t>
         </is>
       </c>
     </row>
@@ -5639,17 +6681,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>隣の席のヤンキー清水さんが髪を黒く染めてきた</t>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>底花(原作) 真田若楓(漫画) ハム(キャラクター原案)</t>
+          <t>KAKERU</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第11話-1</t>
+          <t>第68話「東アイギス2」（後半）</t>
         </is>
       </c>
     </row>
@@ -5659,17 +6701,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+          <t>賢者の孫</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>空野進 sorani ファルまろ</t>
+          <t>緒方俊輔(漫画) 吉岡剛(原作) 菊池政治(キャラクター原案)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第12話　最弱貴族、悪役令嬢と出会う（２）</t>
+          <t>第95話-3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-09-29
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -21,6 +21,7 @@
     <sheet name="2025-09-08" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="2025-09-15" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="2025-09-22" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="2025-09-29" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -5716,22 +5717,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>ワンパンマン</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>211撃目</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>異種族レビュアーズ</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>天原(原作) masha(作画)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第87話</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第71話</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>コミックス第14巻発売告知</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第32話：思考を奪う③</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第６９話『岩鬼停止』③</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第5話 前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>クセ強彼女は床にいざなう</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>須河篤志(著者)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第15話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>六志麻あさ 業務用餅 kisui</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第７２話</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>美人女上司滝沢さん</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>やんBARU(著者)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第203話</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第126話　王家の立場</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第64話 更衣室の戦いが始まった（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>帰ってください！ 阿久津さん</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>長岡太一(著者)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第196話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第78話その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第128話　レムと話してみる（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>ダークサモナーとデキている</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>車王(著者)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第76話</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>蜘蛛ですが、なにか？</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第76話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第５２話　暴走を止める器用貧乏（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>まんきつしたい常連さん</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>しんみりん(著者)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第48話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第50話（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>Ｓ級ギルドを追放されたけど、実は俺だけドラゴンの言葉がわかるので、気付いたときには竜騎士の頂点を極めてました。</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>ひそな(漫画) 三木なずな(原作) 白狼(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第39話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第305話</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第80話　先に行く</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第73話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>戸崎さんは僕にだけ冷たい</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>saku(著者)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第29話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>濁る瞳で何を願う ハイセルク戦記</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>トルトネン 創-taro 斎藤八呑</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第34話 ダンデューグ城へようこそ</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>ニチアサ好きのオタクが悪役生徒に転生した結果、破滅フラグが崩壊していく件について</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>烏丸英（原作） どんぐりす（漫画）</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第14話（後編）急襲…事件の始まり</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第31話</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>君のラブを見せてくれ！</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>リムコロ(著者)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>コミックス第⑤巻発売告知</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第34話 独身貴族は礼の品を贈る（1）</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第110話：王女に贈る子守歌</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>「おかえり、パパ」</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>蝉丸</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第28話　帰宅</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第139話 よくわからないけれどズゥゥゥンときたみたいです（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>聖者無双</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第92話　龍と精霊の信仰（後半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第４２話　勇者、六邪神将相手に舐めプしてたら、ピンチになる（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>ライドンキング</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>馬場康誌</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第83話 大統領と龍の闇卵（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 林たかあき</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第54話 イバラの帰り道</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第6話-2：火蓮の剣</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>小林さんちのメイドラゴン</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>クール教信者</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第150話</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第82話その4</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第127話</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>ダメ人間の愛しかた</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>岩葉(著者)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第20話前編　ダメ人間と3人暮らしの彼女</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>chapter70【37話①】</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第87話　その3</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第5話②「4人で遊園地！」</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第6話　美少女二人（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>生徒会役員共</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>氏家ト全</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>#414</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第25話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>KAKERU</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第68話「東アイギス2」（後半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>賢者の孫</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>緒方俊輔(漫画) 吉岡剛(原作) 菊池政治(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第95話-3</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ワンパンマン</t>
+          <t>異世界おじさん</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>原作/ＯＮＥ 作画/村田雄介</t>
+          <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>211撃目</t>
+          <t>第71話</t>
         </is>
       </c>
     </row>
@@ -5741,17 +6783,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>異種族レビュアーズ</t>
+          <t>「おかえり、パパ」</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>天原(原作) masha(作画)</t>
+          <t>蝉丸</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第87話</t>
+          <t>第28話　帰宅</t>
         </is>
       </c>
     </row>
@@ -5761,17 +6803,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第71話</t>
+          <t>第17話-3：「違法奴隷商討伐」</t>
         </is>
       </c>
     </row>
@@ -5781,17 +6823,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>ニチアサ好きのオタクが悪役生徒に転生した結果、破滅フラグが崩壊していく件について</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>烏丸英（原作） どんぐりす（漫画）</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>コミックス第14巻発売告知</t>
+          <t>第14話（後編）急襲…事件の始まり</t>
         </is>
       </c>
     </row>
@@ -5801,17 +6843,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+          <t>戸崎さんは僕にだけ冷たい</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>zunta(作画) はらわたさいぞう(原作)</t>
+          <t>saku(著者)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第32話：思考を奪う③</t>
+          <t>第29話-1</t>
         </is>
       </c>
     </row>
@@ -5821,17 +6863,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第６９話『岩鬼停止』③</t>
+          <t>第41話①</t>
         </is>
       </c>
     </row>
@@ -5841,17 +6883,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+          <t>生徒会にも穴はある！</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+          <t>むちまろ</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第5話 前編</t>
+          <t>第136話	ぎゅってしたい</t>
         </is>
       </c>
     </row>
@@ -5861,17 +6903,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>クセ強彼女は床にいざなう</t>
+          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>須河篤志(著者)</t>
+          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第15話後半</t>
+          <t>第31話</t>
         </is>
       </c>
     </row>
@@ -5881,17 +6923,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+          <t>君のラブを見せてくれ！</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>六志麻あさ 業務用餅 kisui</t>
+          <t>リムコロ(著者)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第７２話</t>
+          <t>コミックス第⑤巻発売告知</t>
         </is>
       </c>
     </row>
@@ -5901,17 +6943,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>美人女上司滝沢さん</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>やんBARU(著者)</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第203話</t>
+          <t>第６９話『岩鬼停止』④</t>
         </is>
       </c>
     </row>
@@ -5921,17 +6963,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第126話　王家の立場</t>
+          <t>第111話：泥棒の音を取り戻せ</t>
         </is>
       </c>
     </row>
@@ -5941,17 +6983,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第64話 更衣室の戦いが始まった（２）</t>
+          <t>第35話②</t>
         </is>
       </c>
     </row>
@@ -5961,17 +7003,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>帰ってください！ 阿久津さん</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>長岡太一(著者)</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第196話</t>
+          <t>第127話　帝国の思惑</t>
         </is>
       </c>
     </row>
@@ -5981,17 +7023,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第78話その2</t>
+          <t>第11話-2</t>
         </is>
       </c>
     </row>
@@ -6001,17 +7043,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>異世界魔王と召喚少女の奴隷魔術</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第128話　レムと話してみる（後編）</t>
+          <t>休載イラスト</t>
         </is>
       </c>
     </row>
@@ -6021,17 +7063,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ダークサモナーとデキている</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>車王(著者)</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第76話</t>
+          <t>第５３話　虎の尾を踏む器用貧乏（１）</t>
         </is>
       </c>
     </row>
@@ -6041,17 +7083,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>蜘蛛ですが、なにか？</t>
+          <t>ダンジョンの幼なじみ</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+          <t>久真やすひさ(著者)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第76話その1</t>
+          <t>第58話</t>
         </is>
       </c>
     </row>
@@ -6061,17 +7103,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>異世界のんびり農家</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第５２話　暴走を止める器用貧乏（４）</t>
+          <t>第306話</t>
         </is>
       </c>
     </row>
@@ -6081,17 +7123,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>まんきつしたい常連さん</t>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>しんみりん(著者)</t>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第48話前編</t>
+          <t>第２４食　サーモンのカルパッチョ、パクパクですわ！（２）</t>
         </is>
       </c>
     </row>
@@ -6101,17 +7143,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>淫獄団地</t>
+          <t>美人女上司滝沢さん</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+          <t>やんBARU(著者)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第50話（後編）</t>
+          <t>第204話</t>
         </is>
       </c>
     </row>
@@ -6121,17 +7163,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Ｓ級ギルドを追放されたけど、実は俺だけドラゴンの言葉がわかるので、気付いたときには竜騎士の頂点を極めてました。</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ひそな(漫画) 三木なずな(原作) 白狼(キャラクター原案)</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第39話-2</t>
+          <t>第53話①　ダンジョンをクリアしてみた</t>
         </is>
       </c>
     </row>
@@ -6141,17 +7183,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>異世界のんびり農家</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第305話</t>
+          <t>第73話③</t>
         </is>
       </c>
     </row>
@@ -6161,17 +7203,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+          <t>アザミヤコを好きになる</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>板垣恵介 猪原賽 陸井栄史</t>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第80話　先に行く</t>
+          <t>第10話</t>
         </is>
       </c>
     </row>
@@ -6181,17 +7223,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第73話②</t>
+          <t>第25話</t>
         </is>
       </c>
     </row>
@@ -6201,17 +7243,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>戸崎さんは僕にだけ冷たい</t>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>saku(著者)</t>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第29話-1</t>
+          <t>第42話　奴は座っている（前編）</t>
         </is>
       </c>
     </row>
@@ -6221,17 +7263,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>濁る瞳で何を願う ハイセルク戦記</t>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>トルトネン 創-taro 斎藤八呑</t>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第34話 ダンデューグ城へようこそ</t>
+          <t>第34話 独身貴族は礼の品を贈る（2）</t>
         </is>
       </c>
     </row>
@@ -6241,17 +7283,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ニチアサ好きのオタクが悪役生徒に転生した結果、破滅フラグが崩壊していく件について</t>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>烏丸英（原作） どんぐりす（漫画）</t>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第14話（後編）急襲…事件の始まり</t>
+          <t>第48話 緑の塔夏祭り夕食会①</t>
         </is>
       </c>
     </row>
@@ -6261,17 +7303,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
+          <t>物語の黒幕に転生して</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第31話</t>
+          <t>第34話</t>
         </is>
       </c>
     </row>
@@ -6281,17 +7323,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>君のラブを見せてくれ！</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>リムコロ(著者)</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>コミックス第⑤巻発売告知</t>
+          <t>拷問150</t>
         </is>
       </c>
     </row>
@@ -6301,17 +7343,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>リアデイルの大地にて</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>月見だしお(著者) Ceez(原作) てんまそ(キャラクター原案) 涼風涼(構成)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第34話 独身貴族は礼の品を贈る（1）</t>
+          <t>第40章-2</t>
         </is>
       </c>
     </row>
@@ -6321,17 +7363,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
+          <t>おとなりのダウナーさんは無理させない</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
+          <t>瑠璃いろ(著者)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第110話：王女に贈る子守歌</t>
+          <t>第13.5話</t>
         </is>
       </c>
     </row>
@@ -6341,17 +7383,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>「おかえり、パパ」</t>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>蝉丸</t>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第28話　帰宅</t>
+          <t>第73話(前編) ぶらり新生ラクス街</t>
         </is>
       </c>
     </row>
@@ -6361,17 +7403,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第139話 よくわからないけれどズゥゥゥンときたみたいです（２）</t>
+          <t>第４２話　勇者、六邪神将相手に舐めプしてたら、ピンチになる（４）</t>
         </is>
       </c>
     </row>
@@ -6381,17 +7423,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>聖者無双</t>
+          <t>Lv２からチートだった元勇者候補のまったり異世界ライフ</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+          <t>糸町秋音（漫画） 鬼ノ城ミヤ（原作） 片桐（キャラクター原案）</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第92話　龍と精霊の信仰（後半）</t>
+          <t>第61話　成長…？</t>
         </is>
       </c>
     </row>
@@ -6401,17 +7443,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>三吉汐美(著者)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第４２話　勇者、六邪神将相手に舐めプしてたら、ピンチになる（３）</t>
+          <t>第17話後半</t>
         </is>
       </c>
     </row>
@@ -6421,17 +7463,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ライドンキング</t>
+          <t>くらいあの子としたいこと</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>馬場康誌</t>
+          <t>碇マナツ(著者)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第83話 大統領と龍の闇卵（前編）</t>
+          <t>第85話</t>
         </is>
       </c>
     </row>
@@ -6441,17 +7483,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>板垣恵介 林たかあき</t>
+          <t>セレビィ量産型(著者)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第54話 イバラの帰り道</t>
+          <t>第22話後半</t>
         </is>
       </c>
     </row>
@@ -6461,17 +7503,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第6話-2：火蓮の剣</t>
+          <t>第83話(前編)その1</t>
         </is>
       </c>
     </row>
@@ -6481,17 +7523,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>小林さんちのメイドラゴン</t>
+          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>クール教信者</t>
+          <t>三部べべ(漫画) ねうしとら(原作)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第150話</t>
+          <t>第2話-2</t>
         </is>
       </c>
     </row>
@@ -6501,17 +7543,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>バーサス</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第82話その4</t>
+          <t>第28話　工場（2）</t>
         </is>
       </c>
     </row>
@@ -6521,17 +7563,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！</t>
+          <t>インフィニット・デンドログラム</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>丈(著者)</t>
+          <t>今井神 原作：海道左近 キャラクター原案：タイキ</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第127話</t>
+          <t>第73話</t>
         </is>
       </c>
     </row>
@@ -6541,17 +7583,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ダメ人間の愛しかた</t>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>岩葉(著者)</t>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第20話前編　ダメ人間と3人暮らしの彼女</t>
+          <t>第3話前編</t>
         </is>
       </c>
     </row>
@@ -6561,17 +7603,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>漫画/すたひろ 原作/Y.A</t>
+          <t>FUNA 東西 モトエ恵介</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>chapter70【37話①】</t>
+          <t>第122話　襲撃［その１］</t>
         </is>
       </c>
     </row>
@@ -6581,17 +7623,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>お気楽領主の楽しい領地防衛 ～生産系魔術で名もなき村を最強の城塞都市に～</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>青色まろ（漫画） 赤池宗（原作） 転（原作イラスト）</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第87話　その3</t>
+          <t>第34話　永住権</t>
         </is>
       </c>
     </row>
@@ -6601,17 +7643,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
+          <t>幼女戦記</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
+          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第5話②「4人で遊園地！」</t>
+          <t>第百八章：ドードーバード航空戦Ⅲ</t>
         </is>
       </c>
     </row>
@@ -6621,17 +7663,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第6話　美少女二人（後編）</t>
+          <t>第１９話②</t>
         </is>
       </c>
     </row>
@@ -6641,17 +7683,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>生徒会役員共</t>
+          <t>最果てのパラディン</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>氏家ト全</t>
+          <t>奥橋睦（漫画） 柳野かなた（原作） 輪くすさが（キャラクター原案）</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>#414</t>
+          <t>第67話　月の旅路</t>
         </is>
       </c>
     </row>
@@ -6661,17 +7703,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第25話-2</t>
+          <t>第87話　その4</t>
         </is>
       </c>
     </row>
@@ -6681,17 +7723,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>KAKERU</t>
+          <t>はぐはぐ(著者)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第68話「東アイギス2」（後半）</t>
+          <t>第86話</t>
         </is>
       </c>
     </row>
@@ -6701,17 +7743,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>賢者の孫</t>
+          <t>異世界でも無難に生きたい症候群</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>緒方俊輔(漫画) 吉岡剛(原作) 菊池政治(キャラクター原案)</t>
+          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第95話-3</t>
+          <t>第31話④</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-10-06
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -22,6 +22,7 @@
     <sheet name="2025-09-15" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="2025-09-22" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="2025-09-29" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="2025-10-06" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -6758,22 +6759,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第71話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>「おかえり、パパ」</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>蝉丸</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第28話　帰宅</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第17話-3：「違法奴隷商討伐」</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>ニチアサ好きのオタクが悪役生徒に転生した結果、破滅フラグが崩壊していく件について</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>烏丸英（原作） どんぐりす（漫画）</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第14話（後編）急襲…事件の始まり</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>戸崎さんは僕にだけ冷たい</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>saku(著者)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第29話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第41話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第136話	ぎゅってしたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第31話</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>君のラブを見せてくれ！</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>リムコロ(著者)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>コミックス第⑤巻発売告知</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第６９話『岩鬼停止』④</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第111話：泥棒の音を取り戻せ</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第35話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第127話　帝国の思惑</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第11話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第５３話　虎の尾を踏む器用貧乏（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンの幼なじみ</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>久真やすひさ(著者)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第58話</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第306話</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第２４食　サーモンのカルパッチョ、パクパクですわ！（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>美人女上司滝沢さん</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>やんBARU(著者)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第204話</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第53話①　ダンジョンをクリアしてみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第73話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>アザミヤコを好きになる</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第10話</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第25話</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第42話　奴は座っている（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第34話 独身貴族は礼の品を贈る（2）</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第48話 緑の塔夏祭り夕食会①</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>物語の黒幕に転生して</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第34話</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>拷問150</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>リアデイルの大地にて</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>月見だしお(著者) Ceez(原作) てんまそ(キャラクター原案) 涼風涼(構成)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第40章-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>おとなりのダウナーさんは無理させない</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>瑠璃いろ(著者)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第13.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第73話(前編) ぶらり新生ラクス街</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第４２話　勇者、六邪神将相手に舐めプしてたら、ピンチになる（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>Lv２からチートだった元勇者候補のまったり異世界ライフ</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>糸町秋音（漫画） 鬼ノ城ミヤ（原作） 片桐（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第61話　成長…？</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>三吉汐美(著者)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第17話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第85話</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>セレビィ量産型(著者)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第22話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第83話(前編)その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>三部べべ(漫画) ねうしとら(原作)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第2話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>バーサス</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第28話　工場（2）</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>インフィニット・デンドログラム</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>今井神 原作：海道左近 キャラクター原案：タイキ</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第73話</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第3話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>FUNA 東西 モトエ恵介</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第122話　襲撃［その１］</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>お気楽領主の楽しい領地防衛 ～生産系魔術で名もなき村を最強の城塞都市に～</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>青色まろ（漫画） 赤池宗（原作） 転（原作イラスト）</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第34話　永住権</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>幼女戦記</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第百八章：ドードーバード航空戦Ⅲ</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第１９話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>最果てのパラディン</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>奥橋睦（漫画） 柳野かなた（原作） 輪くすさが（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第67話　月の旅路</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第87話　その4</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>はぐはぐ(著者)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第86話</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>異世界でも無難に生きたい症候群</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第31話④</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第71話</t>
+          <t>212撃目</t>
         </is>
       </c>
     </row>
@@ -6783,17 +7825,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>「おかえり、パパ」</t>
+          <t>魔王の俺が奴隷エルフを嫁にしたんだが、どう愛でればいい？</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>蝉丸</t>
+          <t>原作／手島史詞 キャラクター原案／COMTA 漫画／板垣ハコ</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第28話　帰宅</t>
+          <t>第73話</t>
         </is>
       </c>
     </row>
@@ -6803,17 +7845,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第17話-3：「違法奴隷商討伐」</t>
+          <t>第６５話　地雷の戦いが始まった（１）</t>
         </is>
       </c>
     </row>
@@ -6823,17 +7865,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ニチアサ好きのオタクが悪役生徒に転生した結果、破滅フラグが崩壊していく件について</t>
+          <t>異世界居酒屋「のぶ」</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>烏丸英（原作） どんぐりす（漫画）</t>
+          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第14話（後編）急襲…事件の始まり</t>
+          <t>第125話</t>
         </is>
       </c>
     </row>
@@ -6843,17 +7885,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>戸崎さんは僕にだけ冷たい</t>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>saku(著者)</t>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第29話-1</t>
+          <t>【投票開始】人気投票企画『みんなでハロウィン！』【第12巻発売記念】</t>
         </is>
       </c>
     </row>
@@ -6863,17 +7905,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第41話①</t>
+          <t>第79話その1</t>
         </is>
       </c>
     </row>
@@ -6883,17 +7925,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>生徒会にも穴はある！</t>
+          <t>帰ってください！ 阿久津さん</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>むちまろ</t>
+          <t>長岡太一(著者)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第136話	ぎゅってしたい</t>
+          <t>第197話</t>
         </is>
       </c>
     </row>
@@ -6903,17 +7945,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第31話</t>
+          <t>第48話後編</t>
         </is>
       </c>
     </row>
@@ -6923,17 +7965,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>君のラブを見せてくれ！</t>
+          <t>王子様の友達</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>リムコロ(著者)</t>
+          <t>すけろく(著者)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>コミックス第⑤巻発売告知</t>
+          <t>番外編</t>
         </is>
       </c>
     </row>
@@ -6943,17 +7985,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>須河篤志(著者)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第６９話『岩鬼停止』④</t>
+          <t>番外編</t>
         </is>
       </c>
     </row>
@@ -6963,17 +8005,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第111話：泥棒の音を取り戻せ</t>
+          <t>おまけ65</t>
         </is>
       </c>
     </row>
@@ -6983,17 +8025,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+          <t>不純な彼女達は懺悔しない</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+          <t>ポロロッカ(著者)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第35話②</t>
+          <t>第32話</t>
         </is>
       </c>
     </row>
@@ -7003,17 +8045,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第127話　帝国の思惑</t>
+          <t>第129話　三人の門出（前編）</t>
         </is>
       </c>
     </row>
@@ -7023,17 +8065,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第11話-2</t>
+          <t>第25話</t>
         </is>
       </c>
     </row>
@@ -7043,17 +8085,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>休載イラスト</t>
+          <t>第５３話　虎の尾を踏む器用貧乏（２）</t>
         </is>
       </c>
     </row>
@@ -7063,17 +8105,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第５３話　虎の尾を踏む器用貧乏（１）</t>
+          <t>第13話</t>
         </is>
       </c>
     </row>
@@ -7083,17 +8125,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ダンジョンの幼なじみ</t>
+          <t>ダークサモナーとデキている</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>久真やすひさ(著者)</t>
+          <t>車王(著者)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第58話</t>
+          <t>第77話</t>
         </is>
       </c>
     </row>
@@ -7103,17 +8145,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>異世界のんびり農家</t>
+          <t>淫獄団地</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第306話</t>
+          <t>第51話（前編）</t>
         </is>
       </c>
     </row>
@@ -7133,7 +8175,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第２４食　サーモンのカルパッチョ、パクパクですわ！（２）</t>
+          <t>第２４食　サーモンのカルパッチョ、パクパクですわ！（３）</t>
         </is>
       </c>
     </row>
@@ -7143,17 +8185,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>美人女上司滝沢さん</t>
+          <t>魔のものたちは企てる</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>やんBARU(著者)</t>
+          <t>加藤拓弐(原作) ガしガし(作画)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第204話</t>
+          <t>第30話</t>
         </is>
       </c>
     </row>
@@ -7173,7 +8215,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第53話①　ダンジョンをクリアしてみた</t>
+          <t>第53話②　ダンジョンをクリアしてみた</t>
         </is>
       </c>
     </row>
@@ -7193,7 +8235,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第73話③</t>
+          <t>第73話④</t>
         </is>
       </c>
     </row>
@@ -7203,17 +8245,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>アザミヤコを好きになる</t>
+          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第10話</t>
+          <t>第31話</t>
         </is>
       </c>
     </row>
@@ -7223,17 +8265,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第25話</t>
+          <t>第9話</t>
         </is>
       </c>
     </row>
@@ -7243,17 +8285,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第42話　奴は座っている（前編）</t>
+          <t>第140話 よくわからないけれど策略だったみたいです（１）</t>
         </is>
       </c>
     </row>
@@ -7273,7 +8315,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第34話 独身貴族は礼の品を贈る（2）</t>
+          <t>第34話 独身貴族は礼の品を贈る（3）</t>
         </is>
       </c>
     </row>
@@ -7283,17 +8325,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+          <t>戸崎さんは僕にだけ冷たい</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+          <t>saku(著者)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第48話 緑の塔夏祭り夕食会①</t>
+          <t>第29話-2</t>
         </is>
       </c>
     </row>
@@ -7303,17 +8345,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>物語の黒幕に転生して</t>
+          <t>君のラブを見せてくれ！</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+          <t>リムコロ(著者)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第34話</t>
+          <t>コミックス第⑤巻発売告知</t>
         </is>
       </c>
     </row>
@@ -7323,17 +8365,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>ニチアサ好きのオタクが悪役生徒に転生した結果、破滅フラグが崩壊していく件について</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>烏丸英（原作） どんぐりす（漫画）</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>拷問150</t>
+          <t>第14話（後編）急襲…事件の始まり</t>
         </is>
       </c>
     </row>
@@ -7343,17 +8385,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>リアデイルの大地にて</t>
+          <t>「おかえり、パパ」</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>月見だしお(著者) Ceez(原作) てんまそ(キャラクター原案) 涼風涼(構成)</t>
+          <t>蝉丸</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第40章-2</t>
+          <t>第28話　帰宅</t>
         </is>
       </c>
     </row>
@@ -7363,17 +8405,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>おとなりのダウナーさんは無理させない</t>
+          <t>小林さんちのメイドラゴン</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>瑠璃いろ(著者)</t>
+          <t>クール教信者</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第13.5話</t>
+          <t>第151話</t>
         </is>
       </c>
     </row>
@@ -7383,17 +8425,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第73話(前編) ぶらり新生ラクス街</t>
+          <t>第112話：魔曲家ハクシャーマ❶</t>
         </is>
       </c>
     </row>
@@ -7403,17 +8445,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>聖者無双</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第４２話　勇者、六邪神将相手に舐めプしてたら、ピンチになる（４）</t>
+          <t>第93話　妥協ライン（前半）</t>
         </is>
       </c>
     </row>
@@ -7423,17 +8465,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Lv２からチートだった元勇者候補のまったり異世界ライフ</t>
+          <t>ライドンキング</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>糸町秋音（漫画） 鬼ノ城ミヤ（原作） 片桐（キャラクター原案）</t>
+          <t>馬場康誌</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第61話　成長…？</t>
+          <t>第83話 大統領と龍の闇卵（後編）</t>
         </is>
       </c>
     </row>
@@ -7443,17 +8485,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>アイドル辞めるけど結婚してくれますか!?</t>
+          <t>このヒーラー、めんどくさい</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>三吉汐美(著者)</t>
+          <t>丹念に発酵(著者)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第17話後半</t>
+          <t>第90話：ワンちゃん</t>
         </is>
       </c>
     </row>
@@ -7463,17 +8505,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>くらいあの子としたいこと</t>
+          <t>異世界食堂　洋食のねこや</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>碇マナツ(著者)</t>
+          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第85話</t>
+          <t>第41話②</t>
         </is>
       </c>
     </row>
@@ -7483,17 +8525,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>三枝さんはメガネ先輩と恋を描く</t>
+          <t>まったく最近の探偵ときたら</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>セレビィ量産型(著者)</t>
+          <t>五十嵐正邦(著者)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第22話後半</t>
+          <t>第116話</t>
         </is>
       </c>
     </row>
@@ -7503,17 +8545,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第83話(前編)その1</t>
+          <t>第7話-1：新しい目標</t>
         </is>
       </c>
     </row>
@@ -7523,17 +8565,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>三部べべ(漫画) ねうしとら(原作)</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第2話-2</t>
+          <t>第４２話　勇者、六邪神将相手に舐めプしてたら、ピンチになる（５）</t>
         </is>
       </c>
     </row>
@@ -7543,17 +8585,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>バーサス</t>
+          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第28話　工場（2）</t>
+          <t>第39話-2</t>
         </is>
       </c>
     </row>
@@ -7563,17 +8605,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>インフィニット・デンドログラム</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>今井神 原作：海道左近 キャラクター原案：タイキ</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第73話</t>
+          <t>拷問151</t>
         </is>
       </c>
     </row>
@@ -7583,17 +8625,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+          <t>異世界黙示録マイノグーラ ～破滅の文明で始める世界征服～</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+          <t>緑華野菜子(著者) 鹿角フェフ(原作) じゅん(キャラクター原案)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第3話前編</t>
+          <t>第31話　帳②</t>
         </is>
       </c>
     </row>
@@ -7603,17 +8645,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>FUNA 東西 モトエ恵介</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第122話　襲撃［その１］</t>
+          <t>第88話　その1</t>
         </is>
       </c>
     </row>
@@ -7623,17 +8665,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>お気楽領主の楽しい領地防衛 ～生産系魔術で名もなき村を最強の城塞都市に～</t>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>青色まろ（漫画） 赤池宗（原作） 転（原作イラスト）</t>
+          <t>六志麻あさ 業務用餅 kisui</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第34話　永住権</t>
+          <t>第７３話</t>
         </is>
       </c>
     </row>
@@ -7643,17 +8685,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>幼女戦記</t>
+          <t>ウォルテニア戦記</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
+          <t>漫画：八木ゆかり 原作：保利亮太 キャラクター原案：bob</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第百八章：ドードーバード航空戦Ⅲ</t>
+          <t>第58話</t>
         </is>
       </c>
     </row>
@@ -7663,17 +8705,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>女子高生の無駄づかい</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>ビーノ(著者)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第１９話②</t>
+          <t>第136話　へんけん</t>
         </is>
       </c>
     </row>
@@ -7683,17 +8725,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>最果てのパラディン</t>
+          <t>ダメ人間の愛しかた</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>奥橋睦（漫画） 柳野かなた（原作） 輪くすさが（キャラクター原案）</t>
+          <t>岩葉(著者)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第67話　月の旅路</t>
+          <t>第20話後編　ダメ人間と3人暮らしの彼女</t>
         </is>
       </c>
     </row>
@@ -7703,17 +8745,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第87話　その4</t>
+          <t>第30話</t>
         </is>
       </c>
     </row>
@@ -7723,17 +8765,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>サーシャちゃんとクラスメイトオタクくん</t>
+          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>はぐはぐ(著者)</t>
+          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第86話</t>
+          <t>第26話-1</t>
         </is>
       </c>
     </row>
@@ -7743,17 +8785,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>異世界でも無難に生きたい症候群</t>
+          <t>ギャルとダンジョンと周回遅れの探索英雄譚</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
+          <t>漫画家： 水田ケンジ 原作：榊一郎 キャラクター原案：黒獅子</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第31話④</t>
+          <t>第3話</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-10-13
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -23,6 +23,7 @@
     <sheet name="2025-09-22" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="2025-09-29" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="2025-10-06" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="2025-10-13" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -7800,22 +7801,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>ワンパンマン</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>212撃目</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>魔王の俺が奴隷エルフを嫁にしたんだが、どう愛でればいい？</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>原作／手島史詞 キャラクター原案／COMTA 漫画／板垣ハコ</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第73話</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第６５話　地雷の戦いが始まった（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>異世界居酒屋「のぶ」</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第125話</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>【投票開始】人気投票企画『みんなでハロウィン！』【第12巻発売記念】</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第79話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>帰ってください！ 阿久津さん</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>長岡太一(著者)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第197話</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>まんきつしたい常連さん</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>しんみりん(著者)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第48話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>王子様の友達</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>すけろく(著者)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>番外編</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>クセ強彼女は床にいざなう</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>須河篤志(著者)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>番外編</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>おまけ65</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>不純な彼女達は懺悔しない</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>ポロロッカ(著者)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第32話</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第129話　三人の門出（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第25話</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第５３話　虎の尾を踏む器用貧乏（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第13話</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>ダークサモナーとデキている</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>車王(著者)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第77話</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第51話（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第２４食　サーモンのカルパッチョ、パクパクですわ！（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>魔のものたちは企てる</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>加藤拓弐(原作) ガしガし(作画)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第30話</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第53話②　ダンジョンをクリアしてみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第73話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第31話</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第9話</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第140話 よくわからないけれど策略だったみたいです（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第34話 独身貴族は礼の品を贈る（3）</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>戸崎さんは僕にだけ冷たい</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>saku(著者)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第29話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>君のラブを見せてくれ！</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>リムコロ(著者)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>コミックス第⑤巻発売告知</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>ニチアサ好きのオタクが悪役生徒に転生した結果、破滅フラグが崩壊していく件について</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>烏丸英（原作） どんぐりす（漫画）</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第14話（後編）急襲…事件の始まり</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>「おかえり、パパ」</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>蝉丸</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第28話　帰宅</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>小林さんちのメイドラゴン</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>クール教信者</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第151話</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第112話：魔曲家ハクシャーマ❶</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>聖者無双</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第93話　妥協ライン（前半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>ライドンキング</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>馬場康誌</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第83話 大統領と龍の闇卵（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>このヒーラー、めんどくさい</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>丹念に発酵(著者)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第90話：ワンちゃん</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>異世界食堂　洋食のねこや</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第41話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>まったく最近の探偵ときたら</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>五十嵐正邦(著者)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第116話</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第7話-1：新しい目標</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第４２話　勇者、六邪神将相手に舐めプしてたら、ピンチになる（５）</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第39話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>拷問151</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>異世界黙示録マイノグーラ ～破滅の文明で始める世界征服～</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>緑華野菜子(著者) 鹿角フェフ(原作) じゅん(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第31話　帳②</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第88話　その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>六志麻あさ 業務用餅 kisui</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第７３話</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>ウォルテニア戦記</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>漫画：八木ゆかり 原作：保利亮太 キャラクター原案：bob</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第58話</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>女子高生の無駄づかい</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>ビーノ(著者)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第136話　へんけん</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>ダメ人間の愛しかた</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>岩葉(著者)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第20話後編　ダメ人間と3人暮らしの彼女</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第30話</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第26話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>ギャルとダンジョンと周回遅れの探索英雄譚</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>漫画家： 水田ケンジ 原作：榊一郎 キャラクター原案：黒獅子</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第3話</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ワンパンマン</t>
+          <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>原作/ＯＮＥ 作画/村田雄介</t>
+          <t>丈(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>212撃目</t>
+          <t>第128話</t>
         </is>
       </c>
     </row>
@@ -7825,17 +8867,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>魔王の俺が奴隷エルフを嫁にしたんだが、どう愛でればいい？</t>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>原作／手島史詞 キャラクター原案／COMTA 漫画／板垣ハコ</t>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第73話</t>
+          <t>コミックス第６巻発売情報！</t>
         </is>
       </c>
     </row>
@@ -7845,17 +8887,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>転生したらスライムだった件</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>原作：伏瀬 漫画：川上泰樹 キャラクター原案：みっつばー</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第６５話　地雷の戦いが始まった（１）</t>
+          <t>第128話　強欲のマリアベル</t>
         </is>
       </c>
     </row>
@@ -7865,17 +8907,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>異世界居酒屋「のぶ」</t>
+          <t>不徳のギルド</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
+          <t>河添太一</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第125話</t>
+          <t>第９９話：ホシの不在</t>
         </is>
       </c>
     </row>
@@ -7885,17 +8927,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>【投票開始】人気投票企画『みんなでハロウィン！』【第12巻発売記念】</t>
+          <t>第41話➁</t>
         </is>
       </c>
     </row>
@@ -7905,17 +8947,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+          <t>とんでもスキルで異世界放浪メシ</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+          <t>赤岸K（漫画） 江口連（原作） 雅（キャラクター原案）</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第79話その1</t>
+          <t>第55話　「魔獣大戦争」</t>
         </is>
       </c>
     </row>
@@ -7925,17 +8967,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>帰ってください！ 阿久津さん</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>長岡太一(著者)</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第197話</t>
+          <t>第７０話「突貫停止」①</t>
         </is>
       </c>
     </row>
@@ -7945,17 +8987,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>まんきつしたい常連さん</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>しんみりん(著者)</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第48話後編</t>
+          <t>第39話</t>
         </is>
       </c>
     </row>
@@ -7965,17 +9007,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>王子様の友達</t>
+          <t>生徒会にも穴はある！</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>すけろく(著者)</t>
+          <t>むちまろ</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>番外編</t>
+          <t>第137話	虎丸の世界（前編）</t>
         </is>
       </c>
     </row>
@@ -7985,17 +9027,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>クセ強彼女は床にいざなう</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>須河篤志(著者)</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>番外編</t>
+          <t>第６５話　地雷の戦いが始まった（２）</t>
         </is>
       </c>
     </row>
@@ -8005,17 +9047,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>おまけ65</t>
+          <t>第36話①</t>
         </is>
       </c>
     </row>
@@ -8025,17 +9067,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>不純な彼女達は懺悔しない</t>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ポロロッカ(著者)</t>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第32話</t>
+          <t>第12話-1</t>
         </is>
       </c>
     </row>
@@ -8045,17 +9087,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>異世界魔王と召喚少女の奴隷魔術</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第129話　三人の門出（前編）</t>
+          <t>第128話　フレイのお願い</t>
         </is>
       </c>
     </row>
@@ -8065,17 +9107,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>女友達は頼めば意外とヤらせてくれる</t>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ろくろ(漫画) 鏡遊(原作)</t>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第25話</t>
+          <t>更新延期のお知らせ</t>
         </is>
       </c>
     </row>
@@ -8085,17 +9127,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>久遠まこと(著者) 石のやっさん(原作)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第５３話　虎の尾を踏む器用貧乏（２）</t>
+          <t>特別編　ハルカの乙女心ファッション</t>
         </is>
       </c>
     </row>
@@ -8105,17 +9147,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+          <t>ダンジョンの幼なじみ</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+          <t>久真やすひさ(著者)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第13話</t>
+          <t>第59話</t>
         </is>
       </c>
     </row>
@@ -8125,17 +9167,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ダークサモナーとデキている</t>
+          <t>異世界のんびり農家</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>車王(著者)</t>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第77話</t>
+          <t>第307話</t>
         </is>
       </c>
     </row>
@@ -8145,17 +9187,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>淫獄団地</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第51話（前編）</t>
+          <t>第129話　三人の門出（中編）</t>
         </is>
       </c>
     </row>
@@ -8165,17 +9207,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>島知宏 音速炒飯 有都あらゆる</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第２４食　サーモンのカルパッチョ、パクパクですわ！（３）</t>
+          <t>第５３話　虎の尾を踏む器用貧乏（３）</t>
         </is>
       </c>
     </row>
@@ -8185,17 +9227,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>魔のものたちは企てる</t>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>加藤拓弐(原作) ガしガし(作画)</t>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第30話</t>
+          <t>第81話　芸術作品</t>
         </is>
       </c>
     </row>
@@ -8205,17 +9247,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第53話②　ダンジョンをクリアしてみた</t>
+          <t>番外編①　ユクシーさんの冒険の話ですわ！</t>
         </is>
       </c>
     </row>
@@ -8235,7 +9277,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第73話④</t>
+          <t>第74話①</t>
         </is>
       </c>
     </row>
@@ -8245,17 +9287,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>モブ高生の俺でも冒険者になればリア充になれますか？</t>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>原作：百均 漫画：さぎやまれん キャラクター原案：hai</t>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第31話</t>
+          <t>第3話後編</t>
         </is>
       </c>
     </row>
@@ -8265,17 +9307,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第9話</t>
+          <t>第54話①　闇の女神と仲良くなってみた</t>
         </is>
       </c>
     </row>
@@ -8285,17 +9327,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第140話 よくわからないけれど策略だったみたいです（１）</t>
+          <t>第34話 独身貴族は礼の品を贈る（4）</t>
         </is>
       </c>
     </row>
@@ -8305,17 +9347,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第34話 独身貴族は礼の品を贈る（3）</t>
+          <t>第140話 よくわからないけれど策略だったみたいです（２）</t>
         </is>
       </c>
     </row>
@@ -8325,17 +9367,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>戸崎さんは僕にだけ冷たい</t>
+          <t>路地裏で拾った女の子がバッドエンド後の乙女ゲームのヒロインだった件</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>saku(著者)</t>
+          <t>カボチャマスク(原作) 樋乃えなが(作画) へいろー(キャラクター原案)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第29話-2</t>
+          <t>第3話</t>
         </is>
       </c>
     </row>
@@ -8345,17 +9387,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>君のラブを見せてくれ！</t>
+          <t>美人女上司滝沢さん</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>リムコロ(著者)</t>
+          <t>やんBARU(著者)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>コミックス第⑤巻発売告知</t>
+          <t>第205話</t>
         </is>
       </c>
     </row>
@@ -8365,17 +9407,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ニチアサ好きのオタクが悪役生徒に転生した結果、破滅フラグが崩壊していく件について</t>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>烏丸英（原作） どんぐりす（漫画）</t>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第14話（後編）急襲…事件の始まり</t>
+          <t>第42話　奴は座っている（中編）</t>
         </is>
       </c>
     </row>
@@ -8385,17 +9427,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>「おかえり、パパ」</t>
+          <t>くらいあの子としたいこと</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>蝉丸</t>
+          <t>碇マナツ(著者)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第28話　帰宅</t>
+          <t>第86話</t>
         </is>
       </c>
     </row>
@@ -8405,17 +9447,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>小林さんちのメイドラゴン</t>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>クール教信者</t>
+          <t>三吉汐美(著者)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第151話</t>
+          <t>第18話前半</t>
         </is>
       </c>
     </row>
@@ -8425,17 +9467,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ルパン三世 異世界の姫君（ネイバーワールドプリンセス）</t>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>モンキー・パンチ／エム・ピー・ワークス 内々けやき 佐伯庸介 白狼</t>
+          <t>板垣恵介 林たかあき</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第112話：魔曲家ハクシャーマ❶</t>
+          <t>第55話 恋は盲目</t>
         </is>
       </c>
     </row>
@@ -8445,17 +9487,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>聖者無双</t>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+          <t>はぐはぐ(著者)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第93話　妥協ライン（前半）</t>
+          <t>第87話</t>
         </is>
       </c>
     </row>
@@ -8465,17 +9507,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ライドンキング</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>馬場康誌</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第83話 大統領と龍の闇卵（後編）</t>
+          <t>拷問152</t>
         </is>
       </c>
     </row>
@@ -8485,17 +9527,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>このヒーラー、めんどくさい</t>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>丹念に発酵(著者)</t>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第90話：ワンちゃん</t>
+          <t>第２０話①</t>
         </is>
       </c>
     </row>
@@ -8505,17 +9547,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>異世界食堂　洋食のねこや</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第41話②</t>
+          <t>第83話(前編)その2</t>
         </is>
       </c>
     </row>
@@ -8525,17 +9567,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>まったく最近の探偵ときたら</t>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>五十嵐正邦(著者)</t>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第116話</t>
+          <t>第73話(後編) ぶらり新生ラクス街</t>
         </is>
       </c>
     </row>
@@ -8545,17 +9587,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+          <t>追放された底辺職「盗賊」はゲーム知識で無双する。一緒に召喚された先生も外れジョブだったけど効率的に成り上がります</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+          <t>ケンノジ 菅原イチバ カラスBTK</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第7話-1：新しい目標</t>
+          <t>第1話　二人の冒険で無双する</t>
         </is>
       </c>
     </row>
@@ -8565,17 +9607,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>北欧美少女のクラスメイトが、婚約者になったらデレデレの甘々になってしまった件について</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>原作：軽井広 漫画：神楽武志/両角潤香 キャラクター原案：pon</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第４２話　勇者、六邪神将相手に舐めプしてたら、ピンチになる（５）</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -8585,17 +9627,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第39話-2</t>
+          <t>第88話　その2</t>
         </is>
       </c>
     </row>
@@ -8605,17 +9647,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>拷問151</t>
+          <t>【描き下ろしイラスト】休載です！（その１）</t>
         </is>
       </c>
     </row>
@@ -8625,17 +9667,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>異世界黙示録マイノグーラ ～破滅の文明で始める世界征服～</t>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>緑華野菜子(著者) 鹿角フェフ(原作) じゅん(キャラクター原案)</t>
+          <t>KAKERU</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第31話　帳②</t>
+          <t>第69話「光の剣」（前半）</t>
         </is>
       </c>
     </row>
@@ -8645,17 +9687,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>最弱テイマーはゴミ拾いの旅を始めました。@COMIC</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>漫画：蕗野 冬 原作：ほのぼのる500 キャラクター原案：なま</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第88話　その1</t>
+          <t>第27話</t>
         </is>
       </c>
     </row>
@@ -8665,17 +9707,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>六志麻あさ 業務用餅 kisui</t>
+          <t>セレビィ量産型(著者)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第７３話</t>
+          <t>第22.5話</t>
         </is>
       </c>
     </row>
@@ -8685,17 +9727,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ウォルテニア戦記</t>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>漫画：八木ゆかり 原作：保利亮太 キャラクター原案：bob</t>
+          <t>漫画/すたひろ 原作/Y.A</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第58話</t>
+          <t>chapter71【37話②】</t>
         </is>
       </c>
     </row>
@@ -8705,17 +9747,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>女子高生の無駄づかい</t>
+          <t>英雄女騎士に有能とバレた俺の美人ハーレム騎士団 ガイカク・ヒクメの奇術騎士団</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ビーノ(著者)</t>
+          <t>明石六郎(原作) 太盛(作画) 氷室しゅんすけ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第136話　へんけん</t>
+          <t>第11話-2</t>
         </is>
       </c>
     </row>
@@ -8725,17 +9767,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ダメ人間の愛しかた</t>
+          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>岩葉(著者)</t>
+          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第20話後編　ダメ人間と3人暮らしの彼女</t>
+          <t>第58話　帰還</t>
         </is>
       </c>
     </row>
@@ -8745,17 +9787,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
+          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
+          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第30話</t>
+          <t>第84話前半</t>
         </is>
       </c>
     </row>
@@ -8765,17 +9807,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
+          <t>塔の管理をしてみよう</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第26話-1</t>
+          <t>第93話後編</t>
         </is>
       </c>
     </row>
@@ -8785,17 +9827,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ギャルとダンジョンと周回遅れの探索英雄譚</t>
+          <t>暗殺者である俺のステータスが勇者よりも明らかに強いのだが</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>漫画家： 水田ケンジ 原作：榊一郎 キャラクター原案：黒獅子</t>
+          <t>合鴨ひろゆき（漫画） 赤井まつり（原作） 東西（キャラクター原案）</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第3話</t>
+          <t>第34話　ブルート迷宮Ⅳ</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-10-20
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -24,6 +24,7 @@
     <sheet name="2025-09-29" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="2025-10-06" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="2025-10-13" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="2025-10-20" sheetId="19" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -8842,22 +8843,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第128話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>コミックス第６巻発売情報！</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>転生したらスライムだった件</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>原作：伏瀬 漫画：川上泰樹 キャラクター原案：みっつばー</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第128話　強欲のマリアベル</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>不徳のギルド</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>河添太一</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第９９話：ホシの不在</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第41話➁</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>とんでもスキルで異世界放浪メシ</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>赤岸K（漫画） 江口連（原作） 雅（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第55話　「魔獣大戦争」</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第７０話「突貫停止」①</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第39話</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第137話	虎丸の世界（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第６５話　地雷の戦いが始まった（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第36話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第12話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第128話　フレイのお願い</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>更新延期のお知らせ</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>久遠まこと(著者) 石のやっさん(原作)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>特別編　ハルカの乙女心ファッション</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンの幼なじみ</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>久真やすひさ(著者)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第59話</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第307話</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第129話　三人の門出（中編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第５３話　虎の尾を踏む器用貧乏（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第81話　芸術作品</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>番外編①　ユクシーさんの冒険の話ですわ！</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第74話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第3話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第54話①　闇の女神と仲良くなってみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第34話 独身貴族は礼の品を贈る（4）</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第140話 よくわからないけれど策略だったみたいです（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>路地裏で拾った女の子がバッドエンド後の乙女ゲームのヒロインだった件</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>カボチャマスク(原作) 樋乃えなが(作画) へいろー(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第3話</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>美人女上司滝沢さん</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>やんBARU(著者)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第205話</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第42話　奴は座っている（中編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第86話</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>三吉汐美(著者)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第18話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 林たかあき</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第55話 恋は盲目</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>はぐはぐ(著者)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第87話</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>拷問152</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第２０話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第83話(前編)その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第73話(後編) ぶらり新生ラクス街</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>追放された底辺職「盗賊」はゲーム知識で無双する。一緒に召喚された先生も外れジョブだったけど効率的に成り上がります</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>ケンノジ 菅原イチバ カラスBTK</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第1話　二人の冒険で無双する</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>北欧美少女のクラスメイトが、婚約者になったらデレデレの甘々になってしまった件について</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>原作：軽井広 漫画：神楽武志/両角潤香 キャラクター原案：pon</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第88話　その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>【描き下ろしイラスト】休載です！（その１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>KAKERU</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第69話「光の剣」（前半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>最弱テイマーはゴミ拾いの旅を始めました。@COMIC</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>漫画：蕗野 冬 原作：ほのぼのる500 キャラクター原案：なま</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第27話</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>セレビィ量産型(著者)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第22.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>chapter71【37話②】</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>英雄女騎士に有能とバレた俺の美人ハーレム騎士団 ガイカク・ヒクメの奇術騎士団</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>明石六郎(原作) 太盛(作画) 氷室しゅんすけ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第11話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第58話　帰還</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第84話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>塔の管理をしてみよう</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第93話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>暗殺者である俺のステータスが勇者よりも明らかに強いのだが</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>合鴨ひろゆき（漫画） 赤井まつり（原作） 東西（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第34話　ブルート迷宮Ⅳ</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>丈(著者)</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第128話</t>
+          <t>213撃目</t>
         </is>
       </c>
     </row>
@@ -8877,7 +9919,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>コミックス第６巻発売情報！</t>
+          <t>第33話：誰にも負けない完璧②</t>
         </is>
       </c>
     </row>
@@ -8887,17 +9929,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>転生したらスライムだった件</t>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>原作：伏瀬 漫画：川上泰樹 キャラクター原案：みっつばー</t>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第128話　強欲のマリアベル</t>
+          <t>第18話-1：「R18」</t>
         </is>
       </c>
     </row>
@@ -8907,17 +9949,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>不徳のギルド</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>河添太一</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第９９話：ホシの不在</t>
+          <t>第７０話「突貫停止」②</t>
         </is>
       </c>
     </row>
@@ -8927,17 +9969,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第41話➁</t>
+          <t>第６６話　登山の戦いが始まった（１）</t>
         </is>
       </c>
     </row>
@@ -8947,17 +9989,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>とんでもスキルで異世界放浪メシ</t>
+          <t>帰ってください！ 阿久津さん</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>赤岸K（漫画） 江口連（原作） 雅（キャラクター原案）</t>
+          <t>長岡太一(著者)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第55話　「魔獣大戦争」</t>
+          <t>番外編㉓</t>
         </is>
       </c>
     </row>
@@ -8967,17 +10009,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>王子様の友達</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>すけろく(著者)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第７０話「突貫停止」①</t>
+          <t>番外編【マンガ総選挙１位・マニフェスト実施】</t>
         </is>
       </c>
     </row>
@@ -8987,17 +10029,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第39話</t>
+          <t>第79話その2</t>
         </is>
       </c>
     </row>
@@ -9007,17 +10049,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>生徒会にも穴はある！</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>むちまろ</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第137話	虎丸の世界（前編）</t>
+          <t>第129話　未知なる脅威!?</t>
         </is>
       </c>
     </row>
@@ -9027,17 +10069,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第６５話　地雷の戦いが始まった（２）</t>
+          <t>第11話-2</t>
         </is>
       </c>
     </row>
@@ -9047,17 +10089,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+          <t>金属スライムを倒しまくった俺が【黒鋼の王】と呼ばれるまで</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+          <t>藤屋いずこ(著者) 温泉カピバラ(原作) 山椒魚(キャラクター原案)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第36話①</t>
+          <t>第15章-2</t>
         </is>
       </c>
     </row>
@@ -9067,17 +10109,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第12話-1</t>
+          <t>第14話</t>
         </is>
       </c>
     </row>
@@ -9087,17 +10129,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第128話　フレイのお願い</t>
+          <t>第129話　三人の門出（後編）</t>
         </is>
       </c>
     </row>
@@ -9107,17 +10149,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+          <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+          <t>須河篤志(著者)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>更新延期のお知らせ</t>
+          <t>第16話前半</t>
         </is>
       </c>
     </row>
@@ -9127,17 +10169,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>久遠まこと(著者) 石のやっさん(原作)</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>特別編　ハルカの乙女心ファッション</t>
+          <t>第５３話　虎の尾を踏む器用貧乏（４）</t>
         </is>
       </c>
     </row>
@@ -9147,17 +10189,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ダンジョンの幼なじみ</t>
+          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>久真やすひさ(著者)</t>
+          <t>三部べべ(漫画) ねうしとら(原作)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第59話</t>
+          <t>第3話-1</t>
         </is>
       </c>
     </row>
@@ -9167,17 +10209,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>異世界のんびり農家</t>
+          <t>ダークサモナーとデキている</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+          <t>車王(著者)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第307話</t>
+          <t>第78話</t>
         </is>
       </c>
     </row>
@@ -9187,17 +10229,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>異世界魔王と召喚少女の奴隷魔術</t>
+          <t>異世界のんびり農家</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第129話　三人の門出（中編）</t>
+          <t>第308話</t>
         </is>
       </c>
     </row>
@@ -9207,17 +10249,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第５３話　虎の尾を踏む器用貧乏（３）</t>
+          <t>第49話前編</t>
         </is>
       </c>
     </row>
@@ -9227,17 +10269,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>板垣恵介 猪原賽 陸井栄史</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第81話　芸術作品</t>
+          <t>第74話➁</t>
         </is>
       </c>
     </row>
@@ -9257,7 +10299,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>番外編①　ユクシーさんの冒険の話ですわ！</t>
+          <t>討伐のお礼ですわ！</t>
         </is>
       </c>
     </row>
@@ -9267,17 +10309,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>望まぬ不死の冒険者</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>中曽根ハイジ（漫画） 丘野 優（原作） じゃいあん（キャラクター原案）</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第74話①</t>
+          <t>第61話　早く捨てろ</t>
         </is>
       </c>
     </row>
@@ -9287,17 +10329,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+          <t>剥かせて！竜ケ崎さん</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+          <t>一智和智</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第3話後編</t>
+          <t>大学生編 第15話</t>
         </is>
       </c>
     </row>
@@ -9307,17 +10349,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>夜州 nini 藻</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第54話①　闇の女神と仲良くなってみた</t>
+          <t>第70話(前編)</t>
         </is>
       </c>
     </row>
@@ -9337,7 +10379,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第34話 独身貴族は礼の品を贈る（4）</t>
+          <t>第35話 独身貴族はバーでハイボールを作る（1）</t>
         </is>
       </c>
     </row>
@@ -9347,17 +10389,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第140話 よくわからないけれど策略だったみたいです（２）</t>
+          <t>第54話②　闇の女神と仲良くなってみた</t>
         </is>
       </c>
     </row>
@@ -9367,17 +10409,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>路地裏で拾った女の子がバッドエンド後の乙女ゲームのヒロインだった件</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>カボチャマスク(原作) 樋乃えなが(作画) へいろー(キャラクター原案)</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第3話</t>
+          <t>第141話 よくわからないけれど超理論が生み出されたようです（１）</t>
         </is>
       </c>
     </row>
@@ -9387,17 +10429,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>美人女上司滝沢さん</t>
+          <t>聖者無双</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>やんBARU(著者)</t>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第205話</t>
+          <t>第93話　妥協ライン（後半）</t>
         </is>
       </c>
     </row>
@@ -9407,17 +10449,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+          <t>ライドンキング</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+          <t>馬場康誌</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第42話　奴は座っている（中編）</t>
+          <t>第84話 大統領と賢者の過ち（前編）</t>
         </is>
       </c>
     </row>
@@ -9427,17 +10469,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>くらいあの子としたいこと</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>碇マナツ(著者)</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第86話</t>
+          <t>第10話</t>
         </is>
       </c>
     </row>
@@ -9447,17 +10489,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>アイドル辞めるけど結婚してくれますか!?</t>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>三吉汐美(著者)</t>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第18話前半</t>
+          <t>第48話 緑の塔夏祭り夕食会②</t>
         </is>
       </c>
     </row>
@@ -9467,17 +10509,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+          <t>小林さんちのメイドラゴン</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>板垣恵介 林たかあき</t>
+          <t>クール教信者</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第55話 恋は盲目</t>
+          <t>第152話</t>
         </is>
       </c>
     </row>
@@ -9487,17 +10529,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>サーシャちゃんとクラスメイトオタクくん</t>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>はぐはぐ(著者)</t>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第87話</t>
+          <t>第7話-2：新しい目標</t>
         </is>
       </c>
     </row>
@@ -9507,17 +10549,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>六志麻あさ 業務用餅 kisui</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>拷問152</t>
+          <t>第７４話ー①</t>
         </is>
       </c>
     </row>
@@ -9527,17 +10569,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>久遠まこと(著者) 石のやっさん(原作)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第２０話①</t>
+          <t>コミックス６巻発売告知</t>
         </is>
       </c>
     </row>
@@ -9547,17 +10589,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第83話(前編)その2</t>
+          <t>第88話　その3</t>
         </is>
       </c>
     </row>
@@ -9567,17 +10609,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第73話(後編) ぶらり新生ラクス街</t>
+          <t>拷問153</t>
         </is>
       </c>
     </row>
@@ -9587,17 +10629,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>追放された底辺職「盗賊」はゲーム知識で無双する。一緒に召喚された先生も外れジョブだったけど効率的に成り上がります</t>
+          <t>地味子な三葉さんが僕を誘惑する</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>ケンノジ 菅原イチバ カラスBTK</t>
+          <t>はぶらえる(著者)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第1話　二人の冒険で無双する</t>
+          <t>第11話後半</t>
         </is>
       </c>
     </row>
@@ -9607,17 +10649,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>北欧美少女のクラスメイトが、婚約者になったらデレデレの甘々になってしまった件について</t>
+          <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>原作：軽井広 漫画：神楽武志/両角潤香 キャラクター原案：pon</t>
+          <t>丈(著者)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第128話</t>
         </is>
       </c>
     </row>
@@ -9627,17 +10669,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>俺は星間国家の悪徳領主！</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第88話　その2</t>
+          <t>第41話　究極にして至高（前編）</t>
         </is>
       </c>
     </row>
@@ -9647,17 +10689,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>ライブダンジョン！</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>【描き下ろしイラスト】休載です！（その１）</t>
+          <t>第90話前半</t>
         </is>
       </c>
     </row>
@@ -9667,17 +10709,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>KAKERU</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第69話「光の剣」（前半）</t>
+          <t>【描き下ろしイラスト】休載です！（その２）</t>
         </is>
       </c>
     </row>
@@ -9687,17 +10729,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>最弱テイマーはゴミ拾いの旅を始めました。@COMIC</t>
+          <t>ギャルとダンジョンと周回遅れの探索英雄譚</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>漫画：蕗野 冬 原作：ほのぼのる500 キャラクター原案：なま</t>
+          <t>漫画家： 水田ケンジ 原作：榊一郎 キャラクター原案：黒獅子</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第27話</t>
+          <t>第4話</t>
         </is>
       </c>
     </row>
@@ -9707,17 +10749,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>三枝さんはメガネ先輩と恋を描く</t>
+          <t>異世界でも無難に生きたい症候群</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>セレビィ量産型(著者)</t>
+          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第22.5話</t>
+          <t>第32話①</t>
         </is>
       </c>
     </row>
@@ -9727,17 +10769,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+          <t>アザミヤコを好きになる</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>漫画/すたひろ 原作/Y.A</t>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>chapter71【37話②】</t>
+          <t>コミックス第2巻情報公開!!!</t>
         </is>
       </c>
     </row>
@@ -9747,17 +10789,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>英雄女騎士に有能とバレた俺の美人ハーレム騎士団 ガイカク・ヒクメの奇術騎士団</t>
+          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>明石六郎(原作) 太盛(作画) 氷室しゅんすけ(キャラクター原案)</t>
+          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第11話-2</t>
+          <t>第26話-2</t>
         </is>
       </c>
     </row>
@@ -9767,17 +10809,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
+          <t>魔石グルメ　魔物の力を食べたオレは最強！</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
+          <t>菅原健二(作画) 結城涼(原作) 成瀬ちさと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第58話　帰還</t>
+          <t>第68話後半</t>
         </is>
       </c>
     </row>
@@ -9787,17 +10829,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第84話前半</t>
+          <t>第31話</t>
         </is>
       </c>
     </row>
@@ -9807,17 +10849,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>塔の管理をしてみよう</t>
+          <t>めっちゃ召喚された件 THE COMIC</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第93話後編</t>
+          <t>第49話①</t>
         </is>
       </c>
     </row>
@@ -9827,17 +10869,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>暗殺者である俺のステータスが勇者よりも明らかに強いのだが</t>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>合鴨ひろゆき（漫画） 赤井まつり（原作） 東西（キャラクター原案）</t>
+          <t>空野進 sorani ファルまろ</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第34話　ブルート迷宮Ⅳ</t>
+          <t>第13話　最弱貴族、悪役令嬢に賭けを挑む（２）</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-10-27
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -25,6 +25,7 @@
     <sheet name="2025-10-06" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="2025-10-13" sheetId="18" state="visible" r:id="rId18"/>
     <sheet name="2025-10-20" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="2025-10-27" sheetId="20" state="visible" r:id="rId20"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -9884,1000 +9885,1000 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="0" t="inlineStr">
         <is>
           <t>ワンパンマン</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="0" t="inlineStr">
         <is>
           <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="0" t="inlineStr">
         <is>
           <t>213撃目</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="0" t="inlineStr">
         <is>
           <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="0" t="inlineStr">
         <is>
           <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>第33話：誰にも負けない完璧②</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="0" t="inlineStr">
         <is>
           <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="0" t="inlineStr">
         <is>
           <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="0" t="inlineStr">
         <is>
           <t>第18話-1：「R18」</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="0" t="inlineStr">
         <is>
           <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="0" t="inlineStr">
         <is>
           <t>光永康則</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="0" t="inlineStr">
         <is>
           <t>第７０話「突貫停止」②</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="0" t="inlineStr">
         <is>
           <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="0" t="inlineStr">
         <is>
           <t>マツモトケンゴ</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="0" t="inlineStr">
         <is>
           <t>第６６話　登山の戦いが始まった（１）</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="0" t="inlineStr">
         <is>
           <t>帰ってください！ 阿久津さん</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="0" t="inlineStr">
         <is>
           <t>長岡太一(著者)</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="0" t="inlineStr">
         <is>
           <t>番外編㉓</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="0" t="inlineStr">
         <is>
           <t>王子様の友達</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="0" t="inlineStr">
         <is>
           <t>すけろく(著者)</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="0" t="inlineStr">
         <is>
           <t>番外編【マンガ総選挙１位・マニフェスト実施】</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="0" t="inlineStr">
         <is>
           <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="0" t="inlineStr">
         <is>
           <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="0" t="inlineStr">
         <is>
           <t>第79話その2</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="0" t="inlineStr">
         <is>
           <t>実は俺、最強でした？</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="0" t="inlineStr">
         <is>
           <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="0" t="inlineStr">
         <is>
           <t>第129話　未知なる脅威!?</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="0" t="inlineStr">
         <is>
           <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="0" t="inlineStr">
         <is>
           <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="0" t="inlineStr">
         <is>
           <t>第11話-2</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="0" t="inlineStr">
         <is>
           <t>金属スライムを倒しまくった俺が【黒鋼の王】と呼ばれるまで</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="0" t="inlineStr">
         <is>
           <t>藤屋いずこ(著者) 温泉カピバラ(原作) 山椒魚(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="0" t="inlineStr">
         <is>
           <t>第15章-2</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="0" t="inlineStr">
         <is>
           <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="0" t="inlineStr">
         <is>
           <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="0" t="inlineStr">
         <is>
           <t>第14話</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="0" t="inlineStr">
         <is>
           <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="0" t="inlineStr">
         <is>
           <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" s="0" t="inlineStr">
         <is>
           <t>第129話　三人の門出（後編）</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="0" t="inlineStr">
         <is>
           <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="0" t="inlineStr">
         <is>
           <t>須河篤志(著者)</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" s="0" t="inlineStr">
         <is>
           <t>第16話前半</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
+      <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="0" t="inlineStr">
         <is>
           <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="0" t="inlineStr">
         <is>
           <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D16" s="0" t="inlineStr">
         <is>
           <t>第５３話　虎の尾を踏む器用貧乏（４）</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
+      <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="0" t="inlineStr">
         <is>
           <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" s="0" t="inlineStr">
         <is>
           <t>三部べべ(漫画) ねうしとら(原作)</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D17" s="0" t="inlineStr">
         <is>
           <t>第3話-1</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
+      <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="0" t="inlineStr">
         <is>
           <t>ダークサモナーとデキている</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="0" t="inlineStr">
         <is>
           <t>車王(著者)</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D18" s="0" t="inlineStr">
         <is>
           <t>第78話</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
+      <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="0" t="inlineStr">
         <is>
           <t>異世界のんびり農家</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" s="0" t="inlineStr">
         <is>
           <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="D19" s="0" t="inlineStr">
         <is>
           <t>第308話</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
+      <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20" s="0" t="inlineStr">
         <is>
           <t>まんきつしたい常連さん</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" s="0" t="inlineStr">
         <is>
           <t>しんみりん(著者)</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="D20" s="0" t="inlineStr">
         <is>
           <t>第49話前編</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
+      <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" s="0" t="inlineStr">
         <is>
           <t>リビルドワールド</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" s="0" t="inlineStr">
         <is>
           <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="D21" s="0" t="inlineStr">
         <is>
           <t>第74話➁</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
+      <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" s="0" t="inlineStr">
         <is>
           <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C22" s="0" t="inlineStr">
         <is>
           <t>島知宏 音速炒飯 有都あらゆる</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="D22" s="0" t="inlineStr">
         <is>
           <t>討伐のお礼ですわ！</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
+      <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B23" s="0" t="inlineStr">
         <is>
           <t>望まぬ不死の冒険者</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C23" s="0" t="inlineStr">
         <is>
           <t>中曽根ハイジ（漫画） 丘野 優（原作） じゃいあん（キャラクター原案）</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="D23" s="0" t="inlineStr">
         <is>
           <t>第61話　早く捨てろ</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
+      <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" s="0" t="inlineStr">
         <is>
           <t>剥かせて！竜ケ崎さん</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C24" s="0" t="inlineStr">
         <is>
           <t>一智和智</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="D24" s="0" t="inlineStr">
         <is>
           <t>大学生編 第15話</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
+      <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" s="0" t="inlineStr">
         <is>
           <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C25" s="0" t="inlineStr">
         <is>
           <t>夜州 nini 藻</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="D25" s="0" t="inlineStr">
         <is>
           <t>第70話(前編)</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
+      <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" s="0" t="inlineStr">
         <is>
           <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C26" s="0" t="inlineStr">
         <is>
           <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="D26" s="0" t="inlineStr">
         <is>
           <t>第35話 独身貴族はバーでハイボールを作る（1）</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
+      <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B27" s="0" t="inlineStr">
         <is>
           <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C27" s="0" t="inlineStr">
         <is>
           <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="D27" s="0" t="inlineStr">
         <is>
           <t>第54話②　闇の女神と仲良くなってみた</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
+      <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" s="0" t="inlineStr">
         <is>
           <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C28" s="0" t="inlineStr">
         <is>
           <t>内々けやき あし カオミン</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D28" s="0" t="inlineStr">
         <is>
           <t>第141話 よくわからないけれど超理論が生み出されたようです（１）</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
+      <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B29" s="0" t="inlineStr">
         <is>
           <t>聖者無双</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C29" s="0" t="inlineStr">
         <is>
           <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="D29" s="0" t="inlineStr">
         <is>
           <t>第93話　妥協ライン（後半）</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
+      <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B30" s="0" t="inlineStr">
         <is>
           <t>ライドンキング</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C30" s="0" t="inlineStr">
         <is>
           <t>馬場康誌</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="D30" s="0" t="inlineStr">
         <is>
           <t>第84話 大統領と賢者の過ち（前編）</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
+      <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B31" s="0" t="inlineStr">
         <is>
           <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C31" s="0" t="inlineStr">
         <is>
           <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="D31" s="0" t="inlineStr">
         <is>
           <t>第10話</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
+      <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B32" s="0" t="inlineStr">
         <is>
           <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C32" s="0" t="inlineStr">
         <is>
           <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="D32" s="0" t="inlineStr">
         <is>
           <t>第48話 緑の塔夏祭り夕食会②</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
+      <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" s="0" t="inlineStr">
         <is>
           <t>小林さんちのメイドラゴン</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C33" s="0" t="inlineStr">
         <is>
           <t>クール教信者</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="D33" s="0" t="inlineStr">
         <is>
           <t>第152話</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
+      <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" s="0" t="inlineStr">
         <is>
           <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C34" s="0" t="inlineStr">
         <is>
           <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="D34" s="0" t="inlineStr">
         <is>
           <t>第7話-2：新しい目標</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
+      <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B35" s="0" t="inlineStr">
         <is>
           <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C35" s="0" t="inlineStr">
         <is>
           <t>六志麻あさ 業務用餅 kisui</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="D35" s="0" t="inlineStr">
         <is>
           <t>第７４話ー①</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
+      <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B36" s="0" t="inlineStr">
         <is>
           <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="C36" s="0" t="inlineStr">
         <is>
           <t>久遠まこと(著者) 石のやっさん(原作)</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="D36" s="0" t="inlineStr">
         <is>
           <t>コミックス６巻発売告知</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
+      <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B37" s="0" t="inlineStr">
         <is>
           <t>理想のヒモ生活</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C37" s="0" t="inlineStr">
         <is>
           <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="D37" s="0" t="inlineStr">
         <is>
           <t>第88話　その3</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
+      <c r="A38" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" s="0" t="inlineStr">
         <is>
           <t>姫様“拷問”の時間です</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="C38" s="0" t="inlineStr">
         <is>
           <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="D38" s="0" t="inlineStr">
         <is>
           <t>拷問153</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
+      <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" s="0" t="inlineStr">
         <is>
           <t>地味子な三葉さんが僕を誘惑する</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="C39" s="0" t="inlineStr">
         <is>
           <t>はぶらえる(著者)</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="D39" s="0" t="inlineStr">
         <is>
           <t>第11話後半</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="n">
+      <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B40" s="0" t="inlineStr">
         <is>
           <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C40" s="0" t="inlineStr">
         <is>
           <t>丈(著者)</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="D40" s="0" t="inlineStr">
         <is>
           <t>第128話</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
+      <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" s="0" t="inlineStr">
         <is>
           <t>俺は星間国家の悪徳領主！</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C41" s="0" t="inlineStr">
         <is>
           <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="D41" s="0" t="inlineStr">
         <is>
           <t>第41話　究極にして至高（前編）</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
+      <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" s="0" t="inlineStr">
         <is>
           <t>ライブダンジョン！</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C42" s="0" t="inlineStr">
         <is>
           <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="D42" s="0" t="inlineStr">
         <is>
           <t>第90話前半</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="n">
+      <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B43" s="0" t="inlineStr">
         <is>
           <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C43" s="0" t="inlineStr">
         <is>
           <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="D43" s="0" t="inlineStr">
         <is>
           <t>【描き下ろしイラスト】休載です！（その２）</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="n">
+      <c r="A44" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B44" s="0" t="inlineStr">
         <is>
           <t>ギャルとダンジョンと周回遅れの探索英雄譚</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C44" s="0" t="inlineStr">
         <is>
           <t>漫画家： 水田ケンジ 原作：榊一郎 キャラクター原案：黒獅子</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="D44" s="0" t="inlineStr">
         <is>
           <t>第4話</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
+      <c r="A45" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B45" s="0" t="inlineStr">
         <is>
           <t>異世界でも無難に生きたい症候群</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="C45" s="0" t="inlineStr">
         <is>
           <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="D45" s="0" t="inlineStr">
         <is>
           <t>第32話①</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="n">
+      <c r="A46" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B46" s="0" t="inlineStr">
         <is>
           <t>アザミヤコを好きになる</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="C46" s="0" t="inlineStr">
         <is>
           <t>ユニティコング(原作) ツノニガウ(作画)</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="D46" s="0" t="inlineStr">
         <is>
           <t>コミックス第2巻情報公開!!!</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="n">
+      <c r="A47" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B47" s="0" t="inlineStr">
         <is>
           <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C47" s="0" t="inlineStr">
         <is>
           <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="D47" s="0" t="inlineStr">
         <is>
           <t>第26話-2</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="n">
+      <c r="A48" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B48" s="0" t="inlineStr">
         <is>
           <t>魔石グルメ　魔物の力を食べたオレは最強！</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="C48" s="0" t="inlineStr">
         <is>
           <t>菅原健二(作画) 結城涼(原作) 成瀬ちさと(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="D48" s="0" t="inlineStr">
         <is>
           <t>第68話後半</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="n">
+      <c r="A49" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B49" s="0" t="inlineStr">
         <is>
           <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C49" s="0" t="inlineStr">
         <is>
           <t>昼行燈（原作） しいたけ元帥（漫画）</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="D49" s="0" t="inlineStr">
         <is>
           <t>第31話</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="n">
+      <c r="A50" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B50" s="0" t="inlineStr">
         <is>
           <t>めっちゃ召喚された件 THE COMIC</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C50" s="0" t="inlineStr">
         <is>
           <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="D50" s="0" t="inlineStr">
         <is>
           <t>第49話①</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="n">
+      <c r="A51" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B51" s="0" t="inlineStr">
         <is>
           <t>最弱貴族に転生したので悪役たちを集めてみた</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C51" s="0" t="inlineStr">
         <is>
           <t>空野進 sorani ファルまろ</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="D51" s="0" t="inlineStr">
         <is>
           <t>第13話　最弱貴族、悪役令嬢に賭けを挑む（２）</t>
         </is>
@@ -11929,6 +11930,1047 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>第72話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>第72話 前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>第33話：誰にも負けない完璧③</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>第７０話「突貫停止」③</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>第40話</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>第138話	虎丸の世界（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>第６６話　登山の戦いが始まった（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>第36話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>第5話 後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>第12話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>第130話　ライアスの苦悩・前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>黒幕一家に転生したけど原作無視して独立する</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>第５話　ゲス子爵を成敗して独立する（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>第309話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>第51話（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>不純な彼女達は懺悔しない</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ポロロッカ(著者)</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>第33話</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>第５４話　勇者を護る器用貧乏（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>第74話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>番外編②　マリーの日記ですわ！</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>第82話　蛇妖女(メデューサ)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>第35話 独身貴族はバーでハイボールを作る（2）</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>第42話　奴は座っている（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>第141話 よくわからないけれど超理論が生み出されたようです（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>モリタ Ｕ４ nima</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>第14話（１）　春とおぼっちゃまとピクニックランチ（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>美人女上司滝沢さん</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>やんBARU(著者)</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>第206話</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>特別編⑳</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>第83話(前編)その3</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>第4話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>衛宮さんちの今日のごはん</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>TAa(漫画) 只野まこと(料理監修) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>第76話</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>物語の黒幕に転生して</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>第35話</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>板垣恵介 林たかあき</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>第56話 暑い夏、再び</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>拷問154</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>アザミヤコを好きになる</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>単行本2巻豪華応援イラスト！！</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>FUNA 東西 モトエ恵介</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>第123話　襲撃［その２］</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>インフィニット・デンドログラム</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>今井神 原作：海道左近 キャラクター原案：タイキ</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>第74話</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>第２０話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Lv２からチートだった元勇者候補のまったり異世界ライフ</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>糸町秋音（漫画） 鬼ノ城ミヤ（原作） 片桐（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>第62話　双子の成長</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>第88話　その4</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>第74話(前編) イダ乱入</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>KAKERU</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>第69話「光の剣」（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>俺は星間国家の悪徳領主！</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>第41話　究極にして至高（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>第6話①「ダブルデート？」</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>第84話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>chapter72【38話①】</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>幼女戦記</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>第百九章：ドードーバード航空戦Ⅳ</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>塔の管理をしてみよう</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>第94話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>第13話　最弱貴族、悪役令嬢に賭けを挑む（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>女子高生の無駄づかい</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>ビーノ(著者)</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>第137話　せいとかい</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>黄金の経験値</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>第19話（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>オタクに優しいギャルはいない!?</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>のりしろちゃん 魚住さかな</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>【特別話】オタクに優しいギャルはいない!?_学生証風ICカードステッカーPR</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>EP.20②</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Add ranking data for 2025-11-03
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -26,6 +26,7 @@
     <sheet name="2025-10-13" sheetId="18" state="visible" r:id="rId18"/>
     <sheet name="2025-10-20" sheetId="19" state="visible" r:id="rId19"/>
     <sheet name="2025-10-27" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="2025-11-03" sheetId="21" state="visible" r:id="rId21"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -11967,22 +11968,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第72話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第72話 前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第33話：誰にも負けない完璧③</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第７０話「突貫停止」③</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第40話</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第138話	虎丸の世界（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第６６話　登山の戦いが始まった（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第36話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第5話 後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第12話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第130話　ライアスの苦悩・前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>黒幕一家に転生したけど原作無視して独立する</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第５話　ゲス子爵を成敗して独立する（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第309話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第51話（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>不純な彼女達は懺悔しない</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>ポロロッカ(著者)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第33話</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第５４話　勇者を護る器用貧乏（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第74話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>番外編②　マリーの日記ですわ！</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第82話　蛇妖女(メデューサ)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第35話 独身貴族はバーでハイボールを作る（2）</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第42話　奴は座っている（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第141話 よくわからないけれど超理論が生み出されたようです（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>モリタ Ｕ４ nima</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第14話（１）　春とおぼっちゃまとピクニックランチ（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>美人女上司滝沢さん</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>やんBARU(著者)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第206話</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>特別編⑳</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第83話(前編)その3</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第4話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>衛宮さんちの今日のごはん</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>TAa(漫画) 只野まこと(料理監修) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第76話</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>物語の黒幕に転生して</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第35話</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 林たかあき</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第56話 暑い夏、再び</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>拷問154</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>アザミヤコを好きになる</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>単行本2巻豪華応援イラスト！！</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>FUNA 東西 モトエ恵介</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第123話　襲撃［その２］</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>インフィニット・デンドログラム</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>今井神 原作：海道左近 キャラクター原案：タイキ</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第74話</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第２０話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>Lv２からチートだった元勇者候補のまったり異世界ライフ</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>糸町秋音（漫画） 鬼ノ城ミヤ（原作） 片桐（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第62話　双子の成長</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第88話　その4</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第74話(前編) イダ乱入</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>KAKERU</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第69話「光の剣」（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>俺は星間国家の悪徳領主！</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第41話　究極にして至高（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第6話①「ダブルデート？」</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第84話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>chapter72【38話①】</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>幼女戦記</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第百九章：ドードーバード航空戦Ⅳ</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>塔の管理をしてみよう</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第94話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第13話　最弱貴族、悪役令嬢に賭けを挑む（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>女子高生の無駄づかい</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>ビーノ(著者)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第137話　せいとかい</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>黄金の経験値</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第19話（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>オタクに優しいギャルはいない!?</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>のりしろちゃん 魚住さかな</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>【特別話】オタクに優しいギャルはいない!?_学生証風ICカードステッカーPR</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>EP.20②</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>丈(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第72話</t>
+          <t>第129話</t>
         </is>
       </c>
     </row>
@@ -11992,17 +13034,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第72話 前編</t>
+          <t>214撃目</t>
         </is>
       </c>
     </row>
@@ -12012,17 +13054,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>zunta(作画) はらわたさいぞう(原作)</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第33話：誰にも負けない完璧③</t>
+          <t>第42話①</t>
         </is>
       </c>
     </row>
@@ -12032,17 +13074,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第７０話「突貫停止」③</t>
+          <t>第18話-2「R18」</t>
         </is>
       </c>
     </row>
@@ -12052,17 +13094,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>蜘蛛ですが、なにか？</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第40話</t>
+          <t>第76話その2</t>
         </is>
       </c>
     </row>
@@ -12072,17 +13114,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>生徒会にも穴はある！</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>むちまろ</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第138話	虎丸の世界（後編）</t>
+          <t>第７０話「突貫停止」④</t>
         </is>
       </c>
     </row>
@@ -12102,7 +13144,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第６６話　登山の戦いが始まった（２）</t>
+          <t>第６７話　サウナの戦いが始まった</t>
         </is>
       </c>
     </row>
@@ -12112,17 +13154,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+          <t>異世界居酒屋「のぶ」</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第36話②</t>
+          <t>第126話</t>
         </is>
       </c>
     </row>
@@ -12132,17 +13174,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+          <t>ダンジョンの幼なじみ</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+          <t>久真やすひさ(著者)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第5話 後編</t>
+          <t>第60話前編</t>
         </is>
       </c>
     </row>
@@ -12152,17 +13194,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第12話-2</t>
+          <t>おまけ66</t>
         </is>
       </c>
     </row>
@@ -12172,17 +13214,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>須河篤志(著者)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第130話　ライアスの苦悩・前編</t>
+          <t>第16話後半</t>
         </is>
       </c>
     </row>
@@ -12192,17 +13234,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>黒幕一家に転生したけど原作無視して独立する</t>
+          <t>帰ってください！ 阿久津さん</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
+          <t>長岡太一(著者)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第５話　ゲス子爵を成敗して独立する（１）</t>
+          <t>第198話</t>
         </is>
       </c>
     </row>
@@ -12212,17 +13254,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>異世界のんびり農家</t>
+          <t>黒幕一家に転生したけど原作無視して独立する</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第309話</t>
+          <t>第５話　ゲス子爵を成敗して独立する（２）</t>
         </is>
       </c>
     </row>
@@ -12232,17 +13274,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>淫獄団地</t>
+          <t>ダークサモナーとデキている</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+          <t>車王(著者)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第51話（後編）</t>
+          <t>第79話</t>
         </is>
       </c>
     </row>
@@ -12252,17 +13294,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>不純な彼女達は懺悔しない</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ポロロッカ(著者)</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第33話</t>
+          <t>第49話後編</t>
         </is>
       </c>
     </row>
@@ -12272,17 +13314,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>「おかえり、パパ」</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>蝉丸</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第５４話　勇者を護る器用貧乏（１）</t>
+          <t>第29話　憧れ</t>
         </is>
       </c>
     </row>
@@ -12292,17 +13334,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第74話③</t>
+          <t>第５４話　勇者を護る器用貧乏（２）</t>
         </is>
       </c>
     </row>
@@ -12312,17 +13354,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+          <t>ライドンキング</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>島知宏 音速炒飯 有都あらゆる</t>
+          <t>馬場康誌</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>番外編②　マリーの日記ですわ！</t>
+          <t>第84話 大統領と賢者の過ち（後編）</t>
         </is>
       </c>
     </row>
@@ -12332,17 +13374,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>板垣恵介 猪原賽 陸井栄史</t>
+          <t>三部べべ(漫画) ねうしとら(原作)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第82話　蛇妖女(メデューサ)</t>
+          <t>第3話-2</t>
         </is>
       </c>
     </row>
@@ -12352,17 +13394,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>異世界のんびり農家</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第35話 独身貴族はバーでハイボールを作る（2）</t>
+          <t>第310話</t>
         </is>
       </c>
     </row>
@@ -12372,17 +13414,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+          <t>Ｓ級ギルドを追放されたけど、実は俺だけドラゴンの言葉がわかるので、気付いたときには竜騎士の頂点を極めてました。</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+          <t>ひそな(漫画) 三木なずな(原作) 白狼(キャラクター原案)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第42話　奴は座っている（後編）</t>
+          <t>第40話-2</t>
         </is>
       </c>
     </row>
@@ -12392,17 +13434,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>姫ヶ崎櫻子は今日も不憫可愛い</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>安田剛助(著者)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第141話 よくわからないけれど超理論が生み出されたようです（２）</t>
+          <t>第51話</t>
         </is>
       </c>
     </row>
@@ -12412,17 +13454,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>モリタ Ｕ４ nima</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第14話（１）　春とおぼっちゃまとピクニックランチ（１）</t>
+          <t>第11話</t>
         </is>
       </c>
     </row>
@@ -12432,17 +13474,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>美人女上司滝沢さん</t>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>やんBARU(著者)</t>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第206話</t>
+          <t>グッズ制作秘話ですわ！</t>
         </is>
       </c>
     </row>
@@ -12452,17 +13494,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>くらいあの子としたいこと</t>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>碇マナツ(著者)</t>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>特別編⑳</t>
+          <t>第35話 独身貴族はバーでハイボールを作る（3）</t>
         </is>
       </c>
     </row>
@@ -12472,17 +13514,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第83話(前編)その3</t>
+          <t>第74話④</t>
         </is>
       </c>
     </row>
@@ -12492,17 +13534,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+          <t>夜州 nini 藻</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第4話前編</t>
+          <t>第70話(後編)</t>
         </is>
       </c>
     </row>
@@ -12512,17 +13554,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>衛宮さんちの今日のごはん</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>TAa(漫画) 只野まこと(料理監修) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第76話</t>
+          <t>第55話①　新居の大掃除をしてみた</t>
         </is>
       </c>
     </row>
@@ -12532,17 +13574,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>物語の黒幕に転生して</t>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第35話</t>
+          <t>第49話 先生と生徒①</t>
         </is>
       </c>
     </row>
@@ -12552,17 +13594,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>板垣恵介 林たかあき</t>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第56話 暑い夏、再び</t>
+          <t>第8話-1：ゼロ発見</t>
         </is>
       </c>
     </row>
@@ -12572,17 +13614,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>英雄王、武を極めるため転生す ～そして、世界最強の見習い騎士♀～</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>漫画‥くろむら基人 原作‥ハヤケン キャラクター原案‥Nagu</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>拷問154</t>
+          <t>第32話 後編</t>
         </is>
       </c>
     </row>
@@ -12592,17 +13634,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>アザミヤコを好きになる</t>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+          <t>三吉汐美(著者)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>単行本2巻豪華応援イラスト！！</t>
+          <t>第18話後半</t>
         </is>
       </c>
     </row>
@@ -12612,17 +13654,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>FUNA 東西 モトエ恵介</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第123話　襲撃［その２］</t>
+          <t>第83話(後編)その1</t>
         </is>
       </c>
     </row>
@@ -12632,17 +13674,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>インフィニット・デンドログラム</t>
+          <t>田舎で恋は難しい!?</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>今井神 原作：海道左近 キャラクター原案：タイキ</t>
+          <t>ねこうめ(著者)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第74話</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -12652,17 +13694,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>ライブダンジョン！</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第２０話②</t>
+          <t>第90話後半</t>
         </is>
       </c>
     </row>
@@ -12672,17 +13714,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Lv２からチートだった元勇者候補のまったり異世界ライフ</t>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>糸町秋音（漫画） 鬼ノ城ミヤ（原作） 片桐（キャラクター原案）</t>
+          <t>セレビィ量産型(著者)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第62話　双子の成長</t>
+          <t>第23話前半</t>
         </is>
       </c>
     </row>
@@ -12692,17 +13734,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第88話　その4</t>
+          <t>拷問155</t>
         </is>
       </c>
     </row>
@@ -12712,17 +13754,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+          <t>はぐはぐ(著者)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第74話(前編) イダ乱入</t>
+          <t>第5話</t>
         </is>
       </c>
     </row>
@@ -12732,17 +13774,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>KAKERU</t>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第69話「光の剣」（後編）</t>
+          <t>第32話</t>
         </is>
       </c>
     </row>
@@ -12752,17 +13794,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>俺は星間国家の悪徳領主！</t>
+          <t>乙女ゲー世界はモブに厳しい世界です【共和国編】</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
+          <t>三嶋与夢(原作) 行々狸(作画) 孟達(キャラクター原案) マツリセイシロウ(構成) FTops(制作)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第41話　究極にして至高（後編）</t>
+          <t>第3話-2</t>
         </is>
       </c>
     </row>
@@ -12772,17 +13814,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
+          <t>めっちゃ召喚された件 THE COMIC</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
+          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第6話①「ダブルデート？」</t>
+          <t>第49話②</t>
         </is>
       </c>
     </row>
@@ -12792,17 +13834,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+          <t>異世界でも無難に生きたい症候群</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第84話後半</t>
+          <t>第32話②</t>
         </is>
       </c>
     </row>
@@ -12812,17 +13854,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+          <t>天獄で悪魔がボクを魅惑する</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>漫画/すたひろ 原作/Y.A</t>
+          <t>銀河味めてお(著者)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>chapter72【38話①】</t>
+          <t>第37話</t>
         </is>
       </c>
     </row>
@@ -12832,17 +13874,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>幼女戦記</t>
+          <t>絶対死なないステラ姫</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
+          <t>光永康則 大高稲</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第百九章：ドードーバード航空戦Ⅳ</t>
+          <t>第１７話　絶対共謀しない（１）</t>
         </is>
       </c>
     </row>
@@ -12852,17 +13894,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>塔の管理をしてみよう</t>
+          <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+          <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第94話前編</t>
+          <t>第6話-2</t>
         </is>
       </c>
     </row>
@@ -12872,17 +13914,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+          <t>ダメ人間の愛しかた</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>空野進 sorani ファルまろ</t>
+          <t>岩葉(著者)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第13話　最弱貴族、悪役令嬢に賭けを挑む（３）</t>
+          <t>第21話後編　ダメ人間と指導する彼女</t>
         </is>
       </c>
     </row>
@@ -12892,17 +13934,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>女子高生の無駄づかい</t>
+          <t>北海道の現役ハンターが異世界に放り込まれてみた 〜エルフ嫁と巡る異世界狩猟ライフ〜</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ビーノ(著者)</t>
+          <t>原作：ジュピタースタジオ「北海道の現役ハンターが異世界に放り込まれてみた」（小学館「ガガガブックス」刊） 漫画：カルトマ キャラクター原案：夕薙</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第137話　せいとかい</t>
+          <t>第27話②</t>
         </is>
       </c>
     </row>
@@ -12912,17 +13954,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>黄金の経験値</t>
+          <t>ひとりぼっちの異世界攻略</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+          <t>びび（漫画） 五示正司（原作）</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第19話（前編）</t>
+          <t>第242話　逆境をひっくり返す</t>
         </is>
       </c>
     </row>
@@ -12932,17 +13974,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>オタクに優しいギャルはいない!?</t>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>のりしろちゃん 魚住さかな</t>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>【特別話】オタクに優しいギャルはいない!?_学生証風ICカードステッカーPR</t>
+          <t>第5話②</t>
         </is>
       </c>
     </row>
@@ -12952,17 +13994,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
+          <t>異世界ではじめる二拠点生活 ～空間魔法で王都と田舎をいったりきたり～</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
+          <t>丸山りん(漫画) 錬金王(原作) あんべよしろう(キャラクター原案)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>EP.20②</t>
+          <t>コミックス第1巻発売告知</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-11-10
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -27,6 +27,7 @@
     <sheet name="2025-10-20" sheetId="19" state="visible" r:id="rId19"/>
     <sheet name="2025-10-27" sheetId="20" state="visible" r:id="rId20"/>
     <sheet name="2025-11-03" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="2025-11-10" sheetId="22" state="visible" r:id="rId22"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -13009,22 +13010,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第129話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>ワンパンマン</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>214撃目</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第42話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第18話-2「R18」</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>蜘蛛ですが、なにか？</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第76話その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第７０話「突貫停止」④</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第６７話　サウナの戦いが始まった</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>異世界居酒屋「のぶ」</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第126話</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンの幼なじみ</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>久真やすひさ(著者)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第60話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>おまけ66</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>クセ強彼女は床にいざなう</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>須河篤志(著者)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第16話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>帰ってください！ 阿久津さん</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>長岡太一(著者)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第198話</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>黒幕一家に転生したけど原作無視して独立する</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第５話　ゲス子爵を成敗して独立する（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>ダークサモナーとデキている</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>車王(著者)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第79話</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>まんきつしたい常連さん</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>しんみりん(著者)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第49話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>「おかえり、パパ」</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>蝉丸</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第29話　憧れ</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第５４話　勇者を護る器用貧乏（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>ライドンキング</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>馬場康誌</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第84話 大統領と賢者の過ち（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>三部べべ(漫画) ねうしとら(原作)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第3話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第310話</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>Ｓ級ギルドを追放されたけど、実は俺だけドラゴンの言葉がわかるので、気付いたときには竜騎士の頂点を極めてました。</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>ひそな(漫画) 三木なずな(原作) 白狼(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第40話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>姫ヶ崎櫻子は今日も不憫可愛い</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>安田剛助(著者)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第51話</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第11話</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>グッズ制作秘話ですわ！</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第35話 独身貴族はバーでハイボールを作る（3）</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第74話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>夜州 nini 藻</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第70話(後編)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第55話①　新居の大掃除をしてみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第49話 先生と生徒①</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第8話-1：ゼロ発見</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>英雄王、武を極めるため転生す ～そして、世界最強の見習い騎士♀～</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>漫画‥くろむら基人 原作‥ハヤケン キャラクター原案‥Nagu</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第32話 後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>三吉汐美(著者)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第18話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第83話(後編)その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>田舎で恋は難しい!?</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>ねこうめ(著者)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>ライブダンジョン！</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第90話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>セレビィ量産型(著者)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第23話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>拷問155</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>はぐはぐ(著者)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第32話</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>乙女ゲー世界はモブに厳しい世界です【共和国編】</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>三嶋与夢(原作) 行々狸(作画) 孟達(キャラクター原案) マツリセイシロウ(構成) FTops(制作)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第3話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>めっちゃ召喚された件 THE COMIC</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第49話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>異世界でも無難に生きたい症候群</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第32話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>天獄で悪魔がボクを魅惑する</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>銀河味めてお(著者)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第37話</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>絶対死なないステラ姫</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>光永康則 大高稲</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第１７話　絶対共謀しない（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第6話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>ダメ人間の愛しかた</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>岩葉(著者)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第21話後編　ダメ人間と指導する彼女</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>北海道の現役ハンターが異世界に放り込まれてみた 〜エルフ嫁と巡る異世界狩猟ライフ〜</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>原作：ジュピタースタジオ「北海道の現役ハンターが異世界に放り込まれてみた」（小学館「ガガガブックス」刊） 漫画：カルトマ キャラクター原案：夕薙</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第27話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>ひとりぼっちの異世界攻略</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>びび（漫画） 五示正司（原作）</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第242話　逆境をひっくり返す</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第5話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>異世界ではじめる二拠点生活 ～空間魔法で王都と田舎をいったりきたり～</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>丸山りん(漫画) 錬金王(原作) あんべよしろう(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>コミックス第1巻発売告知</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！</t>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>丈(著者)</t>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第129話</t>
+          <t>第72話 後編</t>
         </is>
       </c>
     </row>
@@ -13034,17 +14076,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ワンパンマン</t>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>原作/ＯＮＥ 作画/村田雄介</t>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>214撃目</t>
+          <t>おまけ：ジェットバス</t>
         </is>
       </c>
     </row>
@@ -13054,17 +14096,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>生徒会にも穴はある！</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>むちまろ</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第42話①</t>
+          <t>第139話	汐見のしおしお</t>
         </is>
       </c>
     </row>
@@ -13074,17 +14116,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+          <t>とんでもスキルで異世界放浪メシ</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+          <t>赤岸K（漫画） 江口連（原作） 雅（キャラクター原案）</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第18話-2「R18」</t>
+          <t>第56話　「大漁まつり」</t>
         </is>
       </c>
     </row>
@@ -13094,17 +14136,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>蜘蛛ですが、なにか？</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第76話その2</t>
+          <t>第７１話『扇山停止』⓵</t>
         </is>
       </c>
     </row>
@@ -13114,17 +14156,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>王子様の友達</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>すけろく(著者)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第７０話「突貫停止」④</t>
+          <t>第31話</t>
         </is>
       </c>
     </row>
@@ -13134,17 +14176,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第６７話　サウナの戦いが始まった</t>
+          <t>第41話</t>
         </is>
       </c>
     </row>
@@ -13154,17 +14196,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>異世界居酒屋「のぶ」</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第126話</t>
+          <t>第６８話　ナイトプールの戦いが始まった（１）</t>
         </is>
       </c>
     </row>
@@ -13174,17 +14216,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ダンジョンの幼なじみ</t>
+          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>久真やすひさ(著者)</t>
+          <t>久遠まこと(著者) 石のやっさん(原作)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第60話前編</t>
+          <t>第31話</t>
         </is>
       </c>
     </row>
@@ -13194,17 +14236,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>おまけ66</t>
+          <t>第80話その1</t>
         </is>
       </c>
     </row>
@@ -13214,17 +14256,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>クセ強彼女は床にいざなう</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>須河篤志(著者)</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第16話後半</t>
+          <t>第130話　ライアスの苦悩・後編</t>
         </is>
       </c>
     </row>
@@ -13234,17 +14276,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>帰ってください！ 阿久津さん</t>
+          <t>このヒーラー、めんどくさい</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>長岡太一(著者)</t>
+          <t>丹念に発酵(著者)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第198話</t>
+          <t>「コミックス９巻発売記念！　カーラたちが探検中に転移魔法陣を踏んで飛ばされた先を大募集！」結果発表マンガ</t>
         </is>
       </c>
     </row>
@@ -13254,17 +14296,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>黒幕一家に転生したけど原作無視して独立する</t>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第５話　ゲス子爵を成敗して独立する（２）</t>
+          <t>第15話</t>
         </is>
       </c>
     </row>
@@ -13274,17 +14316,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ダークサモナーとデキている</t>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>車王(著者)</t>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第79話</t>
+          <t>第26話①</t>
         </is>
       </c>
     </row>
@@ -13294,17 +14336,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>まんきつしたい常連さん</t>
+          <t>美人女上司滝沢さん</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>しんみりん(著者)</t>
+          <t>やんBARU(著者)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第49話後編</t>
+          <t>第207話</t>
         </is>
       </c>
     </row>
@@ -13314,17 +14356,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>「おかえり、パパ」</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>蝉丸</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第29話　憧れ</t>
+          <t>第130話　変身してみる（前編）</t>
         </is>
       </c>
     </row>
@@ -13344,7 +14386,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第５４話　勇者を護る器用貧乏（２）</t>
+          <t>第５４話　勇者を護る器用貧乏（３）</t>
         </is>
       </c>
     </row>
@@ -13354,17 +14396,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ライドンキング</t>
+          <t>魔のものたちは企てる</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>馬場康誌</t>
+          <t>加藤拓弐(原作) ガしガし(作画)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第84話 大統領と賢者の過ち（後編）</t>
+          <t>第31話</t>
         </is>
       </c>
     </row>
@@ -13374,17 +14416,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
+          <t>不純な彼女達は懺悔しない</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>三部べべ(漫画) ねうしとら(原作)</t>
+          <t>ポロロッカ(著者)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第3話-2</t>
+          <t>休載イラスト</t>
         </is>
       </c>
     </row>
@@ -13394,17 +14436,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>異世界のんびり農家</t>
+          <t>アザミヤコを好きになる</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第310話</t>
+          <t>第11話前編</t>
         </is>
       </c>
     </row>
@@ -13414,17 +14456,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Ｓ級ギルドを追放されたけど、実は俺だけドラゴンの言葉がわかるので、気付いたときには竜騎士の頂点を極めてました。</t>
+          <t>ライドンキング</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ひそな(漫画) 三木なずな(原作) 白狼(キャラクター原案)</t>
+          <t>馬場康誌</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第40話-2</t>
+          <t>第85話 大統領と宇宙を突く拳</t>
         </is>
       </c>
     </row>
@@ -13434,17 +14476,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>姫ヶ崎櫻子は今日も不憫可愛い</t>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>安田剛助(著者)</t>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第51話</t>
+          <t>第83話　ゴーゴン三姉妹</t>
         </is>
       </c>
     </row>
@@ -13454,17 +14496,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第11話</t>
+          <t>第75話①</t>
         </is>
       </c>
     </row>
@@ -13484,7 +14526,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>グッズ制作秘話ですわ！</t>
+          <t>第２５食　赤スライムのシャーベット、パクパクですわ！（１）</t>
         </is>
       </c>
     </row>
@@ -13504,7 +14546,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第35話 独身貴族はバーでハイボールを作る（3）</t>
+          <t>第35話 独身貴族はバーでハイボールを作る（4）</t>
         </is>
       </c>
     </row>
@@ -13514,17 +14556,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第74話④</t>
+          <t>第142話 よくわからないけれど後始末するみたいです（１）</t>
         </is>
       </c>
     </row>
@@ -13534,17 +14576,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>夜州 nini 藻</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第70話(後編)</t>
+          <t>第55話②　新居の大掃除をしてみた</t>
         </is>
       </c>
     </row>
@@ -13554,17 +14596,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>モリタ Ｕ４ nima</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第55話①　新居の大掃除をしてみた</t>
+          <t>第14話（２）　春とおぼっちゃまとピクニックランチ（２）</t>
         </is>
       </c>
     </row>
@@ -13574,17 +14616,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第49話 先生と生徒①</t>
+          <t>第4話中編</t>
         </is>
       </c>
     </row>
@@ -13594,17 +14636,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+          <t>小林さんちのメイドラゴン</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+          <t>クール教信者</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第8話-1：ゼロ発見</t>
+          <t>第153話</t>
         </is>
       </c>
     </row>
@@ -13614,17 +14656,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>英雄王、武を極めるため転生す ～そして、世界最強の見習い騎士♀～</t>
+          <t>聖者無双</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>漫画‥くろむら基人 原作‥ハヤケン キャラクター原案‥Nagu</t>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第32話 後編</t>
+          <t>第94話　戦乱のドワーフ王国・奴隷の扱い（前半）</t>
         </is>
       </c>
     </row>
@@ -13634,17 +14676,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>アイドル辞めるけど結婚してくれますか!?</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>三吉汐美(著者)</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第18話後半</t>
+          <t>拷問156</t>
         </is>
       </c>
     </row>
@@ -13654,17 +14696,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>田舎で恋は難しい!?</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>ねこうめ(著者)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第83話(後編)その1</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -13674,17 +14716,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>田舎で恋は難しい!?</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ねこうめ(著者)</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第83話(後編)その2</t>
         </is>
       </c>
     </row>
@@ -13694,17 +14736,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ライブダンジョン！</t>
+          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第90話後半</t>
+          <t>第59話　別れと、出立（前編）</t>
         </is>
       </c>
     </row>
@@ -13714,17 +14756,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>三枝さんはメガネ先輩と恋を描く</t>
+          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>セレビィ量産型(著者)</t>
+          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第23話前半</t>
+          <t>第40話-2</t>
         </is>
       </c>
     </row>
@@ -13734,17 +14776,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>板垣恵介 林たかあき</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>拷問155</t>
+          <t>第57話 銃撃戦</t>
         </is>
       </c>
     </row>
@@ -13754,17 +14796,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>サーシャちゃんとクラスメイトオタクくん</t>
+          <t>くらいあの子としたいこと</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>はぐはぐ(著者)</t>
+          <t>碇マナツ(著者)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第5話</t>
+          <t>特別編㉑</t>
         </is>
       </c>
     </row>
@@ -13774,17 +14816,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第32話</t>
+          <t>第89話　その1</t>
         </is>
       </c>
     </row>
@@ -13794,17 +14836,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>乙女ゲー世界はモブに厳しい世界です【共和国編】</t>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>三嶋与夢(原作) 行々狸(作画) 孟達(キャラクター原案) マツリセイシロウ(構成) FTops(制作)</t>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第3話-2</t>
+          <t>第２０話③</t>
         </is>
       </c>
     </row>
@@ -13814,17 +14856,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>めっちゃ召喚された件 THE COMIC</t>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
+          <t>六志麻あさ 業務用餅 kisui</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第49話②</t>
+          <t>第７４話ー②</t>
         </is>
       </c>
     </row>
@@ -13834,17 +14876,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>異世界でも無難に生きたい症候群</t>
+          <t>地味子な三葉さんが僕を誘惑する</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
+          <t>はぶらえる(著者)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第32話②</t>
+          <t>第12話前半</t>
         </is>
       </c>
     </row>
@@ -13854,17 +14896,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>天獄で悪魔がボクを魅惑する</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>銀河味めてお(著者)</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第37話</t>
+          <t>【描き下ろしイラスト】休載です！（その4）</t>
         </is>
       </c>
     </row>
@@ -13874,17 +14916,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>絶対死なないステラ姫</t>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>光永康則 大高稲</t>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第１７話　絶対共謀しない（１）</t>
+          <t>コミックス第4巻発売告知</t>
         </is>
       </c>
     </row>
@@ -13894,17 +14936,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ラスボス討伐後に始める二周目冒険者ライフ はじまりの街でワケあり美少女たちがめちゃくちゃ懐いてきます</t>
+          <t>黄金の経験値</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>鬼麻正明(漫画) 朱月十話(原作) ファルまろ(キャラ原案)</t>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第6話-2</t>
+          <t>第19話（後編）</t>
         </is>
       </c>
     </row>
@@ -13914,17 +14956,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ダメ人間の愛しかた</t>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>岩葉(著者)</t>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第21話後編　ダメ人間と指導する彼女</t>
+          <t>第7話　ショッピングデート（前編）</t>
         </is>
       </c>
     </row>
@@ -13934,17 +14976,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>北海道の現役ハンターが異世界に放り込まれてみた 〜エルフ嫁と巡る異世界狩猟ライフ〜</t>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>原作：ジュピタースタジオ「北海道の現役ハンターが異世界に放り込まれてみた」（小学館「ガガガブックス」刊） 漫画：カルトマ キャラクター原案：夕薙</t>
+          <t>漫画/すたひろ 原作/Y.A</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第27話②</t>
+          <t>chapter73【38話②】</t>
         </is>
       </c>
     </row>
@@ -13954,17 +14996,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ひとりぼっちの異世界攻略</t>
+          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>びび（漫画） 五示正司（原作）</t>
+          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第242話　逆境をひっくり返す</t>
+          <t>第27話-1</t>
         </is>
       </c>
     </row>
@@ -13974,17 +15016,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+          <t>塔の管理をしてみよう</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第5話②</t>
+          <t>第94話後編</t>
         </is>
       </c>
     </row>
@@ -13994,17 +15036,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>異世界ではじめる二拠点生活 ～空間魔法で王都と田舎をいったりきたり～</t>
+          <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>丸山りん(漫画) 錬金王(原作) あんべよしろう(キャラクター原案)</t>
+          <t>丈(著者)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>コミックス第1巻発売告知</t>
+          <t>第129話</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-11-17
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -28,6 +28,7 @@
     <sheet name="2025-10-27" sheetId="20" state="visible" r:id="rId20"/>
     <sheet name="2025-11-03" sheetId="21" state="visible" r:id="rId21"/>
     <sheet name="2025-11-10" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="2025-11-17" sheetId="23" state="visible" r:id="rId23"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -14051,22 +14052,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第72話 後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>おまけ：ジェットバス</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第139話	汐見のしおしお</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>とんでもスキルで異世界放浪メシ</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>赤岸K（漫画） 江口連（原作） 雅（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第56話　「大漁まつり」</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第７１話『扇山停止』⓵</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>王子様の友達</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>すけろく(著者)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第31話</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第41話</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第６８話　ナイトプールの戦いが始まった（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>久遠まこと(著者) 石のやっさん(原作)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第31話</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第80話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第130話　ライアスの苦悩・後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>このヒーラー、めんどくさい</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>丹念に発酵(著者)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>「コミックス９巻発売記念！　カーラたちが探検中に転移魔法陣を踏んで飛ばされた先を大募集！」結果発表マンガ</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第15話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第26話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>美人女上司滝沢さん</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>やんBARU(著者)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第207話</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第130話　変身してみる（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第５４話　勇者を護る器用貧乏（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>魔のものたちは企てる</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>加藤拓弐(原作) ガしガし(作画)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第31話</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>不純な彼女達は懺悔しない</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>ポロロッカ(著者)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>アザミヤコを好きになる</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第11話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>ライドンキング</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>馬場康誌</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第85話 大統領と宇宙を突く拳</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第83話　ゴーゴン三姉妹</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第75話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第２５食　赤スライムのシャーベット、パクパクですわ！（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第35話 独身貴族はバーでハイボールを作る（4）</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第142話 よくわからないけれど後始末するみたいです（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第55話②　新居の大掃除をしてみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>モリタ Ｕ４ nima</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第14話（２）　春とおぼっちゃまとピクニックランチ（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第4話中編</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>小林さんちのメイドラゴン</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>クール教信者</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第153話</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>聖者無双</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第94話　戦乱のドワーフ王国・奴隷の扱い（前半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>拷問156</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>田舎で恋は難しい!?</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>ねこうめ(著者)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第83話(後編)その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第59話　別れと、出立（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第40話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 林たかあき</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第57話 銃撃戦</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>特別編㉑</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第89話　その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第２０話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>六志麻あさ 業務用餅 kisui</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第７４話ー②</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>地味子な三葉さんが僕を誘惑する</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>はぶらえる(著者)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第12話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>【描き下ろしイラスト】休載です！（その4）</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>コミックス第4巻発売告知</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>黄金の経験値</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第19話（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第7話　ショッピングデート（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>chapter73【38話②】</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第27話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>塔の管理をしてみよう</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第94話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第129話</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第72話 後編</t>
+          <t>215撃目</t>
         </is>
       </c>
     </row>
@@ -14076,17 +15118,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+          <t>異種族レビュアーズ</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>zunta(作画) はらわたさいぞう(原作)</t>
+          <t>天原(原作) masha(作画)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>おまけ：ジェットバス</t>
+          <t>第88話</t>
         </is>
       </c>
     </row>
@@ -14096,17 +15138,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>生徒会にも穴はある！</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>むちまろ</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第139話	汐見のしおしお</t>
+          <t>第42話➁</t>
         </is>
       </c>
     </row>
@@ -14116,17 +15158,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>とんでもスキルで異世界放浪メシ</t>
+          <t>不徳のギルド</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>赤岸K（漫画） 江口連（原作） 雅（キャラクター原案）</t>
+          <t>河添太一</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第56話　「大漁まつり」</t>
+          <t>第１００話：ガードウォーズ</t>
         </is>
       </c>
     </row>
@@ -14136,17 +15178,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第７１話『扇山停止』⓵</t>
+          <t>第19話-1「今日も特別な日」</t>
         </is>
       </c>
     </row>
@@ -14156,17 +15198,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>王子様の友達</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>すけろく(著者)</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第31話</t>
+          <t>第７１話『扇山停止』②</t>
         </is>
       </c>
     </row>
@@ -14176,17 +15218,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>魔王の俺が奴隷エルフを嫁にしたんだが、どう愛でればいい？</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>原作／手島史詞 キャラクター原案／COMTA 漫画／板垣ハコ</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第41話</t>
+          <t>第74話</t>
         </is>
       </c>
     </row>
@@ -14206,7 +15248,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第６８話　ナイトプールの戦いが始まった（１）</t>
+          <t>第６８話　ナイトプールの戦いが始まった（２）</t>
         </is>
       </c>
     </row>
@@ -14216,17 +15258,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>久遠まこと(著者) 石のやっさん(原作)</t>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第31話</t>
+          <t>第13話-1</t>
         </is>
       </c>
     </row>
@@ -14236,17 +15278,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第80話その1</t>
+          <t>第131話　画策</t>
         </is>
       </c>
     </row>
@@ -14256,17 +15298,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>ダンジョンの幼なじみ</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>久真やすひさ(著者)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第130話　ライアスの苦悩・後編</t>
+          <t>第60話後編</t>
         </is>
       </c>
     </row>
@@ -14276,17 +15318,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>このヒーラー、めんどくさい</t>
+          <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>丹念に発酵(著者)</t>
+          <t>須河篤志(著者)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>「コミックス９巻発売記念！　カーラたちが探検中に転移魔法陣を踏んで飛ばされた先を大募集！」結果発表マンガ</t>
+          <t>第17話前半</t>
         </is>
       </c>
     </row>
@@ -14296,17 +15338,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+          <t>帰ってください！ 阿久津さん</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+          <t>長岡太一(著者)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第15話</t>
+          <t>番外編㉔</t>
         </is>
       </c>
     </row>
@@ -14316,17 +15358,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>女友達は頼めば意外とヤらせてくれる</t>
+          <t>ダークサモナーとデキている</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ろくろ(漫画) 鏡遊(原作)</t>
+          <t>車王(著者)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第26話①</t>
+          <t>第80話</t>
         </is>
       </c>
     </row>
@@ -14336,17 +15378,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>美人女上司滝沢さん</t>
+          <t>寿司ガキ</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>やんBARU(著者)</t>
+          <t>ichika(著者)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第207話</t>
+          <t>電撃だいおうじVOL.145出張版</t>
         </is>
       </c>
     </row>
@@ -14366,7 +15408,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第130話　変身してみる（前編）</t>
+          <t>第130話　変身してみる（中編）</t>
         </is>
       </c>
     </row>
@@ -14376,17 +15418,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第５４話　勇者を護る器用貧乏（３）</t>
+          <t>第50話前編</t>
         </is>
       </c>
     </row>
@@ -14396,17 +15438,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>魔のものたちは企てる</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>加藤拓弐(原作) ガしガし(作画)</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第31話</t>
+          <t>第５４話　勇者を護る器用貧乏（４）</t>
         </is>
       </c>
     </row>
@@ -14416,17 +15458,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>不純な彼女達は懺悔しない</t>
+          <t>ライドンキング</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ポロロッカ(著者)</t>
+          <t>馬場康誌</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>休載イラスト</t>
+          <t>最終話 大統領と新たなる騎乗序曲</t>
         </is>
       </c>
     </row>
@@ -14436,17 +15478,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>アザミヤコを好きになる</t>
+          <t>淫獄団地</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第11話前編</t>
+          <t>第52話（前編）</t>
         </is>
       </c>
     </row>
@@ -14456,17 +15498,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ライドンキング</t>
+          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>馬場康誌</t>
+          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第85話 大統領と宇宙を突く拳</t>
+          <t>連載再開告知</t>
         </is>
       </c>
     </row>
@@ -14476,17 +15518,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>板垣恵介 猪原賽 陸井栄史</t>
+          <t>三部べべ(漫画) ねうしとら(原作)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第83話　ゴーゴン三姉妹</t>
+          <t>第4話-1</t>
         </is>
       </c>
     </row>
@@ -14506,7 +15548,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第75話①</t>
+          <t>第75話➁</t>
         </is>
       </c>
     </row>
@@ -14526,7 +15568,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第２５食　赤スライムのシャーベット、パクパクですわ！（１）</t>
+          <t>第２５食　赤スライムのシャーベット、パクパクですわ！（２）</t>
         </is>
       </c>
     </row>
@@ -14536,17 +15578,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第35話 独身貴族はバーでハイボールを作る（4）</t>
+          <t>休載イラスト</t>
         </is>
       </c>
     </row>
@@ -14556,17 +15598,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第142話 よくわからないけれど後始末するみたいです（１）</t>
+          <t>第43話　奴は祝う（前編）</t>
         </is>
       </c>
     </row>
@@ -14576,17 +15618,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>夜州 nini 藻</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第55話②　新居の大掃除をしてみた</t>
+          <t>第71話(前編)</t>
         </is>
       </c>
     </row>
@@ -14596,17 +15638,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
+          <t>路地裏で拾った女の子がバッドエンド後の乙女ゲームのヒロインだった件</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>モリタ Ｕ４ nima</t>
+          <t>カボチャマスク(原作) 樋乃えなが(作画) へいろー(キャラクター原案)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第14話（２）　春とおぼっちゃまとピクニックランチ（２）</t>
+          <t>第4話</t>
         </is>
       </c>
     </row>
@@ -14616,17 +15658,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第4話中編</t>
+          <t>第8話-2：ゼロ発見</t>
         </is>
       </c>
     </row>
@@ -14636,17 +15678,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>小林さんちのメイドラゴン</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>クール教信者</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第153話</t>
+          <t>第142話 よくわからないけれど後始末するみたいです（２）</t>
         </is>
       </c>
     </row>
@@ -14656,17 +15698,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>聖者無双</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第94話　戦乱のドワーフ王国・奴隷の扱い（前半）</t>
+          <t>第56話①　ペットを飼ってみた</t>
         </is>
       </c>
     </row>
@@ -14676,17 +15718,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>「おかえり、パパ」</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>蝉丸</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>拷問156</t>
+          <t>単行本5巻限定描きおろし「過去」試し読み</t>
         </is>
       </c>
     </row>
@@ -14696,17 +15738,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>田舎で恋は難しい!?</t>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>ねこうめ(著者)</t>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第49話 先生と生徒②</t>
         </is>
       </c>
     </row>
@@ -14726,7 +15768,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第83話(後編)その2</t>
+          <t>第83話(後編)その3</t>
         </is>
       </c>
     </row>
@@ -14736,17 +15778,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第59話　別れと、出立（前編）</t>
+          <t>第４３話　勇者、合体した六邪神将を撃破し、めでたしめでたし（１）</t>
         </is>
       </c>
     </row>
@@ -14756,17 +15798,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
+          <t>北斗の拳 世紀末ドラマ撮影伝</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
+          <t>原案/武論尊・原哲夫 漫画/倉尾宏</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第40話-2</t>
+          <t>第76話 柏葉、最後の目覚め!!</t>
         </is>
       </c>
     </row>
@@ -14776,17 +15818,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>板垣恵介 林たかあき</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第57話 銃撃戦</t>
+          <t>拷問157</t>
         </is>
       </c>
     </row>
@@ -14796,17 +15838,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>くらいあの子としたいこと</t>
+          <t>おとなりのダウナーさんは無理させない</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>碇マナツ(著者)</t>
+          <t>瑠璃いろ(著者)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>特別編㉑</t>
+          <t>コミックス告知</t>
         </is>
       </c>
     </row>
@@ -14816,17 +15858,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>バーサス</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第89話　その1</t>
+          <t>第29話 魔王VS.ロボット（前編-1）</t>
         </is>
       </c>
     </row>
@@ -14836,17 +15878,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第２０話③</t>
+          <t>第89話　その2</t>
         </is>
       </c>
     </row>
@@ -14856,17 +15898,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+          <t>俺は星間国家の悪徳領主！</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>六志麻あさ 業務用餅 kisui</t>
+          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第７４話ー②</t>
+          <t>第42話　人生終了</t>
         </is>
       </c>
     </row>
@@ -14876,17 +15918,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>地味子な三葉さんが僕を誘惑する</t>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>はぶらえる(著者)</t>
+          <t>セレビィ量産型(著者)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第12話前半</t>
+          <t>第23話後半</t>
         </is>
       </c>
     </row>
@@ -14896,17 +15938,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>【描き下ろしイラスト】休載です！（その4）</t>
+          <t>第74話(後編) イダ乱入</t>
         </is>
       </c>
     </row>
@@ -14916,17 +15958,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+          <t>ライブダンジョン！</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>コミックス第4巻発売告知</t>
+          <t>第91話前半</t>
         </is>
       </c>
     </row>
@@ -14936,17 +15978,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>黄金の経験値</t>
+          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第19話（後編）</t>
+          <t>第59話　別れと、出立（後編）</t>
         </is>
       </c>
     </row>
@@ -14956,17 +15998,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+          <t>英雄女騎士に有能とバレた俺の美人ハーレム騎士団 ガイカク・ヒクメの奇術騎士団</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+          <t>明石六郎(原作) 太盛(作画) 氷室しゅんすけ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第7話　ショッピングデート（前編）</t>
+          <t>第12話-2</t>
         </is>
       </c>
     </row>
@@ -14976,17 +16018,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+          <t>異世界でも無難に生きたい症候群</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>漫画/すたひろ 原作/Y.A</t>
+          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>chapter73【38話②】</t>
+          <t>第32話③</t>
         </is>
       </c>
     </row>
@@ -14996,17 +16038,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
+          <t>女子高生の無駄づかい</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
+          <t>ビーノ(著者)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第27話-1</t>
+          <t>第138話　にんめい</t>
         </is>
       </c>
     </row>
@@ -15016,17 +16058,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>塔の管理をしてみよう</t>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+          <t>KAKERU</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第94話後編</t>
+          <t>第70話「あうと！ せーふ！ よよいのよい！（もうどうにでもなぁれ♡）」（後半)</t>
         </is>
       </c>
     </row>
@@ -15036,17 +16078,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！</t>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>丈(著者)</t>
+          <t>空野進 sorani ファルまろ</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第129話</t>
+          <t>第14話　最弱貴族、悪役令嬢を脱がす（１）</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-11-24
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -29,6 +29,7 @@
     <sheet name="2025-11-03" sheetId="21" state="visible" r:id="rId21"/>
     <sheet name="2025-11-10" sheetId="22" state="visible" r:id="rId22"/>
     <sheet name="2025-11-17" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="2025-11-24" sheetId="24" state="visible" r:id="rId24"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -15093,22 +15094,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>ワンパンマン</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>215撃目</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>異種族レビュアーズ</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>天原(原作) masha(作画)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第88話</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第42話➁</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>不徳のギルド</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>河添太一</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第１００話：ガードウォーズ</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第19話-1「今日も特別な日」</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第７１話『扇山停止』②</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>魔王の俺が奴隷エルフを嫁にしたんだが、どう愛でればいい？</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>原作／手島史詞 キャラクター原案／COMTA 漫画／板垣ハコ</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第74話</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第６８話　ナイトプールの戦いが始まった（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第13話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第131話　画策</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンの幼なじみ</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>久真やすひさ(著者)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第60話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>クセ強彼女は床にいざなう</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>須河篤志(著者)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第17話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>帰ってください！ 阿久津さん</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>長岡太一(著者)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>番外編㉔</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>ダークサモナーとデキている</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>車王(著者)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第80話</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>寿司ガキ</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>ichika(著者)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>電撃だいおうじVOL.145出張版</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第130話　変身してみる（中編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>まんきつしたい常連さん</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>しんみりん(著者)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第50話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第５４話　勇者を護る器用貧乏（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>ライドンキング</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>馬場康誌</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>最終話 大統領と新たなる騎乗序曲</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第52話（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>連載再開告知</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>三部べべ(漫画) ねうしとら(原作)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第4話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第75話➁</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第２５食　赤スライムのシャーベット、パクパクですわ！（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第43話　奴は祝う（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>夜州 nini 藻</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第71話(前編)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>路地裏で拾った女の子がバッドエンド後の乙女ゲームのヒロインだった件</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>カボチャマスク(原作) 樋乃えなが(作画) へいろー(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第4話</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第8話-2：ゼロ発見</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第142話 よくわからないけれど後始末するみたいです（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第56話①　ペットを飼ってみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>「おかえり、パパ」</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>蝉丸</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>単行本5巻限定描きおろし「過去」試し読み</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第49話 先生と生徒②</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第83話(後編)その3</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第４３話　勇者、合体した六邪神将を撃破し、めでたしめでたし（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>北斗の拳 世紀末ドラマ撮影伝</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>原案/武論尊・原哲夫 漫画/倉尾宏</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第76話 柏葉、最後の目覚め!!</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>拷問157</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>おとなりのダウナーさんは無理させない</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>瑠璃いろ(著者)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>コミックス告知</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>バーサス</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第29話 魔王VS.ロボット（前編-1）</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第89話　その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>俺は星間国家の悪徳領主！</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第42話　人生終了</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>セレビィ量産型(著者)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第23話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第74話(後編) イダ乱入</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>ライブダンジョン！</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第91話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第59話　別れと、出立（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>英雄女騎士に有能とバレた俺の美人ハーレム騎士団 ガイカク・ヒクメの奇術騎士団</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>明石六郎(原作) 太盛(作画) 氷室しゅんすけ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第12話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>異世界でも無難に生きたい症候群</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第32話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>女子高生の無駄づかい</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>ビーノ(著者)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第138話　にんめい</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>KAKERU</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第70話「あうと！ せーふ！ よよいのよい！（もうどうにでもなぁれ♡）」（後半)</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第14話　最弱貴族、悪役令嬢を脱がす（１）</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ワンパンマン</t>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>原作/ＯＮＥ 作画/村田雄介</t>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>215撃目</t>
+          <t>第73話 前編</t>
         </is>
       </c>
     </row>
@@ -15118,17 +16160,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>異種族レビュアーズ</t>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>天原(原作) masha(作画)</t>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第88話</t>
+          <t>コミックス第1巻 発売告知記事</t>
         </is>
       </c>
     </row>
@@ -15138,17 +16180,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第42話➁</t>
+          <t>第42話</t>
         </is>
       </c>
     </row>
@@ -15158,17 +16200,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>不徳のギルド</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>河添太一</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第１００話：ガードウォーズ</t>
+          <t>第７１話『扇山停止』③</t>
         </is>
       </c>
     </row>
@@ -15178,17 +16220,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+          <t>生徒会にも穴はある！</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+          <t>むちまろ</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第19話-1「今日も特別な日」</t>
+          <t>第140話	蚊がせめてきたぞっ!!</t>
         </is>
       </c>
     </row>
@@ -15198,17 +16240,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第７１話『扇山停止』②</t>
+          <t>第６９話　爺ちゃんとの戦いが始まった（１）</t>
         </is>
       </c>
     </row>
@@ -15218,17 +16260,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>魔王の俺が奴隷エルフを嫁にしたんだが、どう愛でればいい？</t>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>原作／手島史詞 キャラクター原案／COMTA 漫画／板垣ハコ</t>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第74話</t>
+          <t>第80話その2</t>
         </is>
       </c>
     </row>
@@ -15238,17 +16280,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第６８話　ナイトプールの戦いが始まった（２）</t>
+          <t>第132話　画伯の願い</t>
         </is>
       </c>
     </row>
@@ -15258,17 +16300,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第13話-1</t>
+          <t>第16話</t>
         </is>
       </c>
     </row>
@@ -15278,17 +16320,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第131話　画策</t>
+          <t>第26話②</t>
         </is>
       </c>
     </row>
@@ -15298,17 +16340,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ダンジョンの幼なじみ</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>久真やすひさ(著者)</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第60話後編</t>
+          <t>第130話　変身してみる（後編）</t>
         </is>
       </c>
     </row>
@@ -15318,17 +16360,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>クセ強彼女は床にいざなう</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>須河篤志(著者)</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第17話前半</t>
+          <t>第５４話　勇者を護る器用貧乏（４）</t>
         </is>
       </c>
     </row>
@@ -15338,17 +16380,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>帰ってください！ 阿久津さん</t>
+          <t>異世界のんびり農家</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>長岡太一(著者)</t>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>番外編㉔</t>
+          <t>第311話</t>
         </is>
       </c>
     </row>
@@ -15358,17 +16400,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ダークサモナーとデキている</t>
+          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>車王(著者)</t>
+          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第80話</t>
+          <t>第10話</t>
         </is>
       </c>
     </row>
@@ -15378,17 +16420,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>寿司ガキ</t>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ichika(著者)</t>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>電撃だいおうじVOL.145出張版</t>
+          <t>第84話　慈愛</t>
         </is>
       </c>
     </row>
@@ -15398,17 +16440,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>異世界魔王と召喚少女の奴隷魔術</t>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第130話　変身してみる（中編）</t>
+          <t>第２５食　赤スライムのシャーベット、パクパクですわ！（３）</t>
         </is>
       </c>
     </row>
@@ -15418,17 +16460,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>まんきつしたい常連さん</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>しんみりん(著者)</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第50話前編</t>
+          <t>第75話③</t>
         </is>
       </c>
     </row>
@@ -15438,17 +16480,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第５４話　勇者を護る器用貧乏（４）</t>
+          <t>第12話</t>
         </is>
       </c>
     </row>
@@ -15458,17 +16500,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ライドンキング</t>
+          <t>アザミヤコを好きになる</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>馬場康誌</t>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>最終話 大統領と新たなる騎乗序曲</t>
+          <t>第11話後編</t>
         </is>
       </c>
     </row>
@@ -15478,17 +16520,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>淫獄団地</t>
+          <t>美人女上司滝沢さん</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+          <t>やんBARU(著者)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第52話（前編）</t>
+          <t>第208話</t>
         </is>
       </c>
     </row>
@@ -15498,17 +16540,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
+          <t>貞操逆転世界で頼めばヤれると噂の俺</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
+          <t>澄田佑貴(漫画) aaa168（スリーエー）(原作)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>連載再開告知</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -15518,17 +16560,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>三部べべ(漫画) ねうしとら(原作)</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第4話-1</t>
+          <t>第56話②　ペットを飼ってみた</t>
         </is>
       </c>
     </row>
@@ -15538,17 +16580,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第75話➁</t>
+          <t>第143話 よくわからないけれど人をダメにするみたいです（１）</t>
         </is>
       </c>
     </row>
@@ -15558,17 +16600,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+          <t>聖者無双</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>島知宏 音速炒飯 有都あらゆる</t>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第２５食　赤スライムのシャーベット、パクパクですわ！（２）</t>
+          <t>第94話　戦乱のドワーフ王国・奴隷の扱い（後半）</t>
         </is>
       </c>
     </row>
@@ -15578,17 +16620,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+          <t>モリタ Ｕ４ nima</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>休載イラスト</t>
+          <t>第14話（３）　春とおぼっちゃまとピクニックランチ（３）</t>
         </is>
       </c>
     </row>
@@ -15598,17 +16640,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第43話　奴は祝う（前編）</t>
+          <t>第４３話　勇者、合体した六邪神将を撃破し、めでたしめでたし（２）</t>
         </is>
       </c>
     </row>
@@ -15618,17 +16660,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>夜州 nini 藻</t>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第71話(前編)</t>
+          <t>第4話後編</t>
         </is>
       </c>
     </row>
@@ -15638,17 +16680,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>路地裏で拾った女の子がバッドエンド後の乙女ゲームのヒロインだった件</t>
+          <t>小林さんちのメイドラゴン</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>カボチャマスク(原作) 樋乃えなが(作画) へいろー(キャラクター原案)</t>
+          <t>クール教信者</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第4話</t>
+          <t>第154話</t>
         </is>
       </c>
     </row>
@@ -15658,17 +16700,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+          <t>板垣恵介 林たかあき</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第8話-2：ゼロ発見</t>
+          <t>第58話 帰還</t>
         </is>
       </c>
     </row>
@@ -15678,17 +16720,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>くらいあの子としたいこと</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>碇マナツ(著者)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第142話 よくわからないけれど後始末するみたいです（２）</t>
+          <t>特別編㉒</t>
         </is>
       </c>
     </row>
@@ -15698,17 +16740,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>ダンジョンの幼なじみ</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>久真やすひさ(著者)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第56話①　ペットを飼ってみた</t>
+          <t>【７巻発売＆1000万PV突破記念！】 ダンジョンの幼なじみ第２回人気投票</t>
         </is>
       </c>
     </row>
@@ -15718,17 +16760,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>「おかえり、パパ」</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>蝉丸</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>単行本5巻限定描きおろし「過去」試し読み</t>
+          <t>拷問158</t>
         </is>
       </c>
     </row>
@@ -15738,17 +16780,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+          <t>六志麻あさ 業務用餅 kisui</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第49話 先生と生徒②</t>
+          <t>第７５話</t>
         </is>
       </c>
     </row>
@@ -15758,17 +16800,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第83話(後編)その3</t>
+          <t>第20話④</t>
         </is>
       </c>
     </row>
@@ -15778,17 +16820,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>お気楽領主の楽しい領地防衛 ～生産系魔術で名もなき村を最強の城塞都市に～</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>青色まろ（漫画） 赤池宗（原作） 転（原作イラスト）</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第４３話　勇者、合体した六邪神将を撃破し、めでたしめでたし（１）</t>
+          <t>第35話　侵略者</t>
         </is>
       </c>
     </row>
@@ -15798,17 +16840,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>北斗の拳 世紀末ドラマ撮影伝</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>原案/武論尊・原哲夫 漫画/倉尾宏</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第76話 柏葉、最後の目覚め!!</t>
+          <t>第89話　その3</t>
         </is>
       </c>
     </row>
@@ -15818,17 +16860,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>KAKERU</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>拷問157</t>
+          <t>第70話「あうと！ せーふ！ よよいのよい！（もうどうにでもなぁれ♡）」（後半)</t>
         </is>
       </c>
     </row>
@@ -15838,17 +16880,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>おとなりのダウナーさんは無理させない</t>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>瑠璃いろ(著者)</t>
+          <t>空野進 sorani ファルまろ</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>コミックス告知</t>
+          <t>第14話　最弱貴族、悪役令嬢を脱がす（２）</t>
         </is>
       </c>
     </row>
@@ -15858,17 +16900,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>バーサス</t>
+          <t>最果てのパラディン</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+          <t>奥橋睦（漫画） 柳野かなた（原作） 輪くすさが（キャラクター原案）</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第29話 魔王VS.ロボット（前編-1）</t>
+          <t>第68話　無敵の巨人Ⅰ</t>
         </is>
       </c>
     </row>
@@ -15878,17 +16920,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>Lv２からチートだった元勇者候補のまったり異世界ライフ</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>糸町秋音（漫画） 鬼ノ城ミヤ（原作） 片桐（キャラクター原案）</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第89話　その2</t>
+          <t>第63話　居場所</t>
         </is>
       </c>
     </row>
@@ -15898,17 +16940,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>俺は星間国家の悪徳領主！</t>
+          <t>黄金の経験値</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第42話　人生終了</t>
+          <t>第20話（前編）</t>
         </is>
       </c>
     </row>
@@ -15918,17 +16960,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>三枝さんはメガネ先輩と恋を描く</t>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>セレビィ量産型(著者)</t>
+          <t>漫画/すたひろ 原作/Y.A</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第23話後半</t>
+          <t>chapter74【39話①】</t>
         </is>
       </c>
     </row>
@@ -15938,17 +16980,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第74話(後編) イダ乱入</t>
+          <t>第27話-2</t>
         </is>
       </c>
     </row>
@@ -15958,17 +17000,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ライブダンジョン！</t>
+          <t>塔の管理をしてみよう</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第91話前半</t>
+          <t>第95話前編</t>
         </is>
       </c>
     </row>
@@ -15978,17 +17020,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第59話　別れと、出立（後編）</t>
+          <t>第7話　ショッピングデート（後編）</t>
         </is>
       </c>
     </row>
@@ -15998,17 +17040,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>英雄女騎士に有能とバレた俺の美人ハーレム騎士団 ガイカク・ヒクメの奇術騎士団</t>
+          <t>男子高校生だけどギャルにTSしました</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>明石六郎(原作) 太盛(作画) 氷室しゅんすけ(キャラクター原案)</t>
+          <t>太陽まりい(著者)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第12話-2</t>
+          <t>第21話前編</t>
         </is>
       </c>
     </row>
@@ -16018,17 +17060,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>異世界でも無難に生きたい症候群</t>
+          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
+          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第32話③</t>
+          <t>EP.21②</t>
         </is>
       </c>
     </row>
@@ -16038,17 +17080,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>女子高生の無駄づかい</t>
+          <t>理想の彼女</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ビーノ(著者)</t>
+          <t>もりまりも(著者)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第138話　にんめい</t>
+          <t>第29話</t>
         </is>
       </c>
     </row>
@@ -16058,17 +17100,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+          <t>魔法少女リリカルなのは EXCEEDS</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>KAKERU</t>
+          <t>都築真紀 川上修一</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第70話「あうと！ せーふ！ よよいのよい！（もうどうにでもなぁれ♡）」（後半)</t>
+          <t>第７話①</t>
         </is>
       </c>
     </row>
@@ -16078,17 +17120,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+          <t>魔石グルメ　魔物の力を食べたオレは最強！</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>空野進 sorani ファルまろ</t>
+          <t>菅原健二(作画) 結城涼(原作) 成瀬ちさと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第14話　最弱貴族、悪役令嬢を脱がす（１）</t>
+          <t>第69話後半</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-12-01
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -30,6 +30,7 @@
     <sheet name="2025-11-10" sheetId="22" state="visible" r:id="rId22"/>
     <sheet name="2025-11-17" sheetId="23" state="visible" r:id="rId23"/>
     <sheet name="2025-11-24" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="2025-12-01" sheetId="25" state="visible" r:id="rId25"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -16135,22 +16136,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第73話 前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>コミックス第1巻 発売告知記事</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第42話</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第７１話『扇山停止』③</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第140話	蚊がせめてきたぞっ!!</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第６９話　爺ちゃんとの戦いが始まった（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第80話その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第132話　画伯の願い</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第16話</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第26話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第130話　変身してみる（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第５４話　勇者を護る器用貧乏（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第311話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第10話</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第84話　慈愛</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第２５食　赤スライムのシャーベット、パクパクですわ！（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第75話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第12話</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>アザミヤコを好きになる</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第11話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>美人女上司滝沢さん</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>やんBARU(著者)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第208話</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>貞操逆転世界で頼めばヤれると噂の俺</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>澄田佑貴(漫画) aaa168（スリーエー）(原作)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第56話②　ペットを飼ってみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第143話 よくわからないけれど人をダメにするみたいです（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>聖者無双</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第94話　戦乱のドワーフ王国・奴隷の扱い（後半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>モリタ Ｕ４ nima</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第14話（３）　春とおぼっちゃまとピクニックランチ（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第４３話　勇者、合体した六邪神将を撃破し、めでたしめでたし（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第4話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>小林さんちのメイドラゴン</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>クール教信者</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第154話</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 林たかあき</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第58話 帰還</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>特別編㉒</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンの幼なじみ</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>久真やすひさ(著者)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>【７巻発売＆1000万PV突破記念！】 ダンジョンの幼なじみ第２回人気投票</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>拷問158</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>六志麻あさ 業務用餅 kisui</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第７５話</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第20話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>お気楽領主の楽しい領地防衛 ～生産系魔術で名もなき村を最強の城塞都市に～</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>青色まろ（漫画） 赤池宗（原作） 転（原作イラスト）</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第35話　侵略者</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第89話　その3</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>KAKERU</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第70話「あうと！ せーふ！ よよいのよい！（もうどうにでもなぁれ♡）」（後半)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第14話　最弱貴族、悪役令嬢を脱がす（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>最果てのパラディン</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>奥橋睦（漫画） 柳野かなた（原作） 輪くすさが（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第68話　無敵の巨人Ⅰ</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>Lv２からチートだった元勇者候補のまったり異世界ライフ</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>糸町秋音（漫画） 鬼ノ城ミヤ（原作） 片桐（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第63話　居場所</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>黄金の経験値</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第20話（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>chapter74【39話①】</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第27話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>塔の管理をしてみよう</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第95話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第7話　ショッピングデート（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>男子高校生だけどギャルにTSしました</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>太陽まりい(著者)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第21話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>EP.21②</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>理想の彼女</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>もりまりも(著者)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第29話</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>魔法少女リリカルなのは EXCEEDS</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>都築真紀 川上修一</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第７話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>魔石グルメ　魔物の力を食べたオレは最強！</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>菅原健二(作画) 結城涼(原作) 成瀬ちさと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第69話後半</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+          <t>異世界おじさん</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+          <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第73話 前編</t>
+          <t>第73話</t>
         </is>
       </c>
     </row>
@@ -16160,17 +17202,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>コミックス第1巻 発売告知記事</t>
+          <t>216撃目</t>
         </is>
       </c>
     </row>
@@ -16180,17 +17222,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>蜘蛛ですが、なにか？</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第42話</t>
+          <t>第77話その1</t>
         </is>
       </c>
     </row>
@@ -16210,7 +17252,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第７１話『扇山停止』③</t>
+          <t>第７１話『扇山停止』④</t>
         </is>
       </c>
     </row>
@@ -16220,17 +17262,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>生徒会にも穴はある！</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>むちまろ</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第140話	蚊がせめてきたぞっ!!</t>
+          <t>第６９話　爺ちゃんとの戦いが始まった（２）</t>
         </is>
       </c>
     </row>
@@ -16240,17 +17282,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第６９話　爺ちゃんとの戦いが始まった（１）</t>
+          <t>第33話</t>
         </is>
       </c>
     </row>
@@ -16260,17 +17302,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第80話その2</t>
+          <t>第37話①</t>
         </is>
       </c>
     </row>
@@ -16280,17 +17322,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>異世界居酒屋「のぶ」</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第132話　画伯の願い</t>
+          <t>第127話</t>
         </is>
       </c>
     </row>
@@ -16300,17 +17342,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+          <t>久遠まこと(著者) 石のやっさん(原作)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第16話</t>
+          <t>第32話</t>
         </is>
       </c>
     </row>
@@ -16320,17 +17362,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>女友達は頼めば意外とヤらせてくれる</t>
+          <t>帰ってください！ 阿久津さん</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ろくろ(漫画) 鏡遊(原作)</t>
+          <t>長岡太一(著者)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第26話②</t>
+          <t>第199話</t>
         </is>
       </c>
     </row>
@@ -16340,17 +17382,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>異世界魔王と召喚少女の奴隷魔術</t>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第130話　変身してみる（後編）</t>
+          <t>第13話-2</t>
         </is>
       </c>
     </row>
@@ -16360,17 +17402,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>須河篤志(著者)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第５４話　勇者を護る器用貧乏（４）</t>
+          <t>第17話後半</t>
         </is>
       </c>
     </row>
@@ -16380,17 +17422,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>異世界のんびり農家</t>
+          <t>ダークサモナーとデキている</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+          <t>車王(著者)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第311話</t>
+          <t>第81話</t>
         </is>
       </c>
     </row>
@@ -16400,17 +17442,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第10話</t>
+          <t>おまけ67</t>
         </is>
       </c>
     </row>
@@ -16420,17 +17462,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+          <t>異世界のんびり農家</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>板垣恵介 猪原賽 陸井栄史</t>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第84話　慈愛</t>
+          <t>第312話</t>
         </is>
       </c>
     </row>
@@ -16440,17 +17482,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>島知宏 音速炒飯 有都あらゆる</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第２５食　赤スライムのシャーベット、パクパクですわ！（３）</t>
+          <t>第50話後編</t>
         </is>
       </c>
     </row>
@@ -16460,17 +17502,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>淫獄団地</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第75話③</t>
+          <t>第52話（後編）</t>
         </is>
       </c>
     </row>
@@ -16480,17 +17522,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>「おかえり、パパ」</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>蝉丸</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第12話</t>
+          <t>第30話　再会</t>
         </is>
       </c>
     </row>
@@ -16500,17 +17542,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>アザミヤコを好きになる</t>
+          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+          <t>三部べべ(漫画) ねうしとら(原作)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第11話後編</t>
+          <t>第4話-2</t>
         </is>
       </c>
     </row>
@@ -16520,17 +17562,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>美人女上司滝沢さん</t>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>やんBARU(著者)</t>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第208話</t>
+          <t>第２５食　赤スライムのシャーベット、パクパクですわ！（３）</t>
         </is>
       </c>
     </row>
@@ -16540,17 +17582,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>貞操逆転世界で頼めばヤれると噂の俺</t>
+          <t>姫ヶ崎櫻子は今日も不憫可愛い</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>澄田佑貴(漫画) aaa168（スリーエー）(原作)</t>
+          <t>安田剛助(著者)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第52話</t>
         </is>
       </c>
     </row>
@@ -16560,17 +17602,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第56話②　ペットを飼ってみた</t>
+          <t>第43話　奴は祝う（中編）</t>
         </is>
       </c>
     </row>
@@ -16580,17 +17622,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>物語の黒幕に転生して</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第143話 よくわからないけれど人をダメにするみたいです（１）</t>
+          <t>第36話</t>
         </is>
       </c>
     </row>
@@ -16600,17 +17642,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>聖者無双</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第94話　戦乱のドワーフ王国・奴隷の扱い（後半）</t>
+          <t>第143話 よくわからないけれど人をダメにするみたいです（２）</t>
         </is>
       </c>
     </row>
@@ -16620,17 +17662,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>モリタ Ｕ４ nima</t>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第14話（３）　春とおぼっちゃまとピクニックランチ（３）</t>
+          <t>第26話</t>
         </is>
       </c>
     </row>
@@ -16640,17 +17682,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第４３話　勇者、合体した六邪神将を撃破し、めでたしめでたし（２）</t>
+          <t>第1話：命の使い道</t>
         </is>
       </c>
     </row>
@@ -16660,17 +17702,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第4話後編</t>
+          <t>第49話 先生と生徒③</t>
         </is>
       </c>
     </row>
@@ -16680,17 +17722,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>小林さんちのメイドラゴン</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>クール教信者</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第154話</t>
+          <t>第４３話　勇者、合体した六邪神将を撃破し、めでたしめでたし（３）</t>
         </is>
       </c>
     </row>
@@ -16700,17 +17742,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>板垣恵介 林たかあき</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第58話 帰還</t>
+          <t>第84話その1</t>
         </is>
       </c>
     </row>
@@ -16720,17 +17762,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>くらいあの子としたいこと</t>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>碇マナツ(著者)</t>
+          <t>セレビィ量産型(著者)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>特別編㉒</t>
+          <t>第23.5話</t>
         </is>
       </c>
     </row>
@@ -16740,17 +17782,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ダンジョンの幼なじみ</t>
+          <t>幼女戦記</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>久真やすひさ(著者)</t>
+          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>【７巻発売＆1000万PV突破記念！】 ダンジョンの幼なじみ第２回人気投票</t>
+          <t>第百十章：ドードーバード航空戦Ⅴ</t>
         </is>
       </c>
     </row>
@@ -16770,7 +17812,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>拷問158</t>
+          <t>拷問159</t>
         </is>
       </c>
     </row>
@@ -16780,17 +17822,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+          <t>北斗の拳 世紀末ドラマ撮影伝</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>六志麻あさ 業務用餅 kisui</t>
+          <t>原案/武論尊・原哲夫 漫画/倉尾宏</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第７５話</t>
+          <t>第77話 柏葉サウザー、最後の演技!!</t>
         </is>
       </c>
     </row>
@@ -16800,17 +17842,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第20話④</t>
+          <t>第75話(前編) ヴァルハラからの贈り物</t>
         </is>
       </c>
     </row>
@@ -16820,17 +17862,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>お気楽領主の楽しい領地防衛 ～生産系魔術で名もなき村を最強の城塞都市に～</t>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>青色まろ（漫画） 赤池宗（原作） 転（原作イラスト）</t>
+          <t>FUNA 東西 モトエ恵介</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第35話　侵略者</t>
+          <t>第124話　襲撃［その3］</t>
         </is>
       </c>
     </row>
@@ -16840,17 +17882,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>バーサス</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第89話　その3</t>
+          <t>第29話 魔王VS.ロボット（前編-2）</t>
         </is>
       </c>
     </row>
@@ -16860,17 +17902,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+          <t>回復術士のやり直し</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>KAKERU</t>
+          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第70話「あうと！ せーふ！ よよいのよい！（もうどうにでもなぁれ♡）」（後半)</t>
+          <t>第74話-2</t>
         </is>
       </c>
     </row>
@@ -16890,7 +17932,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第14話　最弱貴族、悪役令嬢を脱がす（２）</t>
+          <t>第14話　最弱貴族、悪役令嬢を脱がす（３）</t>
         </is>
       </c>
     </row>
@@ -16900,17 +17942,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>最果てのパラディン</t>
+          <t>ライブダンジョン！</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>奥橋睦（漫画） 柳野かなた（原作） 輪くすさが（キャラクター原案）</t>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第68話　無敵の巨人Ⅰ</t>
+          <t>第91話後半</t>
         </is>
       </c>
     </row>
@@ -16920,17 +17962,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Lv２からチートだった元勇者候補のまったり異世界ライフ</t>
+          <t>地味子な三葉さんが僕を誘惑する</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>糸町秋音（漫画） 鬼ノ城ミヤ（原作） 片桐（キャラクター原案）</t>
+          <t>はぶらえる(著者)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第63話　居場所</t>
+          <t>第12話後半</t>
         </is>
       </c>
     </row>
@@ -16940,17 +17982,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>黄金の経験値</t>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第20話（前編）</t>
+          <t>第34話</t>
         </is>
       </c>
     </row>
@@ -16960,17 +18002,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+          <t>乙女ゲー世界はモブに厳しい世界です【共和国編】</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>漫画/すたひろ 原作/Y.A</t>
+          <t>三嶋与夢(原作) 行々狸(作画) 孟達(キャラクター原案) マツリセイシロウ(構成) FTops(制作)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>chapter74【39話①】</t>
+          <t>第4話-2</t>
         </is>
       </c>
     </row>
@@ -16980,17 +18022,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
+          <t>めっちゃ召喚された件 THE COMIC</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
+          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第27話-2</t>
+          <t>第50話②</t>
         </is>
       </c>
     </row>
@@ -17000,17 +18042,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>塔の管理をしてみよう</t>
+          <t>天獄で悪魔がボクを魅惑する</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+          <t>銀河味めてお(著者)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第95話前編</t>
+          <t>第38話</t>
         </is>
       </c>
     </row>
@@ -17020,17 +18062,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第7話　ショッピングデート（後編）</t>
+          <t>コミックス告知</t>
         </is>
       </c>
     </row>
@@ -17040,17 +18082,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>男子高校生だけどギャルにTSしました</t>
+          <t>異世界でも無難に生きたい症候群</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>太陽まりい(著者)</t>
+          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第21話前編</t>
+          <t>第32話④</t>
         </is>
       </c>
     </row>
@@ -17060,17 +18102,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
+          <t>転生したらスライムだった件 異聞 ～魔国暮らしのトリニティ～</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
+          <t>伏瀬 戸野タエ みっつばー</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>EP.21②</t>
+          <t>第115話　開国祭二日目［その6］</t>
         </is>
       </c>
     </row>
@@ -17080,17 +18122,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>理想の彼女</t>
+          <t>ダンジョン・シェルパ　迷宮道先案内人</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>もりまりも(著者)</t>
+          <t>原作/加茂セイ 漫画/刀坂アキラ</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第29話</t>
+          <t>最終潜行</t>
         </is>
       </c>
     </row>
@@ -17100,17 +18142,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>魔法少女リリカルなのは EXCEEDS</t>
+          <t>自分を押し売りしてきた奴隷ちゃんがドラゴンをワンパンしてた　戯画版</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>都築真紀 川上修一</t>
+          <t>原作：溝上良 漫画：人生負組 キャラクター原案：ごろー✳︎</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第７話①</t>
+          <t>第2話「俺は静かに暮らしたい」</t>
         </is>
       </c>
     </row>
@@ -17120,17 +18162,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>魔石グルメ　魔物の力を食べたオレは最強！</t>
+          <t>異世界ではじめる二拠点生活 ～空間魔法で王都と田舎をいったりきたり～</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>菅原健二(作画) 結城涼(原作) 成瀬ちさと(キャラクター原案)</t>
+          <t>丸山りん(漫画) 錬金王(原作) あんべよしろう(キャラクター原案)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第69話後半</t>
+          <t>第34話</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-12-08
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -31,6 +31,7 @@
     <sheet name="2025-11-17" sheetId="23" state="visible" r:id="rId23"/>
     <sheet name="2025-11-24" sheetId="24" state="visible" r:id="rId24"/>
     <sheet name="2025-12-01" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="2025-12-08" sheetId="26" state="visible" r:id="rId26"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -17177,22 +17178,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第73話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>ワンパンマン</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>216撃目</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>蜘蛛ですが、なにか？</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第77話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第７１話『扇山停止』④</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第６９話　爺ちゃんとの戦いが始まった（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第33話</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第37話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>異世界居酒屋「のぶ」</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第127話</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>久遠まこと(著者) 石のやっさん(原作)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第32話</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>帰ってください！ 阿久津さん</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>長岡太一(著者)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第199話</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第13話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>クセ強彼女は床にいざなう</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>須河篤志(著者)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第17話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>ダークサモナーとデキている</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>車王(著者)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第81話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>おまけ67</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第312話</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>まんきつしたい常連さん</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>しんみりん(著者)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第50話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第52話（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>「おかえり、パパ」</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>蝉丸</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第30話　再会</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>三部べべ(漫画) ねうしとら(原作)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第4話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第２５食　赤スライムのシャーベット、パクパクですわ！（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>姫ヶ崎櫻子は今日も不憫可愛い</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>安田剛助(著者)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第52話</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第43話　奴は祝う（中編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>物語の黒幕に転生して</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第36話</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第143話 よくわからないけれど人をダメにするみたいです（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第26話</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第1話：命の使い道</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第49話 先生と生徒③</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第４３話　勇者、合体した六邪神将を撃破し、めでたしめでたし（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第84話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>セレビィ量産型(著者)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第23.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>幼女戦記</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第百十章：ドードーバード航空戦Ⅴ</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>拷問159</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>北斗の拳 世紀末ドラマ撮影伝</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>原案/武論尊・原哲夫 漫画/倉尾宏</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第77話 柏葉サウザー、最後の演技!!</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第75話(前編) ヴァルハラからの贈り物</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>FUNA 東西 モトエ恵介</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第124話　襲撃［その3］</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>バーサス</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第29話 魔王VS.ロボット（前編-2）</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>回復術士のやり直し</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第74話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第14話　最弱貴族、悪役令嬢を脱がす（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>ライブダンジョン！</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第91話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>地味子な三葉さんが僕を誘惑する</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>はぶらえる(著者)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第12話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第34話</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>乙女ゲー世界はモブに厳しい世界です【共和国編】</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>三嶋与夢(原作) 行々狸(作画) 孟達(キャラクター原案) マツリセイシロウ(構成) FTops(制作)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第4話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>めっちゃ召喚された件 THE COMIC</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第50話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>天獄で悪魔がボクを魅惑する</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>銀河味めてお(著者)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第38話</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>コミックス告知</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>異世界でも無難に生きたい症候群</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第32話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>転生したらスライムだった件 異聞 ～魔国暮らしのトリニティ～</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>伏瀬 戸野タエ みっつばー</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第115話　開国祭二日目［その6］</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョン・シェルパ　迷宮道先案内人</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>原作/加茂セイ 漫画/刀坂アキラ</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>最終潜行</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>自分を押し売りしてきた奴隷ちゃんがドラゴンをワンパンしてた　戯画版</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>原作：溝上良 漫画：人生負組 キャラクター原案：ごろー✳︎</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第2話「俺は静かに暮らしたい」</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>異世界ではじめる二拠点生活 ～空間魔法で王都と田舎をいったりきたり～</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>丸山りん(漫画) 錬金王(原作) あんべよしろう(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第34話</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第73話</t>
+          <t>第73話 後編</t>
         </is>
       </c>
     </row>
@@ -17202,17 +18244,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ワンパンマン</t>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>原作/ＯＮＥ 作画/村田雄介</t>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>216撃目</t>
+          <t>第34話：プロのテク①</t>
         </is>
       </c>
     </row>
@@ -17222,17 +18264,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>蜘蛛ですが、なにか？</t>
+          <t>生徒会にも穴はある！</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+          <t>むちまろ</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第77話その1</t>
+          <t>第141話	虎丸がんばる！</t>
         </is>
       </c>
     </row>
@@ -17242,17 +18284,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>とんでもスキルで異世界放浪メシ</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>赤岸K（漫画） 江口連（原作） 雅（キャラクター原案）</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第７１話『扇山停止』④</t>
+          <t>第57話　「誘惑だらけの朝市」</t>
         </is>
       </c>
     </row>
@@ -17262,17 +18304,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第６９話　爺ちゃんとの戦いが始まった（２）</t>
+          <t>第７２話『先端停止』①</t>
         </is>
       </c>
     </row>
@@ -17282,17 +18324,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第33話</t>
+          <t>第７０話　鈍感な戦いが始まった</t>
         </is>
       </c>
     </row>
@@ -17302,17 +18344,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+          <t>王子様の友達</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+          <t>すけろく(著者)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第37話①</t>
+          <t>第32話</t>
         </is>
       </c>
     </row>
@@ -17322,17 +18364,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>異世界居酒屋「のぶ」</t>
+          <t>帰ってください！ 阿久津さん</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
+          <t>長岡太一(著者)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第127話</t>
+          <t>第199話</t>
         </is>
       </c>
     </row>
@@ -17342,17 +18384,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>久遠まこと(著者) 石のやっさん(原作)</t>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第32話</t>
+          <t>第81話その1</t>
         </is>
       </c>
     </row>
@@ -17362,17 +18404,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>帰ってください！ 阿久津さん</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>長岡太一(著者)</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第199話</t>
+          <t>第133話　秘密</t>
         </is>
       </c>
     </row>
@@ -17382,17 +18424,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+          <t>黒幕一家に転生したけど原作無視して独立する</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第13話-2</t>
+          <t>第５話　ゲス子爵を成敗して独立する（３）</t>
         </is>
       </c>
     </row>
@@ -17402,17 +18444,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>クセ強彼女は床にいざなう</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>須河篤志(著者)</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第17話後半</t>
+          <t>休載イラスト</t>
         </is>
       </c>
     </row>
@@ -17422,17 +18464,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ダークサモナーとデキている</t>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>車王(著者)</t>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第81話</t>
+          <t>第17話前半</t>
         </is>
       </c>
     </row>
@@ -17442,17 +18484,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>貞操逆転世界で頼めばヤれると噂の俺</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>澄田佑貴(漫画) aaa168（スリーエー）(原作)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>おまけ67</t>
+          <t>第2話</t>
         </is>
       </c>
     </row>
@@ -17462,17 +18504,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>異世界のんびり農家</t>
+          <t>田舎で恋は難しい!?</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+          <t>ねこうめ(著者)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第312話</t>
+          <t>第2話</t>
         </is>
       </c>
     </row>
@@ -17482,17 +18524,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>まんきつしたい常連さん</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>しんみりん(著者)</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第50話後編</t>
+          <t>第131話　幕間（前編）</t>
         </is>
       </c>
     </row>
@@ -17502,17 +18544,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>淫獄団地</t>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第52話（後編）</t>
+          <t>第27話①</t>
         </is>
       </c>
     </row>
@@ -17522,17 +18564,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>「おかえり、パパ」</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>蝉丸</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第30話　再会</t>
+          <t>第５５話　封印を解く器用貧乏（２）</t>
         </is>
       </c>
     </row>
@@ -17542,17 +18584,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
+          <t>このヒーラー、めんどくさい</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>三部べべ(漫画) ねうしとら(原作)</t>
+          <t>丹念に発酵(著者)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第4話-2</t>
+          <t>第92話：特訓</t>
         </is>
       </c>
     </row>
@@ -17562,17 +18604,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+          <t>Ｓ級ギルドを追放されたけど、実は俺だけドラゴンの言葉がわかるので、気付いたときには竜騎士の頂点を極めてました。</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>島知宏 音速炒飯 有都あらゆる</t>
+          <t>ひそな(漫画) 三木なずな(原作) 白狼(キャラクター原案)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第２５食　赤スライムのシャーベット、パクパクですわ！（３）</t>
+          <t>第41話-2</t>
         </is>
       </c>
     </row>
@@ -17582,17 +18624,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>姫ヶ崎櫻子は今日も不憫可愛い</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>安田剛助(著者)</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第52話</t>
+          <t>第75話④</t>
         </is>
       </c>
     </row>
@@ -17602,17 +18644,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第43話　奴は祝う（中編）</t>
+          <t>第85話　不入虎穴(虎穴に入らずんば虎子を得ず)</t>
         </is>
       </c>
     </row>
@@ -17622,17 +18664,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>物語の黒幕に転生して</t>
+          <t>貞操逆転世界の童貞辺境領主騎士</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+          <t>柳瀬こたつ（漫画） 道造（原作） めろん２２（キャラクター原案）</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第36話</t>
+          <t>第11話　やむなき犠牲（前編）</t>
         </is>
       </c>
     </row>
@@ -17642,17 +18684,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>異世界食堂　洋食のねこや</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第143話 よくわからないけれど人をダメにするみたいです（２）</t>
+          <t>第42話➁</t>
         </is>
       </c>
     </row>
@@ -17662,17 +18704,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第26話</t>
+          <t>第57話①　スローライフをしてみた</t>
         </is>
       </c>
     </row>
@@ -17682,17 +18724,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
+          <t>濁る瞳で何を願う ハイセルク戦記</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
+          <t>トルトネン 創-taro 斎藤八呑</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第1話：命の使い道</t>
+          <t>第35話 黒の奔流</t>
         </is>
       </c>
     </row>
@@ -17702,17 +18744,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+          <t>聖者無双</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第49話 先生と生徒③</t>
+          <t>第95話　奴隷の扱い・戦闘準備（前半）</t>
         </is>
       </c>
     </row>
@@ -17722,17 +18764,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>小林さんちのメイドラゴン</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>クール教信者</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第４３話　勇者、合体した六邪神将を撃破し、めでたしめでたし（３）</t>
+          <t>第155話</t>
         </is>
       </c>
     </row>
@@ -17742,17 +18784,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第84話その1</t>
+          <t>第144話 よくわからないけれど港町に着いたみたいです（１）</t>
         </is>
       </c>
     </row>
@@ -17762,17 +18804,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>三枝さんはメガネ先輩と恋を描く</t>
+          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>セレビィ量産型(著者)</t>
+          <t>モリタ Ｕ４ nima</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第23.5話</t>
+          <t>第14話（４）　春とおぼっちゃまとピクニックランチ（４）</t>
         </is>
       </c>
     </row>
@@ -17782,17 +18824,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>幼女戦記</t>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第百十章：ドードーバード航空戦Ⅴ</t>
+          <t>第9話-1：黄昏の茶会</t>
         </is>
       </c>
     </row>
@@ -17802,17 +18844,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>拷問159</t>
+          <t>第13話</t>
         </is>
       </c>
     </row>
@@ -17822,17 +18864,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>北斗の拳 世紀末ドラマ撮影伝</t>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>原案/武論尊・原哲夫 漫画/倉尾宏</t>
+          <t>三吉汐美(著者)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第77話 柏葉サウザー、最後の演技!!</t>
+          <t>第19話前半</t>
         </is>
       </c>
     </row>
@@ -17842,17 +18884,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第75話(前編) ヴァルハラからの贈り物</t>
+          <t>第84話その2</t>
         </is>
       </c>
     </row>
@@ -17862,17 +18904,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>FUNA 東西 モトエ恵介</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第124話　襲撃［その3］</t>
+          <t>第４３話　勇者、合体した六邪神将を撃破し、めでたしめでたし（４）</t>
         </is>
       </c>
     </row>
@@ -17882,17 +18924,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>バーサス</t>
+          <t>衛宮さんちの今日のごはん</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+          <t>TAa(漫画) 只野まこと(料理監修) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第29話 魔王VS.ロボット（前編-2）</t>
+          <t>第77話</t>
         </is>
       </c>
     </row>
@@ -17902,17 +18944,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>回復術士のやり直し</t>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
+          <t>六志麻あさ 業務用餅 kisui</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第74話-2</t>
+          <t>第７６話</t>
         </is>
       </c>
     </row>
@@ -17922,17 +18964,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+          <t>くらいあの子としたいこと</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>空野進 sorani ファルまろ</t>
+          <t>碇マナツ(著者)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第14話　最弱貴族、悪役令嬢を脱がす（３）</t>
+          <t>第87話</t>
         </is>
       </c>
     </row>
@@ -17942,17 +18984,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ライブダンジョン！</t>
+          <t>まったく最近の探偵ときたら</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+          <t>五十嵐正邦(著者)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第91話後半</t>
+          <t>第117話</t>
         </is>
       </c>
     </row>
@@ -17962,17 +19004,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>地味子な三葉さんが僕を誘惑する</t>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>はぶらえる(著者)</t>
+          <t>板垣恵介 林たかあき</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第12話後半</t>
+          <t>第59話 流水の獲物</t>
         </is>
       </c>
     </row>
@@ -17982,17 +19024,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第34話</t>
+          <t>第90話　その1</t>
         </is>
       </c>
     </row>
@@ -18002,17 +19044,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>乙女ゲー世界はモブに厳しい世界です【共和国編】</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>三嶋与夢(原作) 行々狸(作画) 孟達(キャラクター原案) マツリセイシロウ(構成) FTops(制作)</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第4話-2</t>
+          <t>拷問160</t>
         </is>
       </c>
     </row>
@@ -18022,17 +19064,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>めっちゃ召喚された件 THE COMIC</t>
+          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
+          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第50話②</t>
+          <t>第41話-2</t>
         </is>
       </c>
     </row>
@@ -18042,17 +19084,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>天獄で悪魔がボクを魅惑する</t>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>銀河味めてお(著者)</t>
+          <t>KAKERU</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第38話</t>
+          <t>第71話「ファントム・アレイ」（前半）</t>
         </is>
       </c>
     </row>
@@ -18062,17 +19104,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>コミックス告知</t>
+          <t>第21話①</t>
         </is>
       </c>
     </row>
@@ -18082,17 +19124,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>異世界でも無難に生きたい症候群</t>
+          <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
+          <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第32話④</t>
+          <t>第7話①「伝えたいこと」</t>
         </is>
       </c>
     </row>
@@ -18102,17 +19144,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>転生したらスライムだった件 異聞 ～魔国暮らしのトリニティ～</t>
+          <t>陰キャの俺が席替えでS級美少女に囲まれたら秘密の関係が始まった。</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>伏瀬 戸野タエ みっつばー</t>
+          <t>星野 星野(原作) バラマツヒトミ(漫画) 黒兎 ゆう(キャラクター原案)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第115話　開国祭二日目［その6］</t>
+          <t>第8話</t>
         </is>
       </c>
     </row>
@@ -18122,17 +19164,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ダンジョン・シェルパ　迷宮道先案内人</t>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>原作/加茂セイ 漫画/刀坂アキラ</t>
+          <t>漫画/すたひろ 原作/Y.A</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>最終潜行</t>
+          <t>chapter75【39話②】</t>
         </is>
       </c>
     </row>
@@ -18142,17 +19184,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>自分を押し売りしてきた奴隷ちゃんがドラゴンをワンパンしてた　戯画版</t>
+          <t>黄金の経験値</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>原作：溝上良 漫画：人生負組 キャラクター原案：ごろー✳︎</t>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第2話「俺は静かに暮らしたい」</t>
+          <t>第20話（後編）</t>
         </is>
       </c>
     </row>
@@ -18162,17 +19204,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>異世界ではじめる二拠点生活 ～空間魔法で王都と田舎をいったりきたり～</t>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>丸山りん(漫画) 錬金王(原作) あんべよしろう(キャラクター原案)</t>
+          <t>空野進 sorani ファルまろ</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第34話</t>
+          <t>第14話　最弱貴族、悪役令嬢を脱がす（４）</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-12-15
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -32,6 +32,7 @@
     <sheet name="2025-11-24" sheetId="24" state="visible" r:id="rId24"/>
     <sheet name="2025-12-01" sheetId="25" state="visible" r:id="rId25"/>
     <sheet name="2025-12-08" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="2025-12-15" sheetId="27" state="visible" r:id="rId27"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -18219,22 +18220,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第73話 後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第34話：プロのテク①</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第141話	虎丸がんばる！</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>とんでもスキルで異世界放浪メシ</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>赤岸K（漫画） 江口連（原作） 雅（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第57話　「誘惑だらけの朝市」</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第７２話『先端停止』①</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第７０話　鈍感な戦いが始まった</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>王子様の友達</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>すけろく(著者)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第32話</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>帰ってください！ 阿久津さん</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>長岡太一(著者)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第199話</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第81話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第133話　秘密</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>黒幕一家に転生したけど原作無視して独立する</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第５話　ゲス子爵を成敗して独立する（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第17話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>貞操逆転世界で頼めばヤれると噂の俺</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>澄田佑貴(漫画) aaa168（スリーエー）(原作)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第2話</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>田舎で恋は難しい!?</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>ねこうめ(著者)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第2話</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第131話　幕間（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第27話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第５５話　封印を解く器用貧乏（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>このヒーラー、めんどくさい</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>丹念に発酵(著者)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第92話：特訓</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>Ｓ級ギルドを追放されたけど、実は俺だけドラゴンの言葉がわかるので、気付いたときには竜騎士の頂点を極めてました。</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>ひそな(漫画) 三木なずな(原作) 白狼(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第41話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第75話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第85話　不入虎穴(虎穴に入らずんば虎子を得ず)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>貞操逆転世界の童貞辺境領主騎士</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>柳瀬こたつ（漫画） 道造（原作） めろん２２（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第11話　やむなき犠牲（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>異世界食堂　洋食のねこや</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第42話➁</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第57話①　スローライフをしてみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>濁る瞳で何を願う ハイセルク戦記</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>トルトネン 創-taro 斎藤八呑</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第35話 黒の奔流</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>聖者無双</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第95話　奴隷の扱い・戦闘準備（前半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>小林さんちのメイドラゴン</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>クール教信者</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第155話</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第144話 よくわからないけれど港町に着いたみたいです（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>モリタ Ｕ４ nima</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第14話（４）　春とおぼっちゃまとピクニックランチ（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第9話-1：黄昏の茶会</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第13話</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>三吉汐美(著者)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第19話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第84話その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第４３話　勇者、合体した六邪神将を撃破し、めでたしめでたし（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>衛宮さんちの今日のごはん</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>TAa(漫画) 只野まこと(料理監修) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第77話</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>六志麻あさ 業務用餅 kisui</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第７６話</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第87話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>まったく最近の探偵ときたら</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>五十嵐正邦(著者)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第117話</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 林たかあき</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第59話 流水の獲物</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第90話　その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>拷問160</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第41話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>KAKERU</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第71話「ファントム・アレイ」（前半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第21話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第7話①「伝えたいこと」</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>陰キャの俺が席替えでS級美少女に囲まれたら秘密の関係が始まった。</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>星野 星野(原作) バラマツヒトミ(漫画) 黒兎 ゆう(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第8話</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>chapter75【39話②】</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>黄金の経験値</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第20話（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第14話　最弱貴族、悪役令嬢を脱がす（４）</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第73話 後編</t>
+          <t>217撃目</t>
         </is>
       </c>
     </row>
@@ -18244,17 +19286,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+          <t>不徳のギルド</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>zunta(作画) はらわたさいぞう(原作)</t>
+          <t>河添太一</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第34話：プロのテク①</t>
+          <t>第１０１話：新たな一歩</t>
         </is>
       </c>
     </row>
@@ -18264,17 +19306,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>生徒会にも穴はある！</t>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>むちまろ</t>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第141話	虎丸がんばる！</t>
+          <t>第34話：プロのテク②</t>
         </is>
       </c>
     </row>
@@ -18284,17 +19326,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>とんでもスキルで異世界放浪メシ</t>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>赤岸K（漫画） 江口連（原作） 雅（キャラクター原案）</t>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第57話　「誘惑だらけの朝市」</t>
+          <t>第19話-2「今日も特別な日」</t>
         </is>
       </c>
     </row>
@@ -18314,7 +19356,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第７２話『先端停止』①</t>
+          <t>第７２話『先端停止』②</t>
         </is>
       </c>
     </row>
@@ -18324,17 +19366,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第７０話　鈍感な戦いが始まった</t>
+          <t>第37話②</t>
         </is>
       </c>
     </row>
@@ -18344,17 +19386,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>王子様の友達</t>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>すけろく(著者)</t>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第32話</t>
+          <t>第14話-1</t>
         </is>
       </c>
     </row>
@@ -18364,17 +19406,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>帰ってください！ 阿久津さん</t>
+          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>長岡太一(著者)</t>
+          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第199話</t>
+          <t>第34話前半</t>
         </is>
       </c>
     </row>
@@ -18384,17 +19426,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第81話その1</t>
+          <t>第134話　サポーターを決めなくちゃ！</t>
         </is>
       </c>
     </row>
@@ -18404,17 +19446,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>黒幕一家に転生したけど原作無視して独立する</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第133話　秘密</t>
+          <t>第５話　ゲス子爵を成敗して独立する（４）</t>
         </is>
       </c>
     </row>
@@ -18424,17 +19466,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>黒幕一家に転生したけど原作無視して独立する</t>
+          <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
+          <t>須河篤志(著者)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第５話　ゲス子爵を成敗して独立する（３）</t>
+          <t>休載漫画</t>
         </is>
       </c>
     </row>
@@ -18444,17 +19486,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>ダークサモナーとデキている</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>車王(著者)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>休載イラスト</t>
+          <t>第82話</t>
         </is>
       </c>
     </row>
@@ -18464,17 +19506,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第17話前半</t>
+          <t>第51話</t>
         </is>
       </c>
     </row>
@@ -18484,17 +19526,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>貞操逆転世界で頼めばヤれると噂の俺</t>
+          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>澄田佑貴(漫画) aaa168（スリーエー）(原作)</t>
+          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第2話</t>
+          <t>第12話-2</t>
         </is>
       </c>
     </row>
@@ -18504,17 +19546,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>田舎で恋は難しい!?</t>
+          <t>魔のものたちは企てる</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ねこうめ(著者)</t>
+          <t>加藤拓弐(原作) ガしガし(作画)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第2話</t>
+          <t>第32話</t>
         </is>
       </c>
     </row>
@@ -18534,7 +19576,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第131話　幕間（前編）</t>
+          <t>第131話　幕間（中編）</t>
         </is>
       </c>
     </row>
@@ -18544,17 +19586,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>女友達は頼めば意外とヤらせてくれる</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ろくろ(漫画) 鏡遊(原作)</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第27話①</t>
+          <t>第５５話　封印を解く器用貧乏（３）</t>
         </is>
       </c>
     </row>
@@ -18564,17 +19606,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>淫獄団地</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第５５話　封印を解く器用貧乏（２）</t>
+          <t>第53話</t>
         </is>
       </c>
     </row>
@@ -18584,17 +19626,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>このヒーラー、めんどくさい</t>
+          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>丹念に発酵(著者)</t>
+          <t>夜州 nini 藻</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第92話：特訓</t>
+          <t>第71話(後編)</t>
         </is>
       </c>
     </row>
@@ -18604,17 +19646,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Ｓ級ギルドを追放されたけど、実は俺だけドラゴンの言葉がわかるので、気付いたときには竜騎士の頂点を極めてました。</t>
+          <t>ダンジョンの幼なじみ</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ひそな(漫画) 三木なずな(原作) 白狼(キャラクター原案)</t>
+          <t>久真やすひさ(著者)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第41話-2</t>
+          <t>お休みイラスト</t>
         </is>
       </c>
     </row>
@@ -18624,17 +19666,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>三部べべ(漫画) ねうしとら(原作)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第75話④</t>
+          <t>第5話-1</t>
         </is>
       </c>
     </row>
@@ -18644,17 +19686,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+          <t>望まぬ不死の冒険者</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>板垣恵介 猪原賽 陸井栄史</t>
+          <t>中曽根ハイジ（漫画） 丘野 優（原作） じゃいあん（キャラクター原案）</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第85話　不入虎穴(虎穴に入らずんば虎子を得ず)</t>
+          <t>第62話　助太刀</t>
         </is>
       </c>
     </row>
@@ -18664,17 +19706,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>貞操逆転世界の童貞辺境領主騎士</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>柳瀬こたつ（漫画） 道造（原作） めろん２２（キャラクター原案）</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第11話　やむなき犠牲（前編）</t>
+          <t>第76話①</t>
         </is>
       </c>
     </row>
@@ -18684,17 +19726,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>異世界食堂　洋食のねこや</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第42話➁</t>
+          <t>第57話②　スローライフをしてみた</t>
         </is>
       </c>
     </row>
@@ -18704,17 +19746,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第57話①　スローライフをしてみた</t>
+          <t>第144話 よくわからないけれど港町に着いたみたいです（２）</t>
         </is>
       </c>
     </row>
@@ -18724,17 +19766,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>濁る瞳で何を願う ハイセルク戦記</t>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>トルトネン 創-taro 斎藤八呑</t>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第35話 黒の奔流</t>
+          <t>第43話　奴は祝う（後編）</t>
         </is>
       </c>
     </row>
@@ -18744,17 +19786,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>聖者無双</t>
+          <t>美人女上司滝沢さん</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+          <t>やんBARU(著者)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第95話　奴隷の扱い・戦闘準備（前半）</t>
+          <t>第209話</t>
         </is>
       </c>
     </row>
@@ -18764,17 +19806,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>小林さんちのメイドラゴン</t>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>クール教信者</t>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第155話</t>
+          <t>第49話 先生と生徒④</t>
         </is>
       </c>
     </row>
@@ -18784,17 +19826,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>金属スライムを倒しまくった俺が【黒鋼の王】と呼ばれるまで</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>藤屋いずこ(著者) 温泉カピバラ(原作) 山椒魚(キャラクター原案)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第144話 よくわからないけれど港町に着いたみたいです（１）</t>
+          <t>コミックス3巻発売漫画</t>
         </is>
       </c>
     </row>
@@ -18804,17 +19846,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>モリタ Ｕ４ nima</t>
+          <t>はぐはぐ(著者)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第14話（４）　春とおぼっちゃまとピクニックランチ（４）</t>
+          <t>第89話</t>
         </is>
       </c>
     </row>
@@ -18824,17 +19866,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第9話-1：黄昏の茶会</t>
+          <t>第84話その3</t>
         </is>
       </c>
     </row>
@@ -18844,17 +19886,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第13話</t>
+          <t>第４３話　勇者、合体した六邪神将を撃破し、めでたしめでたし（５）</t>
         </is>
       </c>
     </row>
@@ -18864,17 +19906,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>アイドル辞めるけど結婚してくれますか!?</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>三吉汐美(著者)</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第19話前半</t>
+          <t>拷問161</t>
         </is>
       </c>
     </row>
@@ -18884,17 +19926,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第84話その2</t>
+          <t>第2話前編：重すぎる想い</t>
         </is>
       </c>
     </row>
@@ -18904,17 +19946,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第４３話　勇者、合体した六邪神将を撃破し、めでたしめでたし（４）</t>
+          <t>第90話　その2</t>
         </is>
       </c>
     </row>
@@ -18924,17 +19966,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>衛宮さんちの今日のごはん</t>
+          <t>バーサス</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>TAa(漫画) 只野まこと(料理監修) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第77話</t>
+          <t>第29話 魔王VS.ロボット（後編-1）</t>
         </is>
       </c>
     </row>
@@ -18944,17 +19986,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>六志麻あさ 業務用餅 kisui</t>
+          <t>FUNA 東西 モトエ恵介</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第７６話</t>
+          <t>第125話　襲撃［その4］</t>
         </is>
       </c>
     </row>
@@ -18964,17 +20006,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>くらいあの子としたいこと</t>
+          <t>北斗の拳 世紀末ドラマ撮影伝</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>碇マナツ(著者)</t>
+          <t>原案/武論尊・原哲夫 漫画/倉尾宏</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第87話</t>
+          <t>第78話 映画公開、審判の時!!</t>
         </is>
       </c>
     </row>
@@ -18984,17 +20026,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>まったく最近の探偵ときたら</t>
+          <t>塔の管理をしてみよう</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>五十嵐正邦(著者)</t>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第117話</t>
+          <t>第95話後編</t>
         </is>
       </c>
     </row>
@@ -19004,17 +20046,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+          <t>俺は星間国家の悪徳領主！</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>板垣恵介 林たかあき</t>
+          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第59話 流水の獲物</t>
+          <t>第43話　契約</t>
         </is>
       </c>
     </row>
@@ -19024,17 +20066,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>最弱テイマーはゴミ拾いの旅を始めました。@COMIC</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>漫画：蕗野 冬 原作：ほのぼのる500 キャラクター原案：なま</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第90話　その1</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -19044,17 +20086,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>めっちゃ召喚された件 THE COMIC</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>拷問160</t>
+          <t>番外編11</t>
         </is>
       </c>
     </row>
@@ -19064,17 +20106,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
+          <t>セレビィ量産型(著者)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第41話-2</t>
+          <t>第24話前半</t>
         </is>
       </c>
     </row>
@@ -19084,17 +20126,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+          <t>英雄女騎士に有能とバレた俺の美人ハーレム騎士団 ガイカク・ヒクメの奇術騎士団</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>KAKERU</t>
+          <t>明石六郎(原作) 太盛(作画) 氷室しゅんすけ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第71話「ファントム・アレイ」（前半）</t>
+          <t>第13話-2</t>
         </is>
       </c>
     </row>
@@ -19104,17 +20146,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第21話①</t>
+          <t>第75話(後編) ヴァルハラからの贈り物</t>
         </is>
       </c>
     </row>
@@ -19124,17 +20166,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
+          <t>女子高生の無駄づかい</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
+          <t>ビーノ(著者)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第7話①「伝えたいこと」</t>
+          <t>第139話　ぶっけん</t>
         </is>
       </c>
     </row>
@@ -19144,17 +20186,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>陰キャの俺が席替えでS級美少女に囲まれたら秘密の関係が始まった。</t>
+          <t>ライブダンジョン！</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>星野 星野(原作) バラマツヒトミ(漫画) 黒兎 ゆう(キャラクター原案)</t>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第8話</t>
+          <t>第92話前半</t>
         </is>
       </c>
     </row>
@@ -19164,17 +20206,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>漫画/すたひろ 原作/Y.A</t>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>chapter75【39話②】</t>
+          <t>第8話　みんなでカラオケ（前編）</t>
         </is>
       </c>
     </row>
@@ -19184,17 +20226,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>黄金の経験値</t>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+          <t>空野進 sorani ファルまろ</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第20話（後編）</t>
+          <t>第15話　最弱貴族、領地を成長させる（１）</t>
         </is>
       </c>
     </row>
@@ -19204,17 +20246,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>空野進 sorani ファルまろ</t>
+          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第14話　最弱貴族、悪役令嬢を脱がす（４）</t>
+          <t>第85話前半</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-12-22
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -33,6 +33,7 @@
     <sheet name="2025-12-01" sheetId="25" state="visible" r:id="rId25"/>
     <sheet name="2025-12-08" sheetId="26" state="visible" r:id="rId26"/>
     <sheet name="2025-12-15" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="2025-12-22" sheetId="28" state="visible" r:id="rId28"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -19261,22 +19262,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>ワンパンマン</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>217撃目</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>不徳のギルド</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>河添太一</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第１０１話：新たな一歩</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第34話：プロのテク②</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第19話-2「今日も特別な日」</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第７２話『先端停止』②</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第37話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第14話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第34話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第134話　サポーターを決めなくちゃ！</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>黒幕一家に転生したけど原作無視して独立する</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第５話　ゲス子爵を成敗して独立する（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>クセ強彼女は床にいざなう</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>須河篤志(著者)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>休載漫画</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>ダークサモナーとデキている</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>車王(著者)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第82話</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>まんきつしたい常連さん</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>しんみりん(著者)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第51話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第12話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>魔のものたちは企てる</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>加藤拓弐(原作) ガしガし(作画)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第32話</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第131話　幕間（中編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第５５話　封印を解く器用貧乏（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第53話</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>夜州 nini 藻</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第71話(後編)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンの幼なじみ</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>久真やすひさ(著者)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>お休みイラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>三部べべ(漫画) ねうしとら(原作)</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第5話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>望まぬ不死の冒険者</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>中曽根ハイジ（漫画） 丘野 優（原作） じゃいあん（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第62話　助太刀</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第76話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第57話②　スローライフをしてみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第144話 よくわからないけれど港町に着いたみたいです（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第43話　奴は祝う（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>美人女上司滝沢さん</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>やんBARU(著者)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第209話</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第49話 先生と生徒④</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>金属スライムを倒しまくった俺が【黒鋼の王】と呼ばれるまで</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>藤屋いずこ(著者) 温泉カピバラ(原作) 山椒魚(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>コミックス3巻発売漫画</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>はぐはぐ(著者)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第89話</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第84話その3</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第４３話　勇者、合体した六邪神将を撃破し、めでたしめでたし（５）</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>拷問161</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第2話前編：重すぎる想い</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第90話　その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>バーサス</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第29話 魔王VS.ロボット（後編-1）</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>FUNA 東西 モトエ恵介</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第125話　襲撃［その4］</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>北斗の拳 世紀末ドラマ撮影伝</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>原案/武論尊・原哲夫 漫画/倉尾宏</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第78話 映画公開、審判の時!!</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>塔の管理をしてみよう</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第95話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>俺は星間国家の悪徳領主！</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第43話　契約</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>最弱テイマーはゴミ拾いの旅を始めました。@COMIC</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>漫画：蕗野 冬 原作：ほのぼのる500 キャラクター原案：なま</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>めっちゃ召喚された件 THE COMIC</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>番外編11</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>セレビィ量産型(著者)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第24話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>英雄女騎士に有能とバレた俺の美人ハーレム騎士団 ガイカク・ヒクメの奇術騎士団</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>明石六郎(原作) 太盛(作画) 氷室しゅんすけ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第13話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第75話(後編) ヴァルハラからの贈り物</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>女子高生の無駄づかい</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>ビーノ(著者)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第139話　ぶっけん</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>ライブダンジョン！</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第92話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第8話　みんなでカラオケ（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第15話　最弱貴族、領地を成長させる（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第85話前半</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ワンパンマン</t>
+          <t>生徒会にも穴はある！</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>原作/ＯＮＥ 作画/村田雄介</t>
+          <t>むちまろ</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>217撃目</t>
+          <t>第142話	私もぎゅっと!!</t>
         </is>
       </c>
     </row>
@@ -19286,17 +20328,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>不徳のギルド</t>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>河添太一</t>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第１０１話：新たな一歩</t>
+          <t>第34話：プロのテク③</t>
         </is>
       </c>
     </row>
@@ -19306,17 +20348,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>zunta(作画) はらわたさいぞう(原作)</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第34話：プロのテク②</t>
+          <t>第７２話『先端停止』③</t>
         </is>
       </c>
     </row>
@@ -19326,17 +20368,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第19話-2「今日も特別な日」</t>
+          <t>第6話 後編</t>
         </is>
       </c>
     </row>
@@ -19346,17 +20388,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>蜘蛛ですが、なにか？</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第７２話『先端停止』②</t>
+          <t>第77話その2</t>
         </is>
       </c>
     </row>
@@ -19366,17 +20408,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第37話②</t>
+          <t>第43話</t>
         </is>
       </c>
     </row>
@@ -19386,17 +20428,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+          <t>帰ってください！ 阿久津さん</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+          <t>長岡太一(著者)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第14話-1</t>
+          <t>第200話</t>
         </is>
       </c>
     </row>
@@ -19406,17 +20448,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第34話前半</t>
+          <t>第81話その2</t>
         </is>
       </c>
     </row>
@@ -19426,17 +20468,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第134話　サポーターを決めなくちゃ！</t>
+          <t>第17話後半</t>
         </is>
       </c>
     </row>
@@ -19446,17 +20488,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>黒幕一家に転生したけど原作無視して独立する</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>空野進 赤村晃人 笠間三四郎 るろお</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第５話　ゲス子爵を成敗して独立する（４）</t>
+          <t>第135話　腕試ししちゃいましょ♪・前編</t>
         </is>
       </c>
     </row>
@@ -19466,17 +20508,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>クセ強彼女は床にいざなう</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>須河篤志(著者)</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>休載漫画</t>
+          <t>第14話</t>
         </is>
       </c>
     </row>
@@ -19486,17 +20528,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ダークサモナーとデキている</t>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>車王(著者)</t>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第82話</t>
+          <t>第27話②</t>
         </is>
       </c>
     </row>
@@ -19506,17 +20548,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>まんきつしたい常連さん</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>しんみりん(著者)</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第51話</t>
+          <t>第131話　幕間（後編）</t>
         </is>
       </c>
     </row>
@@ -19526,17 +20568,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+          <t>異世界のんびり農家</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第12話-2</t>
+          <t>第313話</t>
         </is>
       </c>
     </row>
@@ -19546,17 +20588,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>魔のものたちは企てる</t>
+          <t>貞操逆転世界で頼めばヤれると噂の俺</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>加藤拓弐(原作) ガしガし(作画)</t>
+          <t>澄田佑貴(漫画) aaa168（スリーエー）(原作)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第32話</t>
+          <t>第3話</t>
         </is>
       </c>
     </row>
@@ -19566,17 +20608,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>異世界魔王と召喚少女の奴隷魔術</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第131話　幕間（中編）</t>
+          <t>第５５話　封印を解く器用貧乏（４）</t>
         </is>
       </c>
     </row>
@@ -19586,17 +20628,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>小林さんちのメイドラゴン</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>クール教信者</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第５５話　封印を解く器用貧乏（３）</t>
+          <t>第156話</t>
         </is>
       </c>
     </row>
@@ -19606,17 +20648,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>淫獄団地</t>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第53話</t>
+          <t>第86話　暇潰し</t>
         </is>
       </c>
     </row>
@@ -19626,17 +20668,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>夜州 nini 藻</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第71話(後編)</t>
+          <t>第76話➁</t>
         </is>
       </c>
     </row>
@@ -19646,17 +20688,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ダンジョンの幼なじみ</t>
+          <t>アザミヤコを好きになる</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>久真やすひさ(著者)</t>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>お休みイラスト</t>
+          <t>第12話前編</t>
         </is>
       </c>
     </row>
@@ -19666,17 +20708,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
+          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>三部べべ(漫画) ねうしとら(原作)</t>
+          <t>モリタ Ｕ４ nima</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第5話-1</t>
+          <t>第14話（５）　春とおぼっちゃまとピクニックランチ（５）</t>
         </is>
       </c>
     </row>
@@ -19686,17 +20728,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>望まぬ不死の冒険者</t>
+          <t>ダンジョンの幼なじみ</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>中曽根ハイジ（漫画） 丘野 優（原作） じゃいあん（キャラクター原案）</t>
+          <t>久真やすひさ(著者)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第62話　助太刀</t>
+          <t>第2回人気投票結果発表！</t>
         </is>
       </c>
     </row>
@@ -19706,17 +20748,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第76話①</t>
+          <t>第58話①　おすそわけをしてみた</t>
         </is>
       </c>
     </row>
@@ -19726,17 +20768,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>貞操逆転世界の童貞辺境領主騎士</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>柳瀬こたつ（漫画） 道造（原作） めろん２２（キャラクター原案）</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第57話②　スローライフをしてみた</t>
+          <t>第11話　やむなき犠牲（後編）</t>
         </is>
       </c>
     </row>
@@ -19746,17 +20788,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第144話 よくわからないけれど港町に着いたみたいです（２）</t>
+          <t>第9話-2：黄昏の茶会</t>
         </is>
       </c>
     </row>
@@ -19766,17 +20808,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第43話　奴は祝う（後編）</t>
+          <t>第145話 よくわからないけれどナメられているみたいです（１）</t>
         </is>
       </c>
     </row>
@@ -19786,17 +20828,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>美人女上司滝沢さん</t>
+          <t>路地裏で拾った女の子がバッドエンド後の乙女ゲームのヒロインだった件</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>やんBARU(著者)</t>
+          <t>カボチャマスク(原作) 樋乃えなが(作画) へいろー(キャラクター原案)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第209話</t>
+          <t>第2話</t>
         </is>
       </c>
     </row>
@@ -19806,17 +20848,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+          <t>骸骨騎士様、只今異世界へお出掛け中</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+          <t>サワノアキラ（漫画） 秤猿鬼（原作） KeG（キャラクター原案）</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第49話 先生と生徒④</t>
+          <t>第65話　エルフ族の決断Ⅳ</t>
         </is>
       </c>
     </row>
@@ -19826,17 +20868,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>金属スライムを倒しまくった俺が【黒鋼の王】と呼ばれるまで</t>
+          <t>聖者無双</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>藤屋いずこ(著者) 温泉カピバラ(原作) 山椒魚(キャラクター原案)</t>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>コミックス3巻発売漫画</t>
+          <t>第95話　奴隷の扱い・戦闘準備（後半）</t>
         </is>
       </c>
     </row>
@@ -19846,17 +20888,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>サーシャちゃんとクラスメイトオタクくん</t>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>はぐはぐ(著者)</t>
+          <t>三吉汐美(著者)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第89話</t>
+          <t>第19話後半</t>
         </is>
       </c>
     </row>
@@ -19866,17 +20908,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第84話その3</t>
+          <t>第5話前編</t>
         </is>
       </c>
     </row>
@@ -19886,17 +20928,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>お気楽領主の楽しい領地防衛 ～生産系魔術で名もなき村を最強の城塞都市に～</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>青色まろ（漫画） 赤池宗（原作） 転（原作イラスト）</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第４３話　勇者、合体した六邪神将を撃破し、めでたしめでたし（５）</t>
+          <t>第36話　出陣</t>
         </is>
       </c>
     </row>
@@ -19906,17 +20948,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>くらいあの子としたいこと</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>碇マナツ(著者)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>拷問161</t>
+          <t>第88話</t>
         </is>
       </c>
     </row>
@@ -19926,17 +20968,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第2話前編：重すぎる想い</t>
+          <t>第４４話　勇者、S級ランクに認定される。弟は、ミカエルとクエストに向かったら、ラファエルが降ってくる（１）</t>
         </is>
       </c>
     </row>
@@ -19946,17 +20988,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>『おっぱい揉みたい』って叫んだら、妹の友達と付き合うことになりました。</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>凪木エコ(原作) 白クマシェイク(キャラクター原案) 逢沢もにょ(作画)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第90話　その2</t>
+          <t>第16話</t>
         </is>
       </c>
     </row>
@@ -19966,17 +21008,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>バーサス</t>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+          <t>板垣恵介 林たかあき</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第29話 魔王VS.ロボット（後編-1）</t>
+          <t>第60話 間合いの緊張感</t>
         </is>
       </c>
     </row>
@@ -19986,17 +21028,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>FUNA 東西 モトエ恵介</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第125話　襲撃［その4］</t>
+          <t>第90話　その3</t>
         </is>
       </c>
     </row>
@@ -20006,17 +21048,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>北斗の拳 世紀末ドラマ撮影伝</t>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>原案/武論尊・原哲夫 漫画/倉尾宏</t>
+          <t>六志麻あさ 業務用餅 kisui</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第78話 映画公開、審判の時!!</t>
+          <t>第７７話</t>
         </is>
       </c>
     </row>
@@ -20026,17 +21068,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>塔の管理をしてみよう</t>
+          <t>BL世界に転生したので、モブ女子とラブコメします。</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+          <t>karl(著者)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第95話後編</t>
+          <t>読切</t>
         </is>
       </c>
     </row>
@@ -20046,17 +21088,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>俺は星間国家の悪徳領主！</t>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第43話　契約</t>
+          <t>第21話②</t>
         </is>
       </c>
     </row>
@@ -20066,17 +21108,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>最弱テイマーはゴミ拾いの旅を始めました。@COMIC</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>漫画：蕗野 冬 原作：ほのぼのる500 キャラクター原案：なま</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第28話</t>
+          <t>拷問162</t>
         </is>
       </c>
     </row>
@@ -20086,17 +21128,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>めっちゃ召喚された件 THE COMIC</t>
+          <t>回復術士のやり直し</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
+          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>番外編11</t>
+          <t>第75話-1</t>
         </is>
       </c>
     </row>
@@ -20106,17 +21148,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>三枝さんはメガネ先輩と恋を描く</t>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>セレビィ量産型(著者)</t>
+          <t>KAKERU</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第24話前半</t>
+          <t>第71話「ファントム・アレイ」（後半）</t>
         </is>
       </c>
     </row>
@@ -20126,17 +21168,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>英雄女騎士に有能とバレた俺の美人ハーレム騎士団 ガイカク・ヒクメの奇術騎士団</t>
+          <t>地味子な三葉さんが僕を誘惑する</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>明石六郎(原作) 太盛(作画) 氷室しゅんすけ(キャラクター原案)</t>
+          <t>はぶらえる(著者)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第13話-2</t>
+          <t>第13話前半</t>
         </is>
       </c>
     </row>
@@ -20146,17 +21188,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+          <t>Lv２からチートだった元勇者候補のまったり異世界ライフ</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+          <t>糸町秋音（漫画） 鬼ノ城ミヤ（原作） 片桐（キャラクター原案）</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第75話(後編) ヴァルハラからの贈り物</t>
+          <t>第64話　混血児</t>
         </is>
       </c>
     </row>
@@ -20166,17 +21208,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>女子高生の無駄づかい</t>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ビーノ(著者)</t>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第139話　ぶっけん</t>
+          <t>第36話</t>
         </is>
       </c>
     </row>
@@ -20186,17 +21228,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ライブダンジョン！</t>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+          <t>漫画/すたひろ 原作/Y.A</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第92話前半</t>
+          <t>chapter76【40話①】</t>
         </is>
       </c>
     </row>
@@ -20206,17 +21248,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+          <t>空野進 sorani ファルまろ</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第8話　みんなでカラオケ（前編）</t>
+          <t>第15話　最弱貴族、領地を成長させる（２）</t>
         </is>
       </c>
     </row>
@@ -20226,17 +21268,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+          <t>世界最高の暗殺者、異世界貴族に転生する</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>空野進 sorani ファルまろ</t>
+          <t>月夜涙(原作) 皇ハマオ(漫画) れい亜(キャラクター原案)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第15話　最弱貴族、領地を成長させる（１）</t>
+          <t>第40話-2</t>
         </is>
       </c>
     </row>
@@ -20246,17 +21288,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+          <t>黄金の経験値</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第85話前半</t>
+          <t>第21話（前編）</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2025-12-29
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -34,6 +34,7 @@
     <sheet name="2025-12-08" sheetId="26" state="visible" r:id="rId26"/>
     <sheet name="2025-12-15" sheetId="27" state="visible" r:id="rId27"/>
     <sheet name="2025-12-22" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="2025-12-29" sheetId="29" state="visible" r:id="rId29"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -20303,22 +20304,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第142話	私もぎゅっと!!</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第34話：プロのテク③</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第７２話『先端停止』③</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第6話 後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>蜘蛛ですが、なにか？</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第77話その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第43話</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>帰ってください！ 阿久津さん</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>長岡太一(著者)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第200話</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第81話その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第17話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第135話　腕試ししちゃいましょ♪・前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第14話</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第27話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第131話　幕間（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第313話</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>貞操逆転世界で頼めばヤれると噂の俺</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>澄田佑貴(漫画) aaa168（スリーエー）(原作)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第3話</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第５５話　封印を解く器用貧乏（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>小林さんちのメイドラゴン</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>クール教信者</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第156話</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第86話　暇潰し</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第76話➁</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>アザミヤコを好きになる</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第12話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>モリタ Ｕ４ nima</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第14話（５）　春とおぼっちゃまとピクニックランチ（５）</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンの幼なじみ</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>久真やすひさ(著者)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第2回人気投票結果発表！</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第58話①　おすそわけをしてみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>貞操逆転世界の童貞辺境領主騎士</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>柳瀬こたつ（漫画） 道造（原作） めろん２２（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第11話　やむなき犠牲（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第9話-2：黄昏の茶会</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第145話 よくわからないけれどナメられているみたいです（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>路地裏で拾った女の子がバッドエンド後の乙女ゲームのヒロインだった件</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>カボチャマスク(原作) 樋乃えなが(作画) へいろー(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第2話</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>骸骨騎士様、只今異世界へお出掛け中</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>サワノアキラ（漫画） 秤猿鬼（原作） KeG（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第65話　エルフ族の決断Ⅳ</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>聖者無双</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第95話　奴隷の扱い・戦闘準備（後半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>三吉汐美(著者)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第19話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第5話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>お気楽領主の楽しい領地防衛 ～生産系魔術で名もなき村を最強の城塞都市に～</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>青色まろ（漫画） 赤池宗（原作） 転（原作イラスト）</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第36話　出陣</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第88話</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第４４話　勇者、S級ランクに認定される。弟は、ミカエルとクエストに向かったら、ラファエルが降ってくる（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>『おっぱい揉みたい』って叫んだら、妹の友達と付き合うことになりました。</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>凪木エコ(原作) 白クマシェイク(キャラクター原案) 逢沢もにょ(作画)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第16話</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 林たかあき</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第60話 間合いの緊張感</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第90話　その3</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>六志麻あさ 業務用餅 kisui</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第７７話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>BL世界に転生したので、モブ女子とラブコメします。</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>karl(著者)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>読切</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第21話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>拷問162</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>回復術士のやり直し</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第75話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>KAKERU</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第71話「ファントム・アレイ」（後半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>地味子な三葉さんが僕を誘惑する</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>はぶらえる(著者)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第13話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>Lv２からチートだった元勇者候補のまったり異世界ライフ</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>糸町秋音（漫画） 鬼ノ城ミヤ（原作） 片桐（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第64話　混血児</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第36話</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>chapter76【40話①】</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第15話　最弱貴族、領地を成長させる（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>世界最高の暗殺者、異世界貴族に転生する</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>月夜涙(原作) 皇ハマオ(漫画) れい亜(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第40話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>黄金の経験値</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第21話（前編）</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>生徒会にも穴はある！</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>むちまろ</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第142話	私もぎゅっと!!</t>
+          <t>218撃目</t>
         </is>
       </c>
     </row>
@@ -20328,17 +21370,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+          <t>異世界おじさん</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>zunta(作画) はらわたさいぞう(原作)</t>
+          <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第34話：プロのテク③</t>
+          <t>第74話</t>
         </is>
       </c>
     </row>
@@ -20348,17 +21390,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>異種族レビュアーズ</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>天原(原作) masha(作画)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第７２話『先端停止』③</t>
+          <t>第89話</t>
         </is>
       </c>
     </row>
@@ -20368,17 +21410,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第6話 後編</t>
+          <t>【描きおろし公開】人気投票企画『みんなでハロウィン！』、結果発表！【第12巻発売記念】</t>
         </is>
       </c>
     </row>
@@ -20388,17 +21430,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>蜘蛛ですが、なにか？</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第77話その2</t>
+          <t>第43話①</t>
         </is>
       </c>
     </row>
@@ -20408,17 +21450,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第43話</t>
+          <t>第20話-1「パーフェクトB級冒険者」</t>
         </is>
       </c>
     </row>
@@ -20428,17 +21470,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>帰ってください！ 阿久津さん</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>長岡太一(著者)</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第200話</t>
+          <t>第７２話『先端停止』④</t>
         </is>
       </c>
     </row>
@@ -20448,17 +21490,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+          <t>魔王の俺が奴隷エルフを嫁にしたんだが、どう愛でればいい？</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+          <t>原作／手島史詞 キャラクター原案／COMTA 漫画／板垣ハコ</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第81話その2</t>
+          <t>第75話</t>
         </is>
       </c>
     </row>
@@ -20468,17 +21510,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第17話後半</t>
+          <t>第14話-2</t>
         </is>
       </c>
     </row>
@@ -20488,17 +21530,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第135話　腕試ししちゃいましょ♪・前編</t>
+          <t>コミックス第7巻発売告知！</t>
         </is>
       </c>
     </row>
@@ -20508,17 +21550,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>久遠まこと(著者) 石のやっさん(原作)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第14話</t>
+          <t>第33話</t>
         </is>
       </c>
     </row>
@@ -20528,17 +21570,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>女友達は頼めば意外とヤらせてくれる</t>
+          <t>金属スライムを倒しまくった俺が【黒鋼の王】と呼ばれるまで</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ろくろ(漫画) 鏡遊(原作)</t>
+          <t>藤屋いずこ(著者) 温泉カピバラ(原作) 山椒魚(キャラクター原案)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第27話②</t>
+          <t>第16章-2</t>
         </is>
       </c>
     </row>
@@ -20548,17 +21590,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>異世界魔王と召喚少女の奴隷魔術</t>
+          <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+          <t>須河篤志(著者)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第131話　幕間（後編）</t>
+          <t>第18話前半</t>
         </is>
       </c>
     </row>
@@ -20568,17 +21610,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>異世界のんびり農家</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第313話</t>
+          <t>第135話　腕試ししちゃいましょ♪・後編</t>
         </is>
       </c>
     </row>
@@ -20588,17 +21630,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>貞操逆転世界で頼めばヤれると噂の俺</t>
+          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>澄田佑貴(漫画) aaa168（スリーエー）(原作)</t>
+          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第3話</t>
+          <t>第34話後半</t>
         </is>
       </c>
     </row>
@@ -20608,17 +21650,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>「おかえり、パパ」</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>蝉丸</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第５５話　封印を解く器用貧乏（４）</t>
+          <t>第31話　庇護</t>
         </is>
       </c>
     </row>
@@ -20628,17 +21670,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>小林さんちのメイドラゴン</t>
+          <t>ダークサモナーとデキている</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>クール教信者</t>
+          <t>車王(著者)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第156話</t>
+          <t>第83話</t>
         </is>
       </c>
     </row>
@@ -20648,17 +21690,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>板垣恵介 猪原賽 陸井栄史</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第86話　暇潰し</t>
+          <t>★描き下ろし色紙プレゼントのお知らせ★</t>
         </is>
       </c>
     </row>
@@ -20668,17 +21710,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第76話➁</t>
+          <t>第52話前編</t>
         </is>
       </c>
     </row>
@@ -20688,17 +21730,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>アザミヤコを好きになる</t>
+          <t>異世界のんびり農家</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第12話前編</t>
+          <t>第314話</t>
         </is>
       </c>
     </row>
@@ -20708,17 +21750,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
+          <t>姫ヶ崎櫻子は今日も不憫可愛い</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>モリタ Ｕ４ nima</t>
+          <t>安田剛助(著者)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第14話（５）　春とおぼっちゃまとピクニックランチ（５）</t>
+          <t>第53話</t>
         </is>
       </c>
     </row>
@@ -20728,17 +21770,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ダンジョンの幼なじみ</t>
+          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>久真やすひさ(著者)</t>
+          <t>三部べべ(漫画) ねうしとら(原作)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第2回人気投票結果発表！</t>
+          <t>第5話-2</t>
         </is>
       </c>
     </row>
@@ -20748,17 +21790,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第58話①　おすそわけをしてみた</t>
+          <t>第76話③</t>
         </is>
       </c>
     </row>
@@ -20768,17 +21810,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>貞操逆転世界の童貞辺境領主騎士</t>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>柳瀬こたつ（漫画） 道造（原作） めろん２２（キャラクター原案）</t>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第11話　やむなき犠牲（後編）</t>
+          <t>第50話 養殖場見学と蜜の酒①</t>
         </is>
       </c>
     </row>
@@ -20788,17 +21830,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+          <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+          <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第9話-2：黄昏の茶会</t>
+          <t>第11話</t>
         </is>
       </c>
     </row>
@@ -20808,17 +21850,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第145話 よくわからないけれどナメられているみたいです（１）</t>
+          <t>第44話　奴は呑まされる</t>
         </is>
       </c>
     </row>
@@ -20828,17 +21870,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>路地裏で拾った女の子がバッドエンド後の乙女ゲームのヒロインだった件</t>
+          <t>物語の黒幕に転生して</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>カボチャマスク(原作) 樋乃えなが(作画) へいろー(キャラクター原案)</t>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第2話</t>
+          <t>第37話</t>
         </is>
       </c>
     </row>
@@ -20848,17 +21890,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>骸骨騎士様、只今異世界へお出掛け中</t>
+          <t>美人女上司滝沢さん</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>サワノアキラ（漫画） 秤猿鬼（原作） KeG（キャラクター原案）</t>
+          <t>やんBARU(著者)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第65話　エルフ族の決断Ⅳ</t>
+          <t>第210話</t>
         </is>
       </c>
     </row>
@@ -20868,17 +21910,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>聖者無双</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第95話　奴隷の扱い・戦闘準備（後半）</t>
+          <t>第58話②　おすそわけをしてみた</t>
         </is>
       </c>
     </row>
@@ -20888,17 +21930,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>アイドル辞めるけど結婚してくれますか!?</t>
+          <t>不純な彼女達は懺悔しない</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>三吉汐美(著者)</t>
+          <t>ポロロッカ(著者)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第19話後半</t>
+          <t>コミックス告知</t>
         </is>
       </c>
     </row>
@@ -20908,17 +21950,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+          <t>田舎で恋は難しい!?</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+          <t>ねこうめ(著者)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第5話前編</t>
+          <t>番外編1</t>
         </is>
       </c>
     </row>
@@ -20928,17 +21970,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>お気楽領主の楽しい領地防衛 ～生産系魔術で名もなき村を最強の城塞都市に～</t>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>青色まろ（漫画） 赤池宗（原作） 転（原作イラスト）</t>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第36話　出陣</t>
+          <t>第27話</t>
         </is>
       </c>
     </row>
@@ -20948,17 +21990,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>くらいあの子としたいこと</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>碇マナツ(著者)</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第88話</t>
+          <t>第145話 よくわからないけれどナメられているみたいです（２）</t>
         </is>
       </c>
     </row>
@@ -20968,17 +22010,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第４４話　勇者、S級ランクに認定される。弟は、ミカエルとクエストに向かったら、ラファエルが降ってくる（１）</t>
+          <t>第2話後編：重すぎる想い</t>
         </is>
       </c>
     </row>
@@ -20988,17 +22030,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>『おっぱい揉みたい』って叫んだら、妹の友達と付き合うことになりました。</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>凪木エコ(原作) 白クマシェイク(キャラクター原案) 逢沢もにょ(作画)</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第16話</t>
+          <t>拷問163</t>
         </is>
       </c>
     </row>
@@ -21008,17 +22050,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>板垣恵介 林たかあき</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第60話 間合いの緊張感</t>
+          <t>第４４話　勇者、S級ランクに認定される。弟は、ミカエルとクエストに向かったら、ラファエルが降ってくる（２）</t>
         </is>
       </c>
     </row>
@@ -21028,17 +22070,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>北斗の拳 世紀末ドラマ撮影伝</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>原案/武論尊・原哲夫 漫画/倉尾宏</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第90話　その3</t>
+          <t>第79話 映画北斗、観客の反応!!（前）</t>
         </is>
       </c>
     </row>
@@ -21048,17 +22090,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+          <t>バーサス</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>六志麻あさ 業務用餅 kisui</t>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第７７話</t>
+          <t>★描き下ろし色紙プレゼントのお知らせ★</t>
         </is>
       </c>
     </row>
@@ -21068,17 +22110,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>BL世界に転生したので、モブ女子とラブコメします。</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>karl(著者)</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>読切</t>
+          <t>第90話　その4</t>
         </is>
       </c>
     </row>
@@ -21088,17 +22130,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第21話②</t>
+          <t>第7話②「伝えたいこと」</t>
         </is>
       </c>
     </row>
@@ -21108,17 +22150,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>最弱テイマーはゴミ拾いの旅を始めました。@COMIC</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>漫画：蕗野 冬 原作：ほのぼのる500 キャラクター原案：なま</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>拷問162</t>
+          <t>第29話</t>
         </is>
       </c>
     </row>
@@ -21128,17 +22170,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>回復術士のやり直し</t>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第75話-1</t>
+          <t>第76話(前編) 闇市と闇売人と闇取引と</t>
         </is>
       </c>
     </row>
@@ -21148,17 +22190,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>KAKERU</t>
+          <t>はぐはぐ(著者)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第71話「ファントム・アレイ」（後半）</t>
+          <t>第90話</t>
         </is>
       </c>
     </row>
@@ -21168,17 +22210,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>地味子な三葉さんが僕を誘惑する</t>
+          <t>塔の管理をしてみよう</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>はぶらえる(著者)</t>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第13話前半</t>
+          <t>第96話前編</t>
         </is>
       </c>
     </row>
@@ -21188,17 +22230,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Lv２からチートだった元勇者候補のまったり異世界ライフ</t>
+          <t>めっちゃ召喚された件 THE COMIC</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>糸町秋音（漫画） 鬼ノ城ミヤ（原作） 片桐（キャラクター原案）</t>
+          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第64話　混血児</t>
+          <t>第51話①</t>
         </is>
       </c>
     </row>
@@ -21208,17 +22250,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
+          <t>セレビィ量産型(著者)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第36話</t>
+          <t>第24.5話</t>
         </is>
       </c>
     </row>
@@ -21228,17 +22270,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+          <t>幼女戦記</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>漫画/すたひろ 原作/Y.A</t>
+          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>chapter76【40話①】</t>
+          <t>第百十一章：ドードーバード航空戦Ⅵ</t>
         </is>
       </c>
     </row>
@@ -21248,17 +22290,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+          <t>ライブダンジョン！</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>空野進 sorani ファルまろ</t>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第15話　最弱貴族、領地を成長させる（２）</t>
+          <t>第92話後半</t>
         </is>
       </c>
     </row>
@@ -21268,17 +22310,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>世界最高の暗殺者、異世界貴族に転生する</t>
+          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>月夜涙(原作) 皇ハマオ(漫画) れい亜(キャラクター原案)</t>
+          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第40話-2</t>
+          <t>第85話後半</t>
         </is>
       </c>
     </row>
@@ -21288,17 +22330,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>黄金の経験値</t>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+          <t>空野進 sorani ファルまろ</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第21話（前編）</t>
+          <t>第15話　最弱貴族、領地を成長させる（３）</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2026-01-05
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -35,6 +35,7 @@
     <sheet name="2025-12-15" sheetId="27" state="visible" r:id="rId27"/>
     <sheet name="2025-12-22" sheetId="28" state="visible" r:id="rId28"/>
     <sheet name="2025-12-29" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="2026-01-05" sheetId="30" state="visible" r:id="rId30"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -21345,1000 +21346,1000 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="0" t="inlineStr">
         <is>
           <t>ワンパンマン</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="0" t="inlineStr">
         <is>
           <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="0" t="inlineStr">
         <is>
           <t>218撃目</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="0" t="inlineStr">
         <is>
           <t>異世界おじさん</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="0" t="inlineStr">
         <is>
           <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>第74話</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="0" t="inlineStr">
         <is>
           <t>異種族レビュアーズ</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="0" t="inlineStr">
         <is>
           <t>天原(原作) masha(作画)</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="0" t="inlineStr">
         <is>
           <t>第89話</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="0" t="inlineStr">
         <is>
           <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="0" t="inlineStr">
         <is>
           <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="0" t="inlineStr">
         <is>
           <t>【描きおろし公開】人気投票企画『みんなでハロウィン！』、結果発表！【第12巻発売記念】</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="0" t="inlineStr">
         <is>
           <t>魔術師クノンは見えている</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="0" t="inlineStr">
         <is>
           <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="0" t="inlineStr">
         <is>
           <t>第43話①</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="0" t="inlineStr">
         <is>
           <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="0" t="inlineStr">
         <is>
           <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="0" t="inlineStr">
         <is>
           <t>第20話-1「パーフェクトB級冒険者」</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="0" t="inlineStr">
         <is>
           <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="0" t="inlineStr">
         <is>
           <t>光永康則</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="0" t="inlineStr">
         <is>
           <t>第７２話『先端停止』④</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="0" t="inlineStr">
         <is>
           <t>魔王の俺が奴隷エルフを嫁にしたんだが、どう愛でればいい？</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="0" t="inlineStr">
         <is>
           <t>原作／手島史詞 キャラクター原案／COMTA 漫画／板垣ハコ</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="0" t="inlineStr">
         <is>
           <t>第75話</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="0" t="inlineStr">
         <is>
           <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="0" t="inlineStr">
         <is>
           <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="0" t="inlineStr">
         <is>
           <t>第14話-2</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="0" t="inlineStr">
         <is>
           <t>クラスで２番目に可愛い女の子と友だちになった</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="0" t="inlineStr">
         <is>
           <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="0" t="inlineStr">
         <is>
           <t>コミックス第7巻発売告知！</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="0" t="inlineStr">
         <is>
           <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="0" t="inlineStr">
         <is>
           <t>久遠まこと(著者) 石のやっさん(原作)</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="0" t="inlineStr">
         <is>
           <t>第33話</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="0" t="inlineStr">
         <is>
           <t>金属スライムを倒しまくった俺が【黒鋼の王】と呼ばれるまで</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="0" t="inlineStr">
         <is>
           <t>藤屋いずこ(著者) 温泉カピバラ(原作) 山椒魚(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="0" t="inlineStr">
         <is>
           <t>第16章-2</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="0" t="inlineStr">
         <is>
           <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="0" t="inlineStr">
         <is>
           <t>須河篤志(著者)</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" s="0" t="inlineStr">
         <is>
           <t>第18話前半</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="0" t="inlineStr">
         <is>
           <t>実は俺、最強でした？</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="0" t="inlineStr">
         <is>
           <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" s="0" t="inlineStr">
         <is>
           <t>第135話　腕試ししちゃいましょ♪・後編</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
+      <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="0" t="inlineStr">
         <is>
           <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="0" t="inlineStr">
         <is>
           <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D16" s="0" t="inlineStr">
         <is>
           <t>第34話後半</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
+      <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="0" t="inlineStr">
         <is>
           <t>「おかえり、パパ」</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" s="0" t="inlineStr">
         <is>
           <t>蝉丸</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D17" s="0" t="inlineStr">
         <is>
           <t>第31話　庇護</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
+      <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="0" t="inlineStr">
         <is>
           <t>ダークサモナーとデキている</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="0" t="inlineStr">
         <is>
           <t>車王(著者)</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D18" s="0" t="inlineStr">
         <is>
           <t>第83話</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
+      <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="0" t="inlineStr">
         <is>
           <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" s="0" t="inlineStr">
         <is>
           <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="D19" s="0" t="inlineStr">
         <is>
           <t>★描き下ろし色紙プレゼントのお知らせ★</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
+      <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20" s="0" t="inlineStr">
         <is>
           <t>まんきつしたい常連さん</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" s="0" t="inlineStr">
         <is>
           <t>しんみりん(著者)</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="D20" s="0" t="inlineStr">
         <is>
           <t>第52話前編</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
+      <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" s="0" t="inlineStr">
         <is>
           <t>異世界のんびり農家</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" s="0" t="inlineStr">
         <is>
           <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="D21" s="0" t="inlineStr">
         <is>
           <t>第314話</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
+      <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" s="0" t="inlineStr">
         <is>
           <t>姫ヶ崎櫻子は今日も不憫可愛い</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C22" s="0" t="inlineStr">
         <is>
           <t>安田剛助(著者)</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="D22" s="0" t="inlineStr">
         <is>
           <t>第53話</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
+      <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B23" s="0" t="inlineStr">
         <is>
           <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C23" s="0" t="inlineStr">
         <is>
           <t>三部べべ(漫画) ねうしとら(原作)</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="D23" s="0" t="inlineStr">
         <is>
           <t>第5話-2</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
+      <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" s="0" t="inlineStr">
         <is>
           <t>リビルドワールド</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C24" s="0" t="inlineStr">
         <is>
           <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="D24" s="0" t="inlineStr">
         <is>
           <t>第76話③</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
+      <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" s="0" t="inlineStr">
         <is>
           <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C25" s="0" t="inlineStr">
         <is>
           <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="D25" s="0" t="inlineStr">
         <is>
           <t>第50話 養殖場見学と蜜の酒①</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
+      <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" s="0" t="inlineStr">
         <is>
           <t>氷結令嬢さまをフォローしたら、メチャメチャ溺愛されてしまった件@comic</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C26" s="0" t="inlineStr">
         <is>
           <t>漫画：ハレノチアメ 原作：愛坂タカト キャラクター原案：Bcoca</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="D26" s="0" t="inlineStr">
         <is>
           <t>第11話</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
+      <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B27" s="0" t="inlineStr">
         <is>
           <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C27" s="0" t="inlineStr">
         <is>
           <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="D27" s="0" t="inlineStr">
         <is>
           <t>第44話　奴は呑まされる</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
+      <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" s="0" t="inlineStr">
         <is>
           <t>物語の黒幕に転生して</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C28" s="0" t="inlineStr">
         <is>
           <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D28" s="0" t="inlineStr">
         <is>
           <t>第37話</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
+      <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B29" s="0" t="inlineStr">
         <is>
           <t>美人女上司滝沢さん</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C29" s="0" t="inlineStr">
         <is>
           <t>やんBARU(著者)</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="D29" s="0" t="inlineStr">
         <is>
           <t>第210話</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
+      <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B30" s="0" t="inlineStr">
         <is>
           <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C30" s="0" t="inlineStr">
         <is>
           <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="D30" s="0" t="inlineStr">
         <is>
           <t>第58話②　おすそわけをしてみた</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
+      <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B31" s="0" t="inlineStr">
         <is>
           <t>不純な彼女達は懺悔しない</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C31" s="0" t="inlineStr">
         <is>
           <t>ポロロッカ(著者)</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="D31" s="0" t="inlineStr">
         <is>
           <t>コミックス告知</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
+      <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B32" s="0" t="inlineStr">
         <is>
           <t>田舎で恋は難しい!?</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C32" s="0" t="inlineStr">
         <is>
           <t>ねこうめ(著者)</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="D32" s="0" t="inlineStr">
         <is>
           <t>番外編1</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
+      <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" s="0" t="inlineStr">
         <is>
           <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C33" s="0" t="inlineStr">
         <is>
           <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="D33" s="0" t="inlineStr">
         <is>
           <t>第27話</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
+      <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" s="0" t="inlineStr">
         <is>
           <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C34" s="0" t="inlineStr">
         <is>
           <t>内々けやき あし カオミン</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="D34" s="0" t="inlineStr">
         <is>
           <t>第145話 よくわからないけれどナメられているみたいです（２）</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
+      <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B35" s="0" t="inlineStr">
         <is>
           <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C35" s="0" t="inlineStr">
         <is>
           <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="D35" s="0" t="inlineStr">
         <is>
           <t>第2話後編：重すぎる想い</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
+      <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B36" s="0" t="inlineStr">
         <is>
           <t>姫様“拷問”の時間です</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="C36" s="0" t="inlineStr">
         <is>
           <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="D36" s="0" t="inlineStr">
         <is>
           <t>拷問163</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
+      <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B37" s="0" t="inlineStr">
         <is>
           <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C37" s="0" t="inlineStr">
         <is>
           <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="D37" s="0" t="inlineStr">
         <is>
           <t>第４４話　勇者、S級ランクに認定される。弟は、ミカエルとクエストに向かったら、ラファエルが降ってくる（２）</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
+      <c r="A38" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" s="0" t="inlineStr">
         <is>
           <t>北斗の拳 世紀末ドラマ撮影伝</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="C38" s="0" t="inlineStr">
         <is>
           <t>原案/武論尊・原哲夫 漫画/倉尾宏</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="D38" s="0" t="inlineStr">
         <is>
           <t>第79話 映画北斗、観客の反応!!（前）</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
+      <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" s="0" t="inlineStr">
         <is>
           <t>バーサス</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="C39" s="0" t="inlineStr">
         <is>
           <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="D39" s="0" t="inlineStr">
         <is>
           <t>★描き下ろし色紙プレゼントのお知らせ★</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="n">
+      <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B40" s="0" t="inlineStr">
         <is>
           <t>理想のヒモ生活</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C40" s="0" t="inlineStr">
         <is>
           <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="D40" s="0" t="inlineStr">
         <is>
           <t>第90話　その4</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
+      <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" s="0" t="inlineStr">
         <is>
           <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C41" s="0" t="inlineStr">
         <is>
           <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="D41" s="0" t="inlineStr">
         <is>
           <t>第7話②「伝えたいこと」</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
+      <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B42" s="0" t="inlineStr">
         <is>
           <t>最弱テイマーはゴミ拾いの旅を始めました。@COMIC</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C42" s="0" t="inlineStr">
         <is>
           <t>漫画：蕗野 冬 原作：ほのぼのる500 キャラクター原案：なま</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="D42" s="0" t="inlineStr">
         <is>
           <t>第29話</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="n">
+      <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B43" s="0" t="inlineStr">
         <is>
           <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C43" s="0" t="inlineStr">
         <is>
           <t>岡沢六十四 るれくちぇ sage・ジョー</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="D43" s="0" t="inlineStr">
         <is>
           <t>第76話(前編) 闇市と闇売人と闇取引と</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="n">
+      <c r="A44" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B44" s="0" t="inlineStr">
         <is>
           <t>サーシャちゃんとクラスメイトオタクくん</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C44" s="0" t="inlineStr">
         <is>
           <t>はぐはぐ(著者)</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="D44" s="0" t="inlineStr">
         <is>
           <t>第90話</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
+      <c r="A45" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B45" s="0" t="inlineStr">
         <is>
           <t>塔の管理をしてみよう</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="C45" s="0" t="inlineStr">
         <is>
           <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="D45" s="0" t="inlineStr">
         <is>
           <t>第96話前編</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="n">
+      <c r="A46" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B46" s="0" t="inlineStr">
         <is>
           <t>めっちゃ召喚された件 THE COMIC</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="C46" s="0" t="inlineStr">
         <is>
           <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="D46" s="0" t="inlineStr">
         <is>
           <t>第51話①</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="n">
+      <c r="A47" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B47" s="0" t="inlineStr">
         <is>
           <t>三枝さんはメガネ先輩と恋を描く</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="C47" s="0" t="inlineStr">
         <is>
           <t>セレビィ量産型(著者)</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="D47" s="0" t="inlineStr">
         <is>
           <t>第24.5話</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="n">
+      <c r="A48" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B48" s="0" t="inlineStr">
         <is>
           <t>幼女戦記</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="C48" s="0" t="inlineStr">
         <is>
           <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="D48" s="0" t="inlineStr">
         <is>
           <t>第百十一章：ドードーバード航空戦Ⅵ</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="n">
+      <c r="A49" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B49" s="0" t="inlineStr">
         <is>
           <t>ライブダンジョン！</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C49" s="0" t="inlineStr">
         <is>
           <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="D49" s="0" t="inlineStr">
         <is>
           <t>第92話後半</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="n">
+      <c r="A50" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B50" s="0" t="inlineStr">
         <is>
           <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C50" s="0" t="inlineStr">
         <is>
           <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="D50" s="0" t="inlineStr">
         <is>
           <t>第85話後半</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="n">
+      <c r="A51" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B51" s="0" t="inlineStr">
         <is>
           <t>最弱貴族に転生したので悪役たちを集めてみた</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C51" s="0" t="inlineStr">
         <is>
           <t>空野進 sorani ファルまろ</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="D51" s="0" t="inlineStr">
         <is>
           <t>第15話　最弱貴族、領地を成長させる（３）</t>
         </is>
@@ -23390,6 +23391,1047 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>貞操逆転世界で頼めばヤれると噂の俺</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>澄田佑貴(漫画) aaa168（スリーエー）(原作)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>第4話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>第44話</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>【描きおろし公開】人気投票企画『みんなでハロウィン！』、結果発表！【第12巻発売記念】</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>異世界居酒屋「のぶ」</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>第128話</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>おまけ68</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>田舎で恋は難しい!?</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ねこうめ(著者)</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>第3話</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>特別編</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>剥かせて！竜ケ崎さん</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>一智和智</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>大学生編 第16話</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>お正月イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>第76話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>小林さんちのメイドラゴン</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>クール教信者</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>第157話</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>第5話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>異世界食堂　洋食のねこや</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>第43話➁</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>第10話-1：友達と一緒なら</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>アザミヤコを好きになる</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>第12話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>★描き下ろし色紙プレゼントのお知らせ★</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>第91話　その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>三吉汐美(著者)</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>第４４話　勇者、S級ランクに認定される。弟は、ミカエルとクエストに向かったら、ラファエルが降ってくる（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ウォルテニア戦記</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>漫画：八木ゆかり 原作：保利亮太 キャラクター原案：bob</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>第59話</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>インフィニット・デンドログラム</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>今井神 原作：海道左近 キャラクター原案：タイキ</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>第75話</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>六志麻あさ 業務用餅 kisui</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>第７８話</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>第21話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>拷問164</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>年始特別編</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ずっと好きだった幼馴染と付き合い始めたら一途ビッチの性欲ジャンキーだったんだがどうすりゃいいですか？</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>原作：トラ子猫 作画：あらいぐま</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>第8話</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>黄金の経験値</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>第21話（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>回復術士のやり直し</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>第75話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ダメ人間の愛しかた</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>岩葉(著者)</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>第23話後編　ダメ人間とプレゼントと彼女</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>第15話　最弱貴族、領地を成長させる（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>モブ司祭だけど、この世界が乙女ゲームだと気づいたのでヒロインを育成します</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>井冬良(漫画) レオナールＤ(原作) りいちゅ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>第5話-1：祝福の時</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>第2話後編：重すぎる想い</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>ひとりぼっちの異世界攻略</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>びび（漫画） 五示正司（原作）</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>第251話　エグい情報承りまーす</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>魔都精兵のスレイブ</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>原作:タカヒロ　漫画:竹村洋平</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>第169話　突入準備</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>理想の彼女</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>もりまりも(著者)</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>第31話</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>オタクに優しいギャルはいない!?</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>のりしろちゃん 魚住さかな</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>【#172】サンタ予備軍</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>異世界帰りの剣聖は、自分の実力に気がつかない　～SSSランクの隠しクエストを受けて帰ってきたらレベル１のF級探索者になったけど、異世界で鍛え上げた剣術が強すぎて王女やS級英雄たちが俺を放ってくれません</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>夜桜ユノ 吉田屋敷 もきゅ</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>第２話　異世界帰りの剣聖は、ハイエナに「ざまぁ」する（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>♀ガキとおじさん</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>サラマンダ(著者)</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>第33話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>生徒会役員共</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>氏家ト全</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>#429</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>第74話</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>第6話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>銀河特急 ミルキー☆サブウェイ</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>河野丼(漫画) 亀山陽平(原作・監修)</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>第7話</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>カナン様はあくまでチョロい</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>nonco</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>第166話	カナンのチェストバースト</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>我輩は猫魔導師である ～キジトラ・ルークの快適チート猫生活～</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>原作：猫神信仰研究会 漫画：三國大和 キャラクター原案：ハム</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>第27話</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>第22話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>一億年ボタンを連打した俺は、気付いたら最強になっていた ～落第剣士の学院無双～</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>士土幽太郎(漫画) 月島秀一(原作) もきゅ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>第43話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>追放された底辺職「盗賊」はゲーム知識で無双する。一緒に召喚された先生も外れジョブだったけど効率的に成り上がります</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>ケンノジ 菅原イチバ カラスBTK</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>第5話　温泉で無双する(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>異種族レビュアーズ</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>天原(原作) masha(作画)</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>第89話</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>バーサス</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>★描き下ろし色紙プレゼントのお知らせ★</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>最強勇者パーティーは愛が知りたい</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>山田肌襦袢</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>第39話「デートは浮かれたっていい」</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Add ranking data for 2026-01-12
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -36,6 +36,7 @@
     <sheet name="2025-12-22" sheetId="28" state="visible" r:id="rId28"/>
     <sheet name="2025-12-29" sheetId="29" state="visible" r:id="rId29"/>
     <sheet name="2026-01-05" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="2026-01-12" sheetId="31" state="visible" r:id="rId31"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -23428,22 +23429,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>貞操逆転世界で頼めばヤれると噂の俺</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>澄田佑貴(漫画) aaa168（スリーエー）(原作)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第4話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第44話</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>【描きおろし公開】人気投票企画『みんなでハロウィン！』、結果発表！【第12巻発売記念】</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>異世界居酒屋「のぶ」</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第128話</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>おまけ68</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>田舎で恋は難しい!?</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>ねこうめ(著者)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第3話</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>特別編</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>剥かせて！竜ケ崎さん</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>一智和智</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>大学生編 第16話</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>お正月イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第76話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>小林さんちのメイドラゴン</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>クール教信者</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第157話</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第5話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>異世界食堂　洋食のねこや</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第43話➁</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第10話-1：友達と一緒なら</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>アザミヤコを好きになる</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第12話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>★描き下ろし色紙プレゼントのお知らせ★</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第91話　その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>三吉汐美(著者)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第４４話　勇者、S級ランクに認定される。弟は、ミカエルとクエストに向かったら、ラファエルが降ってくる（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>ウォルテニア戦記</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>漫画：八木ゆかり 原作：保利亮太 キャラクター原案：bob</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第59話</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>インフィニット・デンドログラム</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>今井神 原作：海道左近 キャラクター原案：タイキ</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第75話</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>六志麻あさ 業務用餅 kisui</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第７８話</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第21話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>拷問164</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>年始特別編</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>ずっと好きだった幼馴染と付き合い始めたら一途ビッチの性欲ジャンキーだったんだがどうすりゃいいですか？</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>原作：トラ子猫 作画：あらいぐま</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第8話</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>黄金の経験値</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第21話（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>回復術士のやり直し</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第75話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>ダメ人間の愛しかた</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>岩葉(著者)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第23話後編　ダメ人間とプレゼントと彼女</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第15話　最弱貴族、領地を成長させる（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>モブ司祭だけど、この世界が乙女ゲームだと気づいたのでヒロインを育成します</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>井冬良(漫画) レオナールＤ(原作) りいちゅ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第5話-1：祝福の時</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第2話後編：重すぎる想い</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>ひとりぼっちの異世界攻略</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>びび（漫画） 五示正司（原作）</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第251話　エグい情報承りまーす</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>魔都精兵のスレイブ</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>原作:タカヒロ　漫画:竹村洋平</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第169話　突入準備</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>理想の彼女</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>もりまりも(著者)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第31話</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>オタクに優しいギャルはいない!?</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>のりしろちゃん 魚住さかな</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>【#172】サンタ予備軍</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>異世界帰りの剣聖は、自分の実力に気がつかない　～SSSランクの隠しクエストを受けて帰ってきたらレベル１のF級探索者になったけど、異世界で鍛え上げた剣術が強すぎて王女やS級英雄たちが俺を放ってくれません</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>夜桜ユノ 吉田屋敷 もきゅ</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第２話　異世界帰りの剣聖は、ハイエナに「ざまぁ」する（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>♀ガキとおじさん</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>サラマンダ(著者)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第33話</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>生徒会役員共</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>氏家ト全</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>#429</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第74話</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第6話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>銀河特急 ミルキー☆サブウェイ</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>河野丼(漫画) 亀山陽平(原作・監修)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第7話</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>カナン様はあくまでチョロい</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>nonco</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第166話	カナンのチェストバースト</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>我輩は猫魔導師である ～キジトラ・ルークの快適チート猫生活～</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>原作：猫神信仰研究会 漫画：三國大和 キャラクター原案：ハム</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第27話</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第22話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>一億年ボタンを連打した俺は、気付いたら最強になっていた ～落第剣士の学院無双～</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>士土幽太郎(漫画) 月島秀一(原作) もきゅ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第43話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>追放された底辺職「盗賊」はゲーム知識で無双する。一緒に召喚された先生も外れジョブだったけど効率的に成り上がります</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>ケンノジ 菅原イチバ カラスBTK</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第5話　温泉で無双する(2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>異種族レビュアーズ</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>天原(原作) masha(作画)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第89話</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>バーサス</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>★描き下ろし色紙プレゼントのお知らせ★</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>最強勇者パーティーは愛が知りたい</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>山田肌襦袢</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第39話「デートは浮かれたっていい」</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>貞操逆転世界で頼めばヤれると噂の俺</t>
+          <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>澄田佑貴(漫画) aaa168（スリーエー）(原作)</t>
+          <t>丈(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第4話</t>
+          <t>宇崎ちゃんは遊びたい！ コミックス14巻情報！！</t>
         </is>
       </c>
     </row>
@@ -23453,17 +24495,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>不徳のギルド</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>河添太一</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第44話</t>
+          <t>第１０２話：大人組</t>
         </is>
       </c>
     </row>
@@ -23473,17 +24515,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>【描きおろし公開】人気投票企画『みんなでハロウィン！』、結果発表！【第12巻発売記念】</t>
+          <t>第35話：発動の線引き①</t>
         </is>
       </c>
     </row>
@@ -23493,17 +24535,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>異世界居酒屋「のぶ」</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第128話</t>
+          <t>第７３話『上昇停止』①</t>
         </is>
       </c>
     </row>
@@ -23513,17 +24555,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>王子様の友達</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>すけろく(著者)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>おまけ68</t>
+          <t>第33話</t>
         </is>
       </c>
     </row>
@@ -23533,17 +24575,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>田舎で恋は難しい!?</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ねこうめ(著者)</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第3話</t>
+          <t>第43話➁</t>
         </is>
       </c>
     </row>
@@ -23553,17 +24595,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>女友達は頼めば意外とヤらせてくれる</t>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ろくろ(漫画) 鏡遊(原作)</t>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>特別編</t>
+          <t>第82話その1</t>
         </is>
       </c>
     </row>
@@ -23573,17 +24615,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>剥かせて！竜ケ崎さん</t>
+          <t>このヒーラー、めんどくさい</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>一智和智</t>
+          <t>丹念に発酵(著者)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>大学生編 第16話</t>
+          <t>第93話：生け贄</t>
         </is>
       </c>
     </row>
@@ -23593,17 +24635,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>お正月イラスト</t>
+          <t>第136話　困ってる人がいる限り！</t>
         </is>
       </c>
     </row>
@@ -23613,17 +24655,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第76話④</t>
+          <t>第132話　王都に戻ってみるⅠ（前編）</t>
         </is>
       </c>
     </row>
@@ -23633,17 +24675,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>小林さんちのメイドラゴン</t>
+          <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>クール教信者</t>
+          <t>須河篤志(著者)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第157話</t>
+          <t>第18話後半</t>
         </is>
       </c>
     </row>
@@ -23653,17 +24695,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第5話後編</t>
+          <t>【第８巻発売記念】描き下ろしイラスト公開！</t>
         </is>
       </c>
     </row>
@@ -23673,17 +24715,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>異世界食堂　洋食のねこや</t>
+          <t>美人女上司滝沢さん</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
+          <t>やんBARU(著者)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第43話➁</t>
+          <t>第211話</t>
         </is>
       </c>
     </row>
@@ -23693,17 +24735,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第10話-1：友達と一緒なら</t>
+          <t>特別編</t>
         </is>
       </c>
     </row>
@@ -23713,17 +24755,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>アザミヤコを好きになる</t>
+          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第12話後編</t>
+          <t>2026年もよろしくお願いいたします</t>
         </is>
       </c>
     </row>
@@ -23733,17 +24775,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>★描き下ろし色紙プレゼントのお知らせ★</t>
+          <t>第87話　献上</t>
         </is>
       </c>
     </row>
@@ -23753,17 +24795,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第91話　その1</t>
+          <t>第77話①</t>
         </is>
       </c>
     </row>
@@ -23773,17 +24815,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>アイドル辞めるけど結婚してくれますか!?</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>三吉汐美(著者)</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>休載イラスト</t>
+          <t>番外編</t>
         </is>
       </c>
     </row>
@@ -23793,17 +24835,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第４４話　勇者、S級ランクに認定される。弟は、ミカエルとクエストに向かったら、ラファエルが降ってくる（３）</t>
+          <t>第59話①　地下王国ドンゴワに行ってみた</t>
         </is>
       </c>
     </row>
@@ -23813,17 +24855,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ウォルテニア戦記</t>
+          <t>濁る瞳で何を願う ハイセルク戦記</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>漫画：八木ゆかり 原作：保利亮太 キャラクター原案：bob</t>
+          <t>トルトネン 創-taro 斎藤八呑</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第59話</t>
+          <t>第36話 意志を持つ天災①</t>
         </is>
       </c>
     </row>
@@ -23833,17 +24875,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>インフィニット・デンドログラム</t>
+          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>今井神 原作：海道左近 キャラクター原案：タイキ</t>
+          <t>モリタ Ｕ４ nima</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第75話</t>
+          <t>第14話（６）　春とおぼっちゃまとピクニックランチ（６）</t>
         </is>
       </c>
     </row>
@@ -23853,17 +24895,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>六志麻あさ 業務用餅 kisui</t>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第７８話</t>
+          <t>祝われし休載まんが</t>
         </is>
       </c>
     </row>
@@ -23873,17 +24915,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第21話③</t>
+          <t>第42話-2</t>
         </is>
       </c>
     </row>
@@ -23893,17 +24935,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>拷問164</t>
+          <t>第91話　その2</t>
         </is>
       </c>
     </row>
@@ -23913,17 +24955,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>くらいあの子としたいこと</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>碇マナツ(著者)</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>年始特別編</t>
+          <t>第４４話　勇者、S級ランクに認定される。弟は、ミカエルとクエストに向かったら、ラファエルが降ってくる（４）</t>
         </is>
       </c>
     </row>
@@ -23933,17 +24975,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ずっと好きだった幼馴染と付き合い始めたら一途ビッチの性欲ジャンキーだったんだがどうすりゃいいですか？</t>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>原作：トラ子猫 作画：あらいぐま</t>
+          <t>板垣恵介 林たかあき</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第8話</t>
+          <t>第61話 ラストフラワー</t>
         </is>
       </c>
     </row>
@@ -23953,17 +24995,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>黄金の経験値</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第21話（後編）</t>
+          <t>拷問165</t>
         </is>
       </c>
     </row>
@@ -23973,17 +25015,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>回復術士のやり直し</t>
+          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
+          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第75話-2</t>
+          <t>第60話　最果ての国を目指して</t>
         </is>
       </c>
     </row>
@@ -23993,17 +25035,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ダメ人間の愛しかた</t>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>岩葉(著者)</t>
+          <t>KAKERU</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第23話後編　ダメ人間とプレゼントと彼女</t>
+          <t>第72話「弓王」（前半）</t>
         </is>
       </c>
     </row>
@@ -24013,17 +25055,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+          <t>バーサス</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>空野進 sorani ファルまろ</t>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第15話　最弱貴族、領地を成長させる（４）</t>
+          <t>第30話　勇者の意思（1）</t>
         </is>
       </c>
     </row>
@@ -24033,17 +25075,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>モブ司祭だけど、この世界が乙女ゲームだと気づいたのでヒロインを育成します</t>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>井冬良(漫画) レオナールＤ(原作) りいちゅ(キャラクター原案)</t>
+          <t>はぐはぐ(著者)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第5話-1：祝福の時</t>
+          <t>第91話</t>
         </is>
       </c>
     </row>
@@ -24053,17 +25095,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
+          <t>漫画/すたひろ 原作/Y.A</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第2話後編：重すぎる想い</t>
+          <t>chapter77【40話②】</t>
         </is>
       </c>
     </row>
@@ -24073,17 +25115,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ひとりぼっちの異世界攻略</t>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>びび（漫画） 五示正司（原作）</t>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第251話　エグい情報承りまーす</t>
+          <t>第76話(後編) 闇市と闇売人と闇取引と</t>
         </is>
       </c>
     </row>
@@ -24093,17 +25135,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>魔都精兵のスレイブ</t>
+          <t>陰キャの俺が席替えでS級美少女に囲まれたら秘密の関係が始まった。</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>原作:タカヒロ　漫画:竹村洋平</t>
+          <t>星野 星野(原作) バラマツヒトミ(漫画) 黒兎 ゆう(キャラクター原案)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第169話　突入準備</t>
+          <t>第9話</t>
         </is>
       </c>
     </row>
@@ -24113,17 +25155,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>理想の彼女</t>
+          <t>英雄女騎士に有能とバレた俺の美人ハーレム騎士団 ガイカク・ヒクメの奇術騎士団</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>もりまりも(著者)</t>
+          <t>明石六郎(原作) 太盛(作画) 氷室しゅんすけ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第31話</t>
+          <t>第14話-2</t>
         </is>
       </c>
     </row>
@@ -24133,17 +25175,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>オタクに優しいギャルはいない!?</t>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>のりしろちゃん 魚住さかな</t>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>【#172】サンタ予備軍</t>
+          <t>第9話　有月勇のトラウマ（前編）</t>
         </is>
       </c>
     </row>
@@ -24153,17 +25195,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>異世界帰りの剣聖は、自分の実力に気がつかない　～SSSランクの隠しクエストを受けて帰ってきたらレベル１のF級探索者になったけど、異世界で鍛え上げた剣術が強すぎて王女やS級英雄たちが俺を放ってくれません</t>
+          <t>せっかく農家に転生したので勇者は目指しません</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>夜桜ユノ 吉田屋敷 もきゅ</t>
+          <t>マツオカヨシノリ(漫画) 月見里嘉助(原作) ゆーにっと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第２話　異世界帰りの剣聖は、ハイエナに「ざまぁ」する（３）</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -24173,17 +25215,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>♀ガキとおじさん</t>
+          <t>路地裏で拾った女の子がバッドエンド後の乙女ゲームのヒロインだった件</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>サラマンダ(著者)</t>
+          <t>カボチャマスク(原作) 樋乃えなが(作画) へいろー(キャラクター原案)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第33話</t>
+          <t>休載イラスト</t>
         </is>
       </c>
     </row>
@@ -24193,17 +25235,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>生徒会役員共</t>
+          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>氏家ト全</t>
+          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>#429</t>
+          <t>EP.23①</t>
         </is>
       </c>
     </row>
@@ -24213,17 +25255,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>地味子な三葉さんが僕を誘惑する</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>はぶらえる(著者)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第74話</t>
+          <t>第13話後半</t>
         </is>
       </c>
     </row>
@@ -24233,17 +25275,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>35歳独身山田、異世界村に理想のセカンドハウスを作りたい　～異世界と現実のいいとこどりライフ～</t>
+          <t>女子高生の無駄づかい</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>出雲大吉(原作) 西尾洋一(作画) ゆのひと(キャラクター原案)</t>
+          <t>ビーノ(著者)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第6話②</t>
+          <t>ばんがいへん</t>
         </is>
       </c>
     </row>
@@ -24253,17 +25295,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>銀河特急 ミルキー☆サブウェイ</t>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>河野丼(漫画) 亀山陽平(原作・監修)</t>
+          <t>空野進 sorani ファルまろ</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第7話</t>
+          <t>第16話 最弱貴族、魔王を拾う(１)</t>
         </is>
       </c>
     </row>
@@ -24273,17 +25315,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>カナン様はあくまでチョロい</t>
+          <t>塔の管理をしてみよう</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>nonco</t>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第166話	カナンのチェストバースト</t>
+          <t>第96話後編</t>
         </is>
       </c>
     </row>
@@ -24293,17 +25335,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>我輩は猫魔導師である ～キジトラ・ルークの快適チート猫生活～</t>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>原作：猫神信仰研究会 漫画：三國大和 キャラクター原案：ハム</t>
+          <t>セレビィ量産型(著者)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第27話</t>
+          <t>新年イラスト</t>
         </is>
       </c>
     </row>
@@ -24313,17 +25355,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ノロマ魔法と呼ばれた魔法使いは重力魔法で無双する　～まだ重力の概念のない世界にて、少年は万有引力の王となる～</t>
+          <t>オタクに優しいギャルはいない!?</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>神原絵理華(漫画) 一森一輝(原作)</t>
+          <t>のりしろちゃん 魚住さかな</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第22話③</t>
+          <t>【#173】日常を君と</t>
         </is>
       </c>
     </row>
@@ -24333,17 +25375,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>一億年ボタンを連打した俺は、気付いたら最強になっていた ～落第剣士の学院無双～</t>
+          <t>病弱少女、転生して健康な肉体（最強）を手に入れる</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>士土幽太郎(漫画) 月島秀一(原作) もきゅ(キャラクター原案)</t>
+          <t>あらた伊里（漫画） アトハ（原作） 狐印（キャラクター原案）</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第43話-1</t>
+          <t>第1話　フィアナ、転生して超健康になる</t>
         </is>
       </c>
     </row>
@@ -24353,17 +25395,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>追放された底辺職「盗賊」はゲーム知識で無双する。一緒に召喚された先生も外れジョブだったけど効率的に成り上がります</t>
+          <t>賢者の孫</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ケンノジ 菅原イチバ カラスBTK</t>
+          <t>緒方俊輔(漫画) 吉岡剛(原作) 菊池政治(キャラクター原案)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第5話　温泉で無双する(2)</t>
+          <t>第97話-3</t>
         </is>
       </c>
     </row>
@@ -24373,17 +25415,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>異種族レビュアーズ</t>
+          <t>ひとりぼっちの異世界攻略</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>天原(原作) masha(作画)</t>
+          <t>びび（漫画） 五示正司（原作）</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第89話</t>
+          <t>第252話　なぜか不思議と</t>
         </is>
       </c>
     </row>
@@ -24393,17 +25435,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>バーサス</t>
+          <t>異世界でスローライフを（願望）</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+          <t>長頼（漫画） シゲ（原作） オウカ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>★描き下ろし色紙プレゼントのお知らせ★</t>
+          <t>第58話　激闘！紅い戦線！</t>
         </is>
       </c>
     </row>
@@ -24413,17 +25455,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>最強勇者パーティーは愛が知りたい</t>
+          <t>ディーふらぐ！</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>山田肌襦袢</t>
+          <t>春野友矢(著者)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第39話「デートは浮かれたっていい」</t>
+          <t>第176話</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2026-01-19
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -37,6 +37,7 @@
     <sheet name="2025-12-29" sheetId="29" state="visible" r:id="rId29"/>
     <sheet name="2026-01-05" sheetId="30" state="visible" r:id="rId30"/>
     <sheet name="2026-01-12" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="2026-01-19" sheetId="32" state="visible" r:id="rId32"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -24470,22 +24471,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！ コミックス14巻情報！！</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>不徳のギルド</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>河添太一</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第１０２話：大人組</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第35話：発動の線引き①</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第７３話『上昇停止』①</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>王子様の友達</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>すけろく(著者)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第33話</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第43話➁</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第82話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>このヒーラー、めんどくさい</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>丹念に発酵(著者)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第93話：生け贄</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第136話　困ってる人がいる限り！</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第132話　王都に戻ってみるⅠ（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>クセ強彼女は床にいざなう</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>須河篤志(著者)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第18話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>【第８巻発売記念】描き下ろしイラスト公開！</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>美人女上司滝沢さん</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>やんBARU(著者)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第211話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>まんきつしたい常連さん</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>しんみりん(著者)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>特別編</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>2026年もよろしくお願いいたします</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第87話　献上</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第77話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>番外編</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第59話①　地下王国ドンゴワに行ってみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>濁る瞳で何を願う ハイセルク戦記</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>トルトネン 創-taro 斎藤八呑</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第36話 意志を持つ天災①</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>モリタ Ｕ４ nima</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第14話（６）　春とおぼっちゃまとピクニックランチ（６）</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>祝われし休載まんが</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第42話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第91話　その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第４４話　勇者、S級ランクに認定される。弟は、ミカエルとクエストに向かったら、ラファエルが降ってくる（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 林たかあき</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第61話 ラストフラワー</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>拷問165</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第60話　最果ての国を目指して</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>KAKERU</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第72話「弓王」（前半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>バーサス</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第30話　勇者の意思（1）</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>はぐはぐ(著者)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第91話</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>chapter77【40話②】</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第76話(後編) 闇市と闇売人と闇取引と</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>陰キャの俺が席替えでS級美少女に囲まれたら秘密の関係が始まった。</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>星野 星野(原作) バラマツヒトミ(漫画) 黒兎 ゆう(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第9話</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>英雄女騎士に有能とバレた俺の美人ハーレム騎士団 ガイカク・ヒクメの奇術騎士団</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>明石六郎(原作) 太盛(作画) 氷室しゅんすけ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第14話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第9話　有月勇のトラウマ（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>せっかく農家に転生したので勇者は目指しません</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>マツオカヨシノリ(漫画) 月見里嘉助(原作) ゆーにっと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>路地裏で拾った女の子がバッドエンド後の乙女ゲームのヒロインだった件</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>カボチャマスク(原作) 樋乃えなが(作画) へいろー(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>EP.23①</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>地味子な三葉さんが僕を誘惑する</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>はぶらえる(著者)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第13話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>女子高生の無駄づかい</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>ビーノ(著者)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>ばんがいへん</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第16話 最弱貴族、魔王を拾う(１)</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>塔の管理をしてみよう</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第96話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>セレビィ量産型(著者)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>新年イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>オタクに優しいギャルはいない!?</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>のりしろちゃん 魚住さかな</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>【#173】日常を君と</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>病弱少女、転生して健康な肉体（最強）を手に入れる</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>あらた伊里（漫画） アトハ（原作） 狐印（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第1話　フィアナ、転生して超健康になる</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>賢者の孫</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>緒方俊輔(漫画) 吉岡剛(原作) 菊池政治(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第97話-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>ひとりぼっちの異世界攻略</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>びび（漫画） 五示正司（原作）</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第252話　なぜか不思議と</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>異世界でスローライフを（願望）</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>長頼（漫画） シゲ（原作） オウカ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第58話　激闘！紅い戦線！</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>ディーふらぐ！</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>春野友矢(著者)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第176話</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！</t>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>丈(著者)</t>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！ コミックス14巻情報！！</t>
+          <t>第35話：発動の線引き②</t>
         </is>
       </c>
     </row>
@@ -24495,17 +25537,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>不徳のギルド</t>
+          <t>生徒会にも穴はある！</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>河添太一</t>
+          <t>むちまろ</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第１０２話：大人組</t>
+          <t>第143話	先輩ラブソング♪♪</t>
         </is>
       </c>
     </row>
@@ -24515,17 +25557,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>zunta(作画) はらわたさいぞう(原作)</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第35話：発動の線引き①</t>
+          <t>第７３話『上昇停止』②</t>
         </is>
       </c>
     </row>
@@ -24535,17 +25577,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第７３話『上昇停止』①</t>
+          <t>第45話</t>
         </is>
       </c>
     </row>
@@ -24555,17 +25597,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>王子様の友達</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>すけろく(著者)</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第33話</t>
+          <t>第７１話　いきなり告白の戦いが始まった（１）</t>
         </is>
       </c>
     </row>
@@ -24575,17 +25617,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第43話➁</t>
+          <t>第15話-1</t>
         </is>
       </c>
     </row>
@@ -24595,17 +25637,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+          <t>ダークサモナーとデキている</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+          <t>車王(著者)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第82話その1</t>
+          <t>第84話</t>
         </is>
       </c>
     </row>
@@ -24615,17 +25657,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>このヒーラー、めんどくさい</t>
+          <t>魔のものたちは企てる</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>丹念に発酵(著者)</t>
+          <t>加藤拓弐(原作) ガしガし(作画)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第93話：生け贄</t>
+          <t>第33話</t>
         </is>
       </c>
     </row>
@@ -24635,17 +25677,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>貞操逆転世界で頼めばヤれると噂の俺</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>澄田佑貴(漫画) aaa168（スリーエー）(原作)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第136話　困ってる人がいる限り！</t>
+          <t>第5話</t>
         </is>
       </c>
     </row>
@@ -24655,17 +25697,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>異世界魔王と召喚少女の奴隷魔術</t>
+          <t>淫獄団地</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第132話　王都に戻ってみるⅠ（前編）</t>
+          <t>祝！奇跡の○○○化決定！！！</t>
         </is>
       </c>
     </row>
@@ -24675,17 +25717,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>クセ強彼女は床にいざなう</t>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>須河篤志(著者)</t>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第18話後半</t>
+          <t>第18話前半</t>
         </is>
       </c>
     </row>
@@ -24695,17 +25737,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>【第８巻発売記念】描き下ろしイラスト公開！</t>
+          <t>第137話　まずは一戦！・前編</t>
         </is>
       </c>
     </row>
@@ -24715,17 +25757,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>美人女上司滝沢さん</t>
+          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>やんBARU(著者)</t>
+          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第211話</t>
+          <t>第13話-2</t>
         </is>
       </c>
     </row>
@@ -24735,17 +25777,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>まんきつしたい常連さん</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>しんみりん(著者)</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>特別編</t>
+          <t>第５６話　勇者を蹂躙する器用貧乏（２）</t>
         </is>
       </c>
     </row>
@@ -24755,17 +25797,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
+          <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
+          <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2026年もよろしくお願いいたします</t>
+          <t>第3話前編：魔物狩る少女たち</t>
         </is>
       </c>
     </row>
@@ -24775,17 +25817,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>板垣恵介 猪原賽 陸井栄史</t>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第87話　献上</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -24795,17 +25837,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第77話①</t>
+          <t>第132話　王都に戻ってみるⅠ（中編）</t>
         </is>
       </c>
     </row>
@@ -24815,17 +25857,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>番外編</t>
+          <t>第77話➁</t>
         </is>
       </c>
     </row>
@@ -24835,17 +25877,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第59話①　地下王国ドンゴワに行ってみた</t>
+          <t>第２６食　夜の森の焼きリンゴ、パクパクですわ！（２）</t>
         </is>
       </c>
     </row>
@@ -24855,17 +25897,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>濁る瞳で何を願う ハイセルク戦記</t>
+          <t>田舎で恋は難しい!?</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>トルトネン 創-taro 斎藤八呑</t>
+          <t>ねこうめ(著者)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第36話 意志を持つ天災①</t>
+          <t>3話おまけ</t>
         </is>
       </c>
     </row>
@@ -24875,17 +25917,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
+          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>モリタ Ｕ４ nima</t>
+          <t>夜州 nini 藻</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第14話（６）　春とおぼっちゃまとピクニックランチ（６）</t>
+          <t>第72話(前編)</t>
         </is>
       </c>
     </row>
@@ -24895,17 +25937,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+          <t>剥かせて！竜ケ崎さん</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+          <t>一智和智</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>祝われし休載まんが</t>
+          <t>大学生編 第17話</t>
         </is>
       </c>
     </row>
@@ -24915,17 +25957,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
+          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
+          <t>三部べべ(漫画) ねうしとら(原作)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第42話-2</t>
+          <t>第6話-1</t>
         </is>
       </c>
     </row>
@@ -24935,17 +25977,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第91話　その2</t>
+          <t>第36話 独身貴族は生ハムの原木を買う（1）</t>
         </is>
       </c>
     </row>
@@ -24955,17 +25997,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第４４話　勇者、S級ランクに認定される。弟は、ミカエルとクエストに向かったら、ラファエルが降ってくる（４）</t>
+          <t>第59話②　地下王国ドンゴワに行ってみた</t>
         </is>
       </c>
     </row>
@@ -24975,17 +26017,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>板垣恵介 林たかあき</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第61話 ラストフラワー</t>
+          <t>第146話 よくわからなけれどシビれるみたいです（１）</t>
         </is>
       </c>
     </row>
@@ -24995,17 +26037,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>拷問165</t>
+          <t>第50話 養殖場見学と蜜の酒②</t>
         </is>
       </c>
     </row>
@@ -25015,17 +26057,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第60話　最果ての国を目指して</t>
+          <t>第10話-2：友達と一緒なら</t>
         </is>
       </c>
     </row>
@@ -25035,17 +26077,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>KAKERU</t>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第72話「弓王」（前半）</t>
+          <t>第6話前編</t>
         </is>
       </c>
     </row>
@@ -25055,17 +26097,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>バーサス</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第30話　勇者の意思（1）</t>
+          <t>第43話➁</t>
         </is>
       </c>
     </row>
@@ -25075,17 +26117,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>サーシャちゃんとクラスメイトオタクくん</t>
+          <t>小林さんちのメイドラゴン</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>はぐはぐ(著者)</t>
+          <t>クール教信者</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第91話</t>
+          <t>第158話</t>
         </is>
       </c>
     </row>
@@ -25095,17 +26137,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>漫画/すたひろ 原作/Y.A</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>chapter77【40話②】</t>
+          <t>第91話　その3</t>
         </is>
       </c>
     </row>
@@ -25115,17 +26157,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第76話(後編) 闇市と闇売人と闇取引と</t>
+          <t>第４４話　勇者、S級ランクに認定される。弟は、ミカエルとクエストに向かったら、ラファエルが降ってくる（５）</t>
         </is>
       </c>
     </row>
@@ -25135,17 +26177,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>陰キャの俺が席替えでS級美少女に囲まれたら秘密の関係が始まった。</t>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>星野 星野(原作) バラマツヒトミ(漫画) 黒兎 ゆう(キャラクター原案)</t>
+          <t>六志麻あさ 業務用餅 kisui</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第9話</t>
+          <t>第７９話</t>
         </is>
       </c>
     </row>
@@ -25155,17 +26197,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>英雄女騎士に有能とバレた俺の美人ハーレム騎士団 ガイカク・ヒクメの奇術騎士団</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>明石六郎(原作) 太盛(作画) 氷室しゅんすけ(キャラクター原案)</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第14話-2</t>
+          <t>拷問166</t>
         </is>
       </c>
     </row>
@@ -25175,17 +26217,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+          <t>くらいあの子としたいこと</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+          <t>碇マナツ(著者)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第9話　有月勇のトラウマ（前編）</t>
+          <t>第89話</t>
         </is>
       </c>
     </row>
@@ -25195,17 +26237,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>せっかく農家に転生したので勇者は目指しません</t>
+          <t>俺は星間国家の悪徳領主！</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>マツオカヨシノリ(漫画) 月見里嘉助(原作) ゆーにっと(キャラクター原案)</t>
+          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>第44話　副官</t>
         </is>
       </c>
     </row>
@@ -25215,17 +26257,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>路地裏で拾った女の子がバッドエンド後の乙女ゲームのヒロインだった件</t>
+          <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>カボチャマスク(原作) 樋乃えなが(作画) へいろー(キャラクター原案)</t>
+          <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>休載イラスト</t>
+          <t>第7.5話「あまりちゃんの観覧車タイム」</t>
         </is>
       </c>
     </row>
@@ -25235,17 +26277,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
+          <t>異世界でも無難に生きたい症候群</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
+          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>EP.23①</t>
+          <t>第33話③</t>
         </is>
       </c>
     </row>
@@ -25255,17 +26297,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>地味子な三葉さんが僕を誘惑する</t>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>はぶらえる(著者)</t>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第13話後半</t>
+          <t>第22話①</t>
         </is>
       </c>
     </row>
@@ -25275,17 +26317,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>女子高生の無駄づかい</t>
+          <t>めっちゃ召喚された件 THE COMIC</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ビーノ(著者)</t>
+          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>ばんがいへん</t>
+          <t>第51話②</t>
         </is>
       </c>
     </row>
@@ -25295,17 +26337,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+          <t>モブ司祭だけど、この世界が乙女ゲームだと気づいたのでヒロインを育成します</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>空野進 sorani ファルまろ</t>
+          <t>井冬良(漫画) レオナールＤ(原作) りいちゅ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第16話 最弱貴族、魔王を拾う(１)</t>
+          <t>第5話-2：祝福の時</t>
         </is>
       </c>
     </row>
@@ -25315,17 +26357,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>塔の管理をしてみよう</t>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>盧恩＆雪笠(Friendly Land)(著者) 早秋(原作) 雨神(キャラクター原案)</t>
+          <t>空野進 sorani ファルまろ</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第96話後編</t>
+          <t>第16話 最弱貴族、魔王を拾う(２)</t>
         </is>
       </c>
     </row>
@@ -25335,17 +26377,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>三枝さんはメガネ先輩と恋を描く</t>
+          <t>29歳独身は異世界で自由に生きた……かった。</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>セレビィ量産型(著者)</t>
+          <t>オオハマイコ(漫画) リュート(原作) 桑島黎音(キャラクター原案)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>新年イラスト</t>
+          <t>第43話-1①</t>
         </is>
       </c>
     </row>
@@ -25355,17 +26397,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>オタクに優しいギャルはいない!?</t>
+          <t>魔石グルメ　魔物の力を食べたオレは最強！</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>のりしろちゃん 魚住さかな</t>
+          <t>菅原健二(作画) 結城涼(原作) 成瀬ちさと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>【#173】日常を君と</t>
+          <t>第71話後半</t>
         </is>
       </c>
     </row>
@@ -25375,17 +26417,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>病弱少女、転生して健康な肉体（最強）を手に入れる</t>
+          <t>無職の英雄　別にスキルなんか要らなかったんだが</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>あらた伊里（漫画） アトハ（原作） 狐印（キャラクター原案）</t>
+          <t>原作：九頭七尾・上田夢人 漫画：名苗秋緒</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第1話　フィアナ、転生して超健康になる</t>
+          <t>第53話</t>
         </is>
       </c>
     </row>
@@ -25395,17 +26437,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>賢者の孫</t>
+          <t>絶対死なないステラ姫</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>緒方俊輔(漫画) 吉岡剛(原作) 菊池政治(キャラクター原案)</t>
+          <t>光永康則 大高稲</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第97話-3</t>
+          <t>第１８話　絶対舞踏会に行かない（４）</t>
         </is>
       </c>
     </row>
@@ -25415,17 +26457,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ひとりぼっちの異世界攻略</t>
+          <t>四天王最弱の自立計画（コミック）</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>びび（漫画） 五示正司（原作）</t>
+          <t>漫画／小野ミサオ 原作／西湖三七三 キャラクター原案／ふわり</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第252話　なぜか不思議と</t>
+          <t>第3話(1)</t>
         </is>
       </c>
     </row>
@@ -25435,17 +26477,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>異世界でスローライフを（願望）</t>
+          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>長頼（漫画） シゲ（原作） オウカ（キャラクター原案）</t>
+          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第58話　激闘！紅い戦線！</t>
+          <t>第10話　ダンジョンの主(前編)</t>
         </is>
       </c>
     </row>
@@ -25455,17 +26497,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ディーふらぐ！</t>
+          <t>ガチャを回して仲間を増やす 最強の美少女軍団を作り上げろ</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>春野友矢(著者)</t>
+          <t>漫画：晴野しゅー 原作：ちんくるり キャラクター原案：イセ川ヤスタカ</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第176話</t>
+          <t>第76話前半</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2026-01-26
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -38,6 +38,7 @@
     <sheet name="2026-01-05" sheetId="30" state="visible" r:id="rId30"/>
     <sheet name="2026-01-12" sheetId="31" state="visible" r:id="rId31"/>
     <sheet name="2026-01-19" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="2026-01-26" sheetId="33" state="visible" r:id="rId33"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -25512,22 +25513,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第35話：発動の線引き②</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第143話	先輩ラブソング♪♪</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第７３話『上昇停止』②</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第45話</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第７１話　いきなり告白の戦いが始まった（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第15話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>ダークサモナーとデキている</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>車王(著者)</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第84話</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>魔のものたちは企てる</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>加藤拓弐(原作) ガしガし(作画)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第33話</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>貞操逆転世界で頼めばヤれると噂の俺</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>澄田佑貴(漫画) aaa168（スリーエー）(原作)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>祝！奇跡の○○○化決定！！！</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第18話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第137話　まずは一戦！・前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第13話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第５６話　勇者を蹂躙する器用貧乏（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第3話前編：魔物狩る少女たち</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第132話　王都に戻ってみるⅠ（中編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第77話➁</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第２６食　夜の森の焼きリンゴ、パクパクですわ！（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>田舎で恋は難しい!?</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>ねこうめ(著者)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>3話おまけ</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>夜州 nini 藻</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第72話(前編)</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>剥かせて！竜ケ崎さん</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>一智和智</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>大学生編 第17話</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>三部べべ(漫画) ねうしとら(原作)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第6話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第36話 独身貴族は生ハムの原木を買う（1）</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第59話②　地下王国ドンゴワに行ってみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第146話 よくわからなけれどシビれるみたいです（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第50話 養殖場見学と蜜の酒②</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第10話-2：友達と一緒なら</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第6話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第43話➁</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>小林さんちのメイドラゴン</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>クール教信者</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第158話</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第91話　その3</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第４４話　勇者、S級ランクに認定される。弟は、ミカエルとクエストに向かったら、ラファエルが降ってくる（５）</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>六志麻あさ 業務用餅 kisui</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第７９話</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>拷問166</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第89話</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>俺は星間国家の悪徳領主！</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第44話　副官</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第7.5話「あまりちゃんの観覧車タイム」</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>異世界でも無難に生きたい症候群</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第33話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第22話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>めっちゃ召喚された件 THE COMIC</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第51話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>モブ司祭だけど、この世界が乙女ゲームだと気づいたのでヒロインを育成します</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>井冬良(漫画) レオナールＤ(原作) りいちゅ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第5話-2：祝福の時</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第16話 最弱貴族、魔王を拾う(２)</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>29歳独身は異世界で自由に生きた……かった。</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>オオハマイコ(漫画) リュート(原作) 桑島黎音(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第43話-1①</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>魔石グルメ　魔物の力を食べたオレは最強！</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>菅原健二(作画) 結城涼(原作) 成瀬ちさと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第71話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>無職の英雄　別にスキルなんか要らなかったんだが</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>原作：九頭七尾・上田夢人 漫画：名苗秋緒</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第53話</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>絶対死なないステラ姫</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>光永康則 大高稲</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第１８話　絶対舞踏会に行かない（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>四天王最弱の自立計画（コミック）</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>漫画／小野ミサオ 原作／西湖三七三 キャラクター原案／ふわり</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第3話(1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第10話　ダンジョンの主(前編)</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>ガチャを回して仲間を増やす 最強の美少女軍団を作り上げろ</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>漫画：晴野しゅー 原作：ちんくるり キャラクター原案：イセ川ヤスタカ</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第76話前半</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+          <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>zunta(作画) はらわたさいぞう(原作)</t>
+          <t>丈(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第35話：発動の線引き②</t>
+          <t>第130話</t>
         </is>
       </c>
     </row>
@@ -25537,17 +26579,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>生徒会にも穴はある！</t>
+          <t>転生したらスライムだった件</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>むちまろ</t>
+          <t>原作：伏瀬 漫画：川上泰樹 キャラクター原案：みっつばー</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第143話	先輩ラブソング♪♪</t>
+          <t>★描き下ろし色紙プレゼントのお知らせ★</t>
         </is>
       </c>
     </row>
@@ -25557,17 +26599,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第７３話『上昇停止』②</t>
+          <t>219撃目</t>
         </is>
       </c>
     </row>
@@ -25577,17 +26619,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>異世界おじさん</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第45話</t>
+          <t>番外編10</t>
         </is>
       </c>
     </row>
@@ -25597,17 +26639,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第７１話　いきなり告白の戦いが始まった（１）</t>
+          <t>第75話</t>
         </is>
       </c>
     </row>
@@ -25617,17 +26659,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第15話-1</t>
+          <t>第35話：発動の線引き③</t>
         </is>
       </c>
     </row>
@@ -25637,17 +26679,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ダークサモナーとデキている</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>車王(著者)</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第84話</t>
+          <t>第７３話『上昇停止』③</t>
         </is>
       </c>
     </row>
@@ -25657,17 +26699,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>魔のものたちは企てる</t>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>加藤拓弐(原作) ガしガし(作画)</t>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第33話</t>
+          <t>第7話 前編</t>
         </is>
       </c>
     </row>
@@ -25677,17 +26719,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>貞操逆転世界で頼めばヤれると噂の俺</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>澄田佑貴(漫画) aaa168（スリーエー）(原作)</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第5話</t>
+          <t>第７１話　いきなり告白の戦いが始まった（２）</t>
         </is>
       </c>
     </row>
@@ -25697,17 +26739,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>淫獄団地</t>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>祝！奇跡の○○○化決定！！！</t>
+          <t>第82話その2</t>
         </is>
       </c>
     </row>
@@ -25727,7 +26769,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第18話前半</t>
+          <t>第18話後半</t>
         </is>
       </c>
     </row>
@@ -25737,17 +26779,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第137話　まずは一戦！・前編</t>
+          <t>第５６話　勇者を蹂躙する器用貧乏（３）</t>
         </is>
       </c>
     </row>
@@ -25757,17 +26799,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第13話-2</t>
+          <t>第137話　まずは一戦！・後編</t>
         </is>
       </c>
     </row>
@@ -25777,17 +26819,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第５６話　勇者を蹂躙する器用貧乏（２）</t>
+          <t>第35話</t>
         </is>
       </c>
     </row>
@@ -25797,17 +26839,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第3話前編：魔物狩る少女たち</t>
+          <t>第132話　王都に戻ってみるⅠ（後編）</t>
         </is>
       </c>
     </row>
@@ -25817,17 +26859,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>女友達は頼めば意外とヤらせてくれる</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ろくろ(漫画) 鏡遊(原作)</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第28話</t>
+          <t>第52話後編</t>
         </is>
       </c>
     </row>
@@ -25837,17 +26879,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>異世界魔王と召喚少女の奴隷魔術</t>
+          <t>異世界のんびり農家</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第132話　王都に戻ってみるⅠ（中編）</t>
+          <t>第315話</t>
         </is>
       </c>
     </row>
@@ -25857,17 +26899,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第77話➁</t>
+          <t>第88話　種</t>
         </is>
       </c>
     </row>
@@ -25877,17 +26919,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+          <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>島知宏 音速炒飯 有都あらゆる</t>
+          <t>須河篤志(著者)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第２６食　夜の森の焼きリンゴ、パクパクですわ！（２）</t>
+          <t>休載イラスト</t>
         </is>
       </c>
     </row>
@@ -25897,17 +26939,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>田舎で恋は難しい!?</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ねこうめ(著者)</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>3話おまけ</t>
+          <t>第15話</t>
         </is>
       </c>
     </row>
@@ -25917,17 +26959,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>夜州 nini 藻</t>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第72話(前編)</t>
+          <t>第２６食　夜の森の焼きリンゴ、パクパクですわ！（３）</t>
         </is>
       </c>
     </row>
@@ -25937,17 +26979,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>剥かせて！竜ケ崎さん</t>
+          <t>おとなりのダウナーさんは無理させない</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>一智和智</t>
+          <t>瑠璃いろ(著者)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>大学生編 第17話</t>
+          <t>第14話</t>
         </is>
       </c>
     </row>
@@ -25957,17 +26999,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>三部べべ(漫画) ねうしとら(原作)</t>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第6話-1</t>
+          <t>第36話 独身貴族は生ハムの原木を買う（2）</t>
         </is>
       </c>
     </row>
@@ -25977,17 +27019,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第36話 独身貴族は生ハムの原木を買う（1）</t>
+          <t>第77話③</t>
         </is>
       </c>
     </row>
@@ -25997,17 +27039,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第59話②　地下王国ドンゴワに行ってみた</t>
+          <t>第45話　奴は巡る（前編）</t>
         </is>
       </c>
     </row>
@@ -26017,17 +27059,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第146話 よくわからなけれどシビれるみたいです（１）</t>
+          <t>第60話①　ニコニ坑道の異変を調べてみた</t>
         </is>
       </c>
     </row>
@@ -26037,17 +27079,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第50話 養殖場見学と蜜の酒②</t>
+          <t>第146話 よくわからなけれどシビれるみたいです（２）</t>
         </is>
       </c>
     </row>
@@ -26057,17 +27099,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+          <t>濁る瞳で何を願う ハイセルク戦記</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+          <t>トルトネン 創-taro 斎藤八呑</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第10話-2：友達と一緒なら</t>
+          <t>第37話　意思を持つ天災②</t>
         </is>
       </c>
     </row>
@@ -26077,17 +27119,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+          <t>三吉汐美(著者)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第6話前編</t>
+          <t>第20話前半</t>
         </is>
       </c>
     </row>
@@ -26097,17 +27139,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第43話➁</t>
+          <t>第91話　その4</t>
         </is>
       </c>
     </row>
@@ -26117,17 +27159,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>小林さんちのメイドラゴン</t>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>クール教信者</t>
+          <t>板垣恵介 林たかあき</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第158話</t>
+          <t>第62話 勝利への執着</t>
         </is>
       </c>
     </row>
@@ -26137,17 +27179,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第91話　その3</t>
+          <t>拷問167</t>
         </is>
       </c>
     </row>
@@ -26157,17 +27199,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>Lv２からチートだった元勇者候補のまったり異世界ライフ</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>糸町秋音（漫画） 鬼ノ城ミヤ（原作） 片桐（キャラクター原案）</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第４４話　勇者、S級ランクに認定される。弟は、ミカエルとクエストに向かったら、ラファエルが降ってくる（５）</t>
+          <t>第65話　はじめての</t>
         </is>
       </c>
     </row>
@@ -26177,17 +27219,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>六志麻あさ 業務用餅 kisui</t>
+          <t>KAKERU</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第７９話</t>
+          <t>第72話「弓王」（後半）</t>
         </is>
       </c>
     </row>
@@ -26197,17 +27239,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>世界最強の後衛 ～迷宮国の新人探索者～</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>力蔵(著者) とーわ(原作) 風花風花(キャラクター原案)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>拷問166</t>
+          <t>第41話-3</t>
         </is>
       </c>
     </row>
@@ -26217,17 +27259,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>くらいあの子としたいこと</t>
+          <t>バーサス</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>碇マナツ(著者)</t>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第89話</t>
+          <t>第30話　勇者の意思（2）</t>
         </is>
       </c>
     </row>
@@ -26237,17 +27279,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>俺は星間国家の悪徳領主！</t>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
+          <t>FUNA 東西 モトエ恵介</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第44話　副官</t>
+          <t>第126話　襲撃［その５］</t>
         </is>
       </c>
     </row>
@@ -26257,17 +27299,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
+          <t>回復術士のやり直し</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
+          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第7.5話「あまりちゃんの観覧車タイム」</t>
+          <t>第75話-3</t>
         </is>
       </c>
     </row>
@@ -26277,17 +27319,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>異世界でも無難に生きたい症候群</t>
+          <t>最果てのパラディン</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
+          <t>奥橋睦（漫画） 柳野かなた（原作） 輪くすさが（キャラクター原案）</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第33話③</t>
+          <t>第69話　無敵の巨人Ⅱ</t>
         </is>
       </c>
     </row>
@@ -26297,17 +27339,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>漫画/すたひろ 原作/Y.A</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第22話①</t>
+          <t>chapter78【41話①】</t>
         </is>
       </c>
     </row>
@@ -26317,17 +27359,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>めっちゃ召喚された件 THE COMIC</t>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第51話②</t>
+          <t>第9話　有月勇のトラウマ（後編）</t>
         </is>
       </c>
     </row>
@@ -26337,17 +27379,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>モブ司祭だけど、この世界が乙女ゲームだと気づいたのでヒロインを育成します</t>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>井冬良(漫画) レオナールＤ(原作) りいちゅ(キャラクター原案)</t>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第5話-2：祝福の時</t>
+          <t>第37話</t>
         </is>
       </c>
     </row>
@@ -26357,17 +27399,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>空野進 sorani ファルまろ</t>
+          <t>はぐはぐ(著者)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第16話 最弱貴族、魔王を拾う(２)</t>
+          <t>第92話</t>
         </is>
       </c>
     </row>
@@ -26377,17 +27419,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>29歳独身は異世界で自由に生きた……かった。</t>
+          <t>ライブダンジョン！</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>オオハマイコ(漫画) リュート(原作) 桑島黎音(キャラクター原案)</t>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第43話-1①</t>
+          <t>第93話前半</t>
         </is>
       </c>
     </row>
@@ -26397,17 +27439,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>魔石グルメ　魔物の力を食べたオレは最強！</t>
+          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>菅原健二(作画) 結城涼(原作) 成瀬ちさと(キャラクター原案)</t>
+          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第71話後半</t>
+          <t>第86話前半</t>
         </is>
       </c>
     </row>
@@ -26417,17 +27459,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>無職の英雄　別にスキルなんか要らなかったんだが</t>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>原作：九頭七尾・上田夢人 漫画：名苗秋緒</t>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第53話</t>
+          <t>第77話(前編) レッツ闇鍋パーティー！</t>
         </is>
       </c>
     </row>
@@ -26437,17 +27479,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>絶対死なないステラ姫</t>
+          <t>黄金の経験値</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>光永康則 大高稲</t>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第１８話　絶対舞踏会に行かない（４）</t>
+          <t>第22話（前編）</t>
         </is>
       </c>
     </row>
@@ -26457,17 +27499,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>四天王最弱の自立計画（コミック）</t>
+          <t>女子高生の無駄づかい</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>漫画／小野ミサオ 原作／西湖三七三 キャラクター原案／ふわり</t>
+          <t>ビーノ(著者)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第3話(1)</t>
+          <t>第140話　かいかく</t>
         </is>
       </c>
     </row>
@@ -26477,17 +27519,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
+          <t>空野進 sorani ファルまろ</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第10話　ダンジョンの主(前編)</t>
+          <t>第16話 最弱貴族、魔王を拾う(３)</t>
         </is>
       </c>
     </row>
@@ -26497,17 +27539,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ガチャを回して仲間を増やす 最強の美少女軍団を作り上げろ</t>
+          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>漫画：晴野しゅー 原作：ちんくるり キャラクター原案：イセ川ヤスタカ</t>
+          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第76話前半</t>
+          <t>最終話-1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2026-02-02
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -39,6 +39,7 @@
     <sheet name="2026-01-12" sheetId="31" state="visible" r:id="rId31"/>
     <sheet name="2026-01-19" sheetId="32" state="visible" r:id="rId32"/>
     <sheet name="2026-01-26" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="2026-02-02" sheetId="34" state="visible" r:id="rId34"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -26554,22 +26555,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第130話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>転生したらスライムだった件</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>原作：伏瀬 漫画：川上泰樹 キャラクター原案：みっつばー</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>★描き下ろし色紙プレゼントのお知らせ★</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>ワンパンマン</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>219撃目</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>番外編10</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第75話</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第35話：発動の線引き③</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第７３話『上昇停止』③</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第7話 前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第７１話　いきなり告白の戦いが始まった（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第82話その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第18話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第５６話　勇者を蹂躙する器用貧乏（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第137話　まずは一戦！・後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第35話</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第132話　王都に戻ってみるⅠ（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>まんきつしたい常連さん</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>しんみりん(著者)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第52話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第315話</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第88話　種</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>クセ強彼女は床にいざなう</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>須河篤志(著者)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第15話</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第２６食　夜の森の焼きリンゴ、パクパクですわ！（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>おとなりのダウナーさんは無理させない</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>瑠璃いろ(著者)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第14話</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第36話 独身貴族は生ハムの原木を買う（2）</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第77話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第45話　奴は巡る（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第60話①　ニコニ坑道の異変を調べてみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第146話 よくわからなけれどシビれるみたいです（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>濁る瞳で何を願う ハイセルク戦記</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>トルトネン 創-taro 斎藤八呑</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第37話　意思を持つ天災②</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>三吉汐美(著者)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第20話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第91話　その4</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 林たかあき</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第62話 勝利への執着</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>拷問167</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>Lv２からチートだった元勇者候補のまったり異世界ライフ</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>糸町秋音（漫画） 鬼ノ城ミヤ（原作） 片桐（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第65話　はじめての</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>KAKERU</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第72話「弓王」（後半）</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の後衛 ～迷宮国の新人探索者～</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>力蔵(著者) とーわ(原作) 風花風花(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第41話-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>バーサス</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第30話　勇者の意思（2）</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>FUNA 東西 モトエ恵介</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第126話　襲撃［その５］</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>回復術士のやり直し</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第75話-3</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>最果てのパラディン</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>奥橋睦（漫画） 柳野かなた（原作） 輪くすさが（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第69話　無敵の巨人Ⅱ</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>漫画/すたひろ 原作/Y.A</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>chapter78【41話①】</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第9話　有月勇のトラウマ（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第37話</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>はぐはぐ(著者)</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第92話</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>ライブダンジョン！</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第93話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第86話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第77話(前編) レッツ闇鍋パーティー！</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>黄金の経験値</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第22話（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>女子高生の無駄づかい</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>ビーノ(著者)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第140話　かいかく</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>空野進 sorani ファルまろ</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第16話 最弱貴族、魔王を拾う(３)</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>最終話-1</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！</t>
+          <t>転生したらスライムだった件</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>丈(著者)</t>
+          <t>原作：伏瀬 漫画：川上泰樹 キャラクター原案：みっつばー</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第130話</t>
+          <t>第130話　最後に笑う者</t>
         </is>
       </c>
     </row>
@@ -26579,17 +27621,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>転生したらスライムだった件</t>
+          <t>異世界おじさん</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>原作：伏瀬 漫画：川上泰樹 キャラクター原案：みっつばー</t>
+          <t>殆ど死んでいる(著者)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>★描き下ろし色紙プレゼントのお知らせ★</t>
+          <t>番外編11</t>
         </is>
       </c>
     </row>
@@ -26599,17 +27641,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ワンパンマン</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>原作/ＯＮＥ 作画/村田雄介</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>219撃目</t>
+          <t>第44話①</t>
         </is>
       </c>
     </row>
@@ -26619,17 +27661,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>番外編10</t>
+          <t>第20話-2「パーフェクトB級冒険者」</t>
         </is>
       </c>
     </row>
@@ -26639,17 +27681,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>新米オッサン冒険者、最強パーティに死ぬほど鍛えられて無敵になる</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>漫画：荻野ケン 原作：岸馬きらく キャラクター原案：Tea</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第75話</t>
+          <t>★描き下ろし色紙プレゼントのお知らせ★</t>
         </is>
       </c>
     </row>
@@ -26659,17 +27701,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+          <t>生徒会にも穴はある！</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>zunta(作画) はらわたさいぞう(原作)</t>
+          <t>むちまろ</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第35話：発動の線引き③</t>
+          <t>第144話	ヒステリックミステリック</t>
         </is>
       </c>
     </row>
@@ -26679,17 +27721,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第７３話『上昇停止』③</t>
+          <t>★描き下ろし色紙プレゼントのお知らせ★</t>
         </is>
       </c>
     </row>
@@ -26699,17 +27741,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+          <t>異世界居酒屋「のぶ」</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第7話 前編</t>
+          <t>第129話</t>
         </is>
       </c>
     </row>
@@ -26719,17 +27761,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第７１話　いきなり告白の戦いが始まった（２）</t>
+          <t>第38話①</t>
         </is>
       </c>
     </row>
@@ -26739,17 +27781,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第82話その2</t>
+          <t>第45.5話</t>
         </is>
       </c>
     </row>
@@ -26759,17 +27801,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第18話後半</t>
+          <t>第15話-2</t>
         </is>
       </c>
     </row>
@@ -26779,17 +27821,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>帰ってください！ 阿久津さん</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>長岡太一(著者)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第５６話　勇者を蹂躙する器用貧乏（３）</t>
+          <t>第201話</t>
         </is>
       </c>
     </row>
@@ -26799,17 +27841,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>久遠まこと(著者) 石のやっさん(原作)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第137話　まずは一戦！・後編</t>
+          <t>第34話</t>
         </is>
       </c>
     </row>
@@ -26819,17 +27861,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
+          <t>ダークサモナーとデキている</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
+          <t>車王(著者)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第35話</t>
+          <t>第84.5話</t>
         </is>
       </c>
     </row>
@@ -26839,17 +27881,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>異世界魔王と召喚少女の奴隷魔術</t>
+          <t>不純な彼女達は懺悔しない</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+          <t>ポロロッカ(著者)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第132話　王都に戻ってみるⅠ（後編）</t>
+          <t>第34話</t>
         </is>
       </c>
     </row>
@@ -26859,17 +27901,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>まんきつしたい常連さん</t>
+          <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>しんみりん(著者)</t>
+          <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第52話後編</t>
+          <t>第3話後編：魔物狩る少女たち</t>
         </is>
       </c>
     </row>
@@ -26879,17 +27921,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>異世界のんびり農家</t>
+          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+          <t>三部べべ(漫画) ねうしとら(原作)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第315話</t>
+          <t>第6話-2</t>
         </is>
       </c>
     </row>
@@ -26899,17 +27941,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>板垣恵介 猪原賽 陸井栄史</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第88話　種</t>
+          <t>おまけ69</t>
         </is>
       </c>
     </row>
@@ -26919,17 +27961,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>クセ強彼女は床にいざなう</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>須河篤志(著者)</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>休載イラスト</t>
+          <t>第５６話　勇者を蹂躙する器用貧乏（４）</t>
         </is>
       </c>
     </row>
@@ -26939,17 +27981,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>異世界のんびり農家</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第15話</t>
+          <t>第316話</t>
         </is>
       </c>
     </row>
@@ -26959,17 +28001,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+          <t>「おかえり、パパ」</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>島知宏 音速炒飯 有都あらゆる</t>
+          <t>蝉丸</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第２６食　夜の森の焼きリンゴ、パクパクですわ！（３）</t>
+          <t>第32話　接触</t>
         </is>
       </c>
     </row>
@@ -26979,17 +28021,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>おとなりのダウナーさんは無理させない</t>
+          <t>せっかく農家に転生したので勇者は目指しません</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>瑠璃いろ(著者)</t>
+          <t>マツオカヨシノリ(漫画) 月見里嘉助(原作) ゆーにっと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第14話</t>
+          <t>第2話③</t>
         </is>
       </c>
     </row>
@@ -26999,17 +28041,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>丈(著者)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第36話 独身貴族は生ハムの原木を買う（2）</t>
+          <t>第130話</t>
         </is>
       </c>
     </row>
@@ -27019,17 +28061,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第77話③</t>
+          <t>第36話 独身貴族は生ハムの原木を買う（3）</t>
         </is>
       </c>
     </row>
@@ -27039,17 +28081,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+          <t>物語の黒幕に転生して</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第45話　奴は巡る（前編）</t>
+          <t>第38話</t>
         </is>
       </c>
     </row>
@@ -27059,17 +28101,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第60話①　ニコニ坑道の異変を調べてみた</t>
+          <t>第２７食　コカトリスのフライドチキン、パクパクですわ！（１）</t>
         </is>
       </c>
     </row>
@@ -27079,17 +28121,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>アザミヤコを好きになる</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第146話 よくわからなけれどシビれるみたいです（２）</t>
+          <t>第13話前編</t>
         </is>
       </c>
     </row>
@@ -27099,17 +28141,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>濁る瞳で何を願う ハイセルク戦記</t>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>トルトネン 創-taro 斎藤八呑</t>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第37話　意思を持つ天災②</t>
+          <t>第6話後編</t>
         </is>
       </c>
     </row>
@@ -27119,17 +28161,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>アイドル辞めるけど結婚してくれますか!?</t>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>三吉汐美(著者)</t>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第20話前半</t>
+          <t>第50話 養殖場見学と蜜の酒③</t>
         </is>
       </c>
     </row>
@@ -27139,17 +28181,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第91話　その4</t>
+          <t>第147話 よくわからないけれど滾るみたいです（１）</t>
         </is>
       </c>
     </row>
@@ -27159,17 +28201,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>板垣恵介 林たかあき</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第62話 勝利への執着</t>
+          <t>第60話②　ニコニ坑道の異変を調べてみた</t>
         </is>
       </c>
     </row>
@@ -27179,17 +28221,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>拷問167</t>
+          <t>第11話-1：普通の高校生</t>
         </is>
       </c>
     </row>
@@ -27199,17 +28241,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Lv２からチートだった元勇者候補のまったり異世界ライフ</t>
+          <t>田舎で恋は難しい!?</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>糸町秋音（漫画） 鬼ノ城ミヤ（原作） 片桐（キャラクター原案）</t>
+          <t>ねこうめ(著者)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第65話　はじめての</t>
+          <t>許嫁の合歓園寧寧に着てほしいコスプレ大募集!!!!【コメント企画】</t>
         </is>
       </c>
     </row>
@@ -27219,17 +28261,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+          <t>美人女上司滝沢さん</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>KAKERU</t>
+          <t>やんBARU(著者)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第72話「弓王」（後半）</t>
+          <t>第212話</t>
         </is>
       </c>
     </row>
@@ -27239,17 +28281,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>世界最強の後衛 ～迷宮国の新人探索者～</t>
+          <t>幼女戦記</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>力蔵(著者) とーわ(原作) 風花風花(キャラクター原案)</t>
+          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第41話-3</t>
+          <t>第百十二章：ドードーバード航空戦Ⅶ</t>
         </is>
       </c>
     </row>
@@ -27259,17 +28301,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>バーサス</t>
+          <t>異世界食堂　洋食のねこや</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第30話　勇者の意思（2）</t>
+          <t>第44話➁</t>
         </is>
       </c>
     </row>
@@ -27279,17 +28321,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>FUNA 東西 モトエ恵介</t>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第126話　襲撃［その５］</t>
+          <t>第28話</t>
         </is>
       </c>
     </row>
@@ -27299,17 +28341,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>回復術士のやり直し</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>月夜涙(原作) 羽賀ソウケン(漫画) しおこんぶ(キャラクター原案)</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第75話-3</t>
+          <t>第85話その1</t>
         </is>
       </c>
     </row>
@@ -27319,17 +28361,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>最果てのパラディン</t>
+          <t>衛宮さんちの今日のごはん</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>奥橋睦（漫画） 柳野かなた（原作） 輪くすさが（キャラクター原案）</t>
+          <t>TAa(漫画) 只野まこと(料理監修) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第69話　無敵の巨人Ⅱ</t>
+          <t>第78話</t>
         </is>
       </c>
     </row>
@@ -27339,17 +28381,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
+          <t>理想のヒモ生活</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>漫画/すたひろ 原作/Y.A</t>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>chapter78【41話①】</t>
+          <t>第104話　その2</t>
         </is>
       </c>
     </row>
@@ -27359,17 +28401,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>10年ぶりに再会したクソガキは清純美少女JKに成長していた</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>緑青黒羽（漫画） 館西夕木（原作） ひげ猫（キャラクター原案）</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第9話　有月勇のトラウマ（後編）</t>
+          <t>拷問168</t>
         </is>
       </c>
     </row>
@@ -27379,17 +28421,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
+          <t>くらいあの子としたいこと</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
+          <t>碇マナツ(著者)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第37話</t>
+          <t>第90話</t>
         </is>
       </c>
     </row>
@@ -27399,17 +28441,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>サーシャちゃんとクラスメイトオタクくん</t>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>はぐはぐ(著者)</t>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第92話</t>
+          <t>第22話②</t>
         </is>
       </c>
     </row>
@@ -27419,17 +28461,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ライブダンジョン！</t>
+          <t>異世界でも無難に生きたい症候群</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第93話前半</t>
+          <t>第33話④</t>
         </is>
       </c>
     </row>
@@ -27439,17 +28481,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+          <t>めっちゃ召喚された件 THE COMIC</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第86話前半</t>
+          <t>第52話①</t>
         </is>
       </c>
     </row>
@@ -27459,17 +28501,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>解雇された暗黒兵士(30代)のスローなセカンドライフ</t>
+          <t>地味子な三葉さんが僕を誘惑する</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>岡沢六十四 るれくちぇ sage・ジョー</t>
+          <t>はぶらえる(著者)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第77話(前編) レッツ闇鍋パーティー！</t>
+          <t>コミックス告知</t>
         </is>
       </c>
     </row>
@@ -27479,17 +28521,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>黄金の経験値</t>
+          <t>世界最高の暗殺者、異世界貴族に転生する</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+          <t>月夜涙(原作) 皇ハマオ(漫画) れい亜(キャラクター原案)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第22話（前編）</t>
+          <t>第41話-2</t>
         </is>
       </c>
     </row>
@@ -27499,17 +28541,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>女子高生の無駄づかい</t>
+          <t>病弱少女、転生して健康な肉体（最強）を手に入れる</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ビーノ(著者)</t>
+          <t>あらた伊里（漫画） アトハ（原作） 狐印（キャラクター原案）</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第140話　かいかく</t>
+          <t>第2話　フィアナ、模擬戦に挑む（後編）</t>
         </is>
       </c>
     </row>
@@ -27519,17 +28561,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
+          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>空野進 sorani ファルまろ</t>
+          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第16話 最弱貴族、魔王を拾う(３)</t>
+          <t>第10話　ダンジョンの主(後編)</t>
         </is>
       </c>
     </row>
@@ -27539,17 +28581,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>俺以外誰も採取できない素材なのに「素材採取率が低い」とパワハラする幼馴染錬金術師と絶縁した専属魔導士、辺境の町でスローライフを送りたい。</t>
+          <t>ひとりぼっちの異世界攻略</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>狐御前(原作) 西岡知三(作画) ＮＯＣＯ(キャラクター原案)</t>
+          <t>びび（漫画） 五示正司（原作）</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>最終話-1</t>
+          <t>第255話　複雑な家庭環境…？</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2026-02-09
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -40,6 +40,7 @@
     <sheet name="2026-01-19" sheetId="32" state="visible" r:id="rId32"/>
     <sheet name="2026-01-26" sheetId="33" state="visible" r:id="rId33"/>
     <sheet name="2026-02-02" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="2026-02-09" sheetId="35" state="visible" r:id="rId35"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -27596,22 +27597,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>転生したらスライムだった件</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>原作：伏瀬 漫画：川上泰樹 キャラクター原案：みっつばー</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第130話　最後に笑う者</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>異世界おじさん</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>殆ど死んでいる(著者)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>番外編11</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第44話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第20話-2「パーフェクトB級冒険者」</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>★描き下ろし色紙プレゼントのお知らせ★</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第144話	ヒステリックミステリック</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>★描き下ろし色紙プレゼントのお知らせ★</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>異世界居酒屋「のぶ」</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第129話</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第38話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第45.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第15話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>帰ってください！ 阿久津さん</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>長岡太一(著者)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第201話</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>久遠まこと(著者) 石のやっさん(原作)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第34話</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>ダークサモナーとデキている</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>車王(著者)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第84.5話</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>不純な彼女達は懺悔しない</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>ポロロッカ(著者)</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第34話</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第3話後編：魔物狩る少女たち</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>三部べべ(漫画) ねうしとら(原作)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第6話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>おまけ69</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第５６話　勇者を蹂躙する器用貧乏（４）</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>異世界のんびり農家</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第316話</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>「おかえり、パパ」</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>蝉丸</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第32話　接触</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>せっかく農家に転生したので勇者は目指しません</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>マツオカヨシノリ(漫画) 月見里嘉助(原作) ゆーにっと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第2話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第130話</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第36話 独身貴族は生ハムの原木を買う（3）</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>物語の黒幕に転生して</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第38話</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第２７食　コカトリスのフライドチキン、パクパクですわ！（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>アザミヤコを好きになる</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第13話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第6話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第50話 養殖場見学と蜜の酒③</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第147話 よくわからないけれど滾るみたいです（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第60話②　ニコニ坑道の異変を調べてみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第11話-1：普通の高校生</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>田舎で恋は難しい!?</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>ねこうめ(著者)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>許嫁の合歓園寧寧に着てほしいコスプレ大募集!!!!【コメント企画】</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>美人女上司滝沢さん</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>やんBARU(著者)</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第212話</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>幼女戦記</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第百十二章：ドードーバード航空戦Ⅶ</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>異世界食堂　洋食のねこや</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第44話➁</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第28話</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第85話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>衛宮さんちの今日のごはん</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>TAa(漫画) 只野まこと(料理監修) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第78話</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>理想のヒモ生活</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第104話　その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>拷問168</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>第90話</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第22話②</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>異世界でも無難に生きたい症候群</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第33話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>めっちゃ召喚された件 THE COMIC</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第52話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>地味子な三葉さんが僕を誘惑する</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>はぶらえる(著者)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>コミックス告知</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>世界最高の暗殺者、異世界貴族に転生する</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>月夜涙(原作) 皇ハマオ(漫画) れい亜(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第41話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>病弱少女、転生して健康な肉体（最強）を手に入れる</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>あらた伊里（漫画） アトハ（原作） 狐印（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第2話　フィアナ、模擬戦に挑む（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第10話　ダンジョンの主(後編)</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>ひとりぼっちの異世界攻略</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>びび（漫画） 五示正司（原作）</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第255話　複雑な家庭環境…？</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>転生したらスライムだった件</t>
+          <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>原作：伏瀬 漫画：川上泰樹 キャラクター原案：みっつばー</t>
+          <t>丈(著者)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第130話　最後に笑う者</t>
+          <t>第131話</t>
         </is>
       </c>
     </row>
@@ -27621,17 +28663,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>異世界おじさん</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>殆ど死んでいる(著者)</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>番外編11</t>
+          <t>220撃目</t>
         </is>
       </c>
     </row>
@@ -27641,17 +28683,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>転生したらスライムだった件</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>原作：伏瀬 漫画：川上泰樹 キャラクター原案：みっつばー</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第44話①</t>
+          <t>第132話　視察と研究成果</t>
         </is>
       </c>
     </row>
@@ -27661,17 +28703,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第20話-2「パーフェクトB級冒険者」</t>
+          <t>第36話：クソガキ①</t>
         </is>
       </c>
     </row>
@@ -27681,17 +28723,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>魔王の俺が奴隷エルフを嫁にしたんだが、どう愛でればいい？</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>原作／手島史詞 キャラクター原案／COMTA 漫画／板垣ハコ</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>★描き下ろし色紙プレゼントのお知らせ★</t>
+          <t>第76話</t>
         </is>
       </c>
     </row>
@@ -27701,17 +28743,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>生徒会にも穴はある！</t>
+          <t>蜘蛛ですが、なにか？</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>むちまろ</t>
+          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第144話	ヒステリックミステリック</t>
+          <t>第78話その1</t>
         </is>
       </c>
     </row>
@@ -27721,17 +28763,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>★描き下ろし色紙プレゼントのお知らせ★</t>
+          <t>第７４話『半球停止』⓵</t>
         </is>
       </c>
     </row>
@@ -27741,17 +28783,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>異世界居酒屋「のぶ」</t>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>蝉川夏哉(原作) ヴァージニア二等兵(漫画) 転(キャラクター原案)</t>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第129話</t>
+          <t>第7話 後編</t>
         </is>
       </c>
     </row>
@@ -27761,17 +28803,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>クラスで２番目に可愛い女の子と友だちになった</t>
+          <t>王子様の友達</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
+          <t>すけろく(著者)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第38話①</t>
+          <t>第34話</t>
         </is>
       </c>
     </row>
@@ -27781,17 +28823,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第45.5話</t>
+          <t>第７３話　合評の戦いが始まった（１）</t>
         </is>
       </c>
     </row>
@@ -27801,17 +28843,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+          <t>立ち飲み居酒屋でクーデレダウナー系女子大生が隣に来る話</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+          <t>原作:剃り残し 漫画:大窪太一</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第15話-2</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -27821,17 +28863,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>帰ってください！ 阿久津さん</t>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>長岡太一(著者)</t>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第201話</t>
+          <t>第83話その1</t>
         </is>
       </c>
     </row>
@@ -27841,17 +28883,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>勇者に全部奪われた俺は勇者の母親とパーティを組みました！</t>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>久遠まこと(著者) 石のやっさん(原作)</t>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第34話</t>
+          <t>第29話①</t>
         </is>
       </c>
     </row>
@@ -27861,17 +28903,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ダークサモナーとデキている</t>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>車王(著者)</t>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第84.5話</t>
+          <t>第19話前半</t>
         </is>
       </c>
     </row>
@@ -27881,17 +28923,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>不純な彼女達は懺悔しない</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ポロロッカ(著者)</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第34話</t>
+          <t>第５７話　和解する器用貧乏（１）</t>
         </is>
       </c>
     </row>
@@ -27901,17 +28943,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
+          <t>実は俺、最強でした？</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第3話後編：魔物狩る少女たち</t>
+          <t>第138話　わたくしと戦いませんか？・前編</t>
         </is>
       </c>
     </row>
@@ -27921,17 +28963,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
+          <t>田舎で恋は難しい!?</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>三部べべ(漫画) ねうしとら(原作)</t>
+          <t>ねこうめ(著者)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第6話-2</t>
+          <t>第4話</t>
         </is>
       </c>
     </row>
@@ -27941,17 +28983,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>実は俺、最強でした？</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>原作：澄守 彩 漫画：高橋 愛</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>おまけ69</t>
+          <t>第133話　王都に戻ってみるⅡ（前編）</t>
         </is>
       </c>
     </row>
@@ -27961,17 +29003,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第５６話　勇者を蹂躙する器用貧乏（４）</t>
+          <t>第53話前編</t>
         </is>
       </c>
     </row>
@@ -27981,17 +29023,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>異世界のんびり農家</t>
+          <t>貞操逆転世界で頼めばヤれると噂の俺</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
+          <t>澄田佑貴(漫画) aaa168（スリーエー）(原作)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第316話</t>
+          <t>休載イラスト</t>
         </is>
       </c>
     </row>
@@ -28001,17 +29043,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>「おかえり、パパ」</t>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>蝉丸</t>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第32話　接触</t>
+          <t>第89話　天罰</t>
         </is>
       </c>
     </row>
@@ -28021,17 +29063,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>せっかく農家に転生したので勇者は目指しません</t>
+          <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>マツオカヨシノリ(漫画) 月見里嘉助(原作) ゆーにっと(キャラクター原案)</t>
+          <t>須河篤志(著者)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第2話③</t>
+          <t>休載イラストその２</t>
         </is>
       </c>
     </row>
@@ -28041,17 +29083,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！</t>
+          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>丈(著者)</t>
+          <t>モリタ Ｕ４ nima</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第130話</t>
+          <t>第15話（１）　お嬢様と宰相と、とびきりの滋養食（１）</t>
         </is>
       </c>
     </row>
@@ -28061,17 +29103,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>せっかく農家に転生したので勇者は目指しません</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>マツオカヨシノリ(漫画) 月見里嘉助(原作) ゆーにっと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第36話 独身貴族は生ハムの原木を買う（3）</t>
+          <t>第2話④</t>
         </is>
       </c>
     </row>
@@ -28081,17 +29123,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>物語の黒幕に転生して</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>瀬川はじめ(漫画) 結城涼(原作) なかむら(キャラクター原案)</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第38話</t>
+          <t>第77話④</t>
         </is>
       </c>
     </row>
@@ -28111,7 +29153,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第２７食　コカトリスのフライドチキン、パクパクですわ！（１）</t>
+          <t>第２７食　コカトリスのフライドチキン、パクパクですわ！（２）</t>
         </is>
       </c>
     </row>
@@ -28121,17 +29163,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>アザミヤコを好きになる</t>
+          <t>ぽんドロイド！ はまさん</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+          <t>はれやまはれぞう(著者)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第13話前編</t>
+          <t>第16話</t>
         </is>
       </c>
     </row>
@@ -28141,17 +29183,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第6話後編</t>
+          <t>第36話 独身貴族は生ハムの原木を買う（4）</t>
         </is>
       </c>
     </row>
@@ -28161,17 +29203,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+          <t>聖者無双</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第50話 養殖場見学と蜜の酒③</t>
+          <t>第96話　戦闘準備・消えた魔物の死体①</t>
         </is>
       </c>
     </row>
@@ -28191,7 +29233,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第147話 よくわからないけれど滾るみたいです（１）</t>
+          <t>第147話 よくわからないけれど滾るみたいです（２）</t>
         </is>
       </c>
     </row>
@@ -28201,17 +29243,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>悪友の俺がポンコツ騎士を見てられないんだが、どう世話を焼きゃいい？ ～まどめ外伝～</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>原作：手島史詞 漫画：双葉もも キャラクター原案：COMTA 構成：板垣ハコ</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第60話②　ニコニ坑道の異変を調べてみた</t>
+          <t>第19話</t>
         </is>
       </c>
     </row>
@@ -28221,17 +29263,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+          <t>小林さんちのメイドラゴン</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+          <t>クール教信者</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第11話-1：普通の高校生</t>
+          <t>第159話</t>
         </is>
       </c>
     </row>
@@ -28241,17 +29283,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>田舎で恋は難しい!?</t>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>ねこうめ(著者)</t>
+          <t>板垣恵介 林たかあき</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>許嫁の合歓園寧寧に着てほしいコスプレ大募集!!!!【コメント企画】</t>
+          <t>第63話 同類の香り</t>
         </is>
       </c>
     </row>
@@ -28261,17 +29303,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>美人女上司滝沢さん</t>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>やんBARU(著者)</t>
+          <t>六志麻あさ 業務用餅 kisui</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第212話</t>
+          <t>第８０話</t>
         </is>
       </c>
     </row>
@@ -28281,17 +29323,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>幼女戦記</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>東條チカ(漫画) カルロ・ゼン(原作) 篠月しのぶ(キャラクター原案)</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第百十二章：ドードーバード航空戦Ⅶ</t>
+          <t>第85話その2</t>
         </is>
       </c>
     </row>
@@ -28301,17 +29343,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>異世界食堂　洋食のねこや</t>
+          <t>北斗の拳 世紀末ドラマ撮影伝</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>犬塚惇平(ヒーロー文庫／イマジカインフォス)(原作) ヤミザワ(漫画) モロザワ(漫画) エナミカツミ(キャラクター原案)</t>
+          <t>原案/武論尊・原哲夫 漫画/倉尾宏</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第44話➁</t>
+          <t>第80話 映画北斗、観客の反応!!（後）</t>
         </is>
       </c>
     </row>
@@ -28321,17 +29363,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>男嫌いな美人姉妹を名前も告げずに助けたら一体どうなる?</t>
+          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>みょん(原作) 司馬淳子(漫画) ぎうにう(キャラクターデザイン)</t>
+          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第28話</t>
+          <t>第43話-2</t>
         </is>
       </c>
     </row>
@@ -28341,17 +29383,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第85話その1</t>
+          <t>第４５話　エリーゼ、死す（１）</t>
         </is>
       </c>
     </row>
@@ -28361,17 +29403,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>衛宮さんちの今日のごはん</t>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>TAa(漫画) 只野まこと(料理監修) ＴＹＰＥ－ＭＯＯＮ(原作)</t>
+          <t>三吉汐美(著者)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第78話</t>
+          <t>第20話後半</t>
         </is>
       </c>
     </row>
@@ -28381,17 +29423,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>理想のヒモ生活</t>
+          <t>ヴァージン・キラー忍法帖</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>日月ネコ(漫画) 渡辺恒彦（ヒーロー文庫／イマジカインフォス）(原作) 文倉十(キャラクター原案)</t>
+          <t>成田芋虫</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第104話　その2</t>
+          <t>一之巻</t>
         </is>
       </c>
     </row>
@@ -28401,17 +29443,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>淫獄団地</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>拷問168</t>
+          <t>コミックス告知</t>
         </is>
       </c>
     </row>
@@ -28421,17 +29463,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>くらいあの子としたいこと</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>碇マナツ(著者)</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>第90話</t>
+          <t>拷問169</t>
         </is>
       </c>
     </row>
@@ -28441,17 +29483,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>KAKERU</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第22話②</t>
+          <t>第73話「弓王2」(前半)</t>
         </is>
       </c>
     </row>
@@ -28461,17 +29503,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>異世界でも無難に生きたい症候群</t>
+          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>原作：安泰（一二三書房刊） 漫画：笹峰コウ キャラクター原案：ひたきゆう</t>
+          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第33話④</t>
+          <t>第61話　勇の剣</t>
         </is>
       </c>
     </row>
@@ -28481,17 +29523,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>めっちゃ召喚された件 THE COMIC</t>
+          <t>陰キャの俺が席替えでS級美少女に囲まれたら秘密の関係が始まった。</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>漫画：六甲島カモメ 原作：さいとうさ キャラクター原案：ツグトク</t>
+          <t>星野 星野(原作) バラマツヒトミ(漫画) 黒兎 ゆう(キャラクター原案)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第52話①</t>
+          <t>第10話</t>
         </is>
       </c>
     </row>
@@ -28501,17 +29543,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>地味子な三葉さんが僕を誘惑する</t>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>はぶらえる(著者)</t>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>コミックス告知</t>
+          <t>第38話</t>
         </is>
       </c>
     </row>
@@ -28521,17 +29563,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>世界最高の暗殺者、異世界貴族に転生する</t>
+          <t>ライブダンジョン！</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>月夜涙(原作) 皇ハマオ(漫画) れい亜(キャラクター原案)</t>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第41話-2</t>
+          <t>第93話後半</t>
         </is>
       </c>
     </row>
@@ -28541,17 +29583,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>病弱少女、転生して健康な肉体（最強）を手に入れる</t>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>あらた伊里（漫画） アトハ（原作） 狐印（キャラクター原案）</t>
+          <t>セレビィ量産型(著者)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第2話　フィアナ、模擬戦に挑む（後編）</t>
+          <t>第25話</t>
         </is>
       </c>
     </row>
@@ -28561,17 +29603,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>スキル【万物支配】に目覚めたおっさんは、ダンジョンで生計を立てることにしました～無職から始める支配者無双～</t>
+          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>岸本和葉 原田 臙 シミズヒロノリ 吉武</t>
+          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第10話　ダンジョンの主(後編)</t>
+          <t>第86話後半</t>
         </is>
       </c>
     </row>
@@ -28581,17 +29623,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ひとりぼっちの異世界攻略</t>
+          <t>黄金の経験値</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>びび（漫画） 五示正司（原作）</t>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第255話　複雑な家庭環境…？</t>
+          <t>第22話（後編）</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2026-02-16
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -41,6 +41,7 @@
     <sheet name="2026-01-26" sheetId="33" state="visible" r:id="rId33"/>
     <sheet name="2026-02-02" sheetId="34" state="visible" r:id="rId34"/>
     <sheet name="2026-02-09" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="2026-02-16" sheetId="36" state="visible" r:id="rId36"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -28638,22 +28639,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第131話</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>ワンパンマン</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>220撃目</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>転生したらスライムだった件</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>原作：伏瀬 漫画：川上泰樹 キャラクター原案：みっつばー</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第132話　視察と研究成果</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第36話：クソガキ①</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>魔王の俺が奴隷エルフを嫁にしたんだが、どう愛でればいい？</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>原作／手島史詞 キャラクター原案／COMTA 漫画／板垣ハコ</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第76話</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>蜘蛛ですが、なにか？</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第78話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第７４話『半球停止』⓵</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第7話 後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>王子様の友達</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>すけろく(著者)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>第34話</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第７３話　合評の戦いが始まった（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>立ち飲み居酒屋でクーデレダウナー系女子大生が隣に来る話</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>原作:剃り残し 漫画:大窪太一</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>第1話</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第83話その1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第29話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第19話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第５７話　和解する器用貧乏（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第138話　わたくしと戦いませんか？・前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>田舎で恋は難しい!?</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>ねこうめ(著者)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第4話</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第133話　王都に戻ってみるⅡ（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>まんきつしたい常連さん</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>しんみりん(著者)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第53話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>貞操逆転世界で頼めばヤれると噂の俺</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>澄田佑貴(漫画) aaa168（スリーエー）(原作)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第89話　天罰</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>クセ強彼女は床にいざなう</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>須河篤志(著者)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>休載イラストその２</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>モリタ Ｕ４ nima</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第15話（１）　お嬢様と宰相と、とびきりの滋養食（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>せっかく農家に転生したので勇者は目指しません</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>マツオカヨシノリ(漫画) 月見里嘉助(原作) ゆーにっと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第2話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>リビルドワールド</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第77話④</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第２７食　コカトリスのフライドチキン、パクパクですわ！（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>ぽんドロイド！ はまさん</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>はれやまはれぞう(著者)</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第16話</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第36話 独身貴族は生ハムの原木を買う（4）</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>聖者無双</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>第96話　戦闘準備・消えた魔物の死体①</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第147話 よくわからないけれど滾るみたいです（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>悪友の俺がポンコツ騎士を見てられないんだが、どう世話を焼きゃいい？ ～まどめ外伝～</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>原作：手島史詞 漫画：双葉もも キャラクター原案：COMTA 構成：板垣ハコ</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第19話</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>小林さんちのメイドラゴン</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>クール教信者</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第159話</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>板垣恵介 林たかあき</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第63話 同類の香り</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>六志麻あさ 業務用餅 kisui</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第８０話</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第85話その2</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>北斗の拳 世紀末ドラマ撮影伝</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>原案/武論尊・原哲夫 漫画/倉尾宏</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第80話 映画北斗、観客の反応!!（後）</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第43話-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第４５話　エリーゼ、死す（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>三吉汐美(著者)</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第20話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>ヴァージン・キラー忍法帖</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>成田芋虫</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>一之巻</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>コミックス告知</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>拷問169</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>KAKERU</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第73話「弓王2」(前半)</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第61話　勇の剣</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>陰キャの俺が席替えでS級美少女に囲まれたら秘密の関係が始まった。</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>星野 星野(原作) バラマツヒトミ(漫画) 黒兎 ゆう(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第10話</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第38話</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>ライブダンジョン！</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第93話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>三枝さんはメガネ先輩と恋を描く</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>セレビィ量産型(著者)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>第25話</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第86話後半</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>黄金の経験値</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第22話（後編）</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！</t>
+          <t>転生したらスライムだった件</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>丈(著者)</t>
+          <t>原作：伏瀬 漫画：川上泰樹 キャラクター原案：みっつばー</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第131話</t>
+          <t>第132話　視察と研究成果</t>
         </is>
       </c>
     </row>
@@ -28663,17 +29705,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ワンパンマン</t>
+          <t>魔術師クノンは見えている</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>原作/ＯＮＥ 作画/村田雄介</t>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>220撃目</t>
+          <t>第44話➁</t>
         </is>
       </c>
     </row>
@@ -28683,17 +29725,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>転生したらスライムだった件</t>
+          <t>不徳のギルド</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>原作：伏瀬 漫画：川上泰樹 キャラクター原案：みっつばー</t>
+          <t>河添太一</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第132話　視察と研究成果</t>
+          <t>第１０３話：Let's school</t>
         </is>
       </c>
     </row>
@@ -28713,7 +29755,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第36話：クソガキ①</t>
+          <t>第36話：クソガキ②</t>
         </is>
       </c>
     </row>
@@ -28723,17 +29765,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>魔王の俺が奴隷エルフを嫁にしたんだが、どう愛でればいい？</t>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>原作／手島史詞 キャラクター原案／COMTA 漫画／板垣ハコ</t>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第76話</t>
+          <t>第20話-3「パーフェクトB級冒険者」</t>
         </is>
       </c>
     </row>
@@ -28743,17 +29785,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>蜘蛛ですが、なにか？</t>
+          <t>生徒会にも穴はある！</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>かかし朝浩(著者) 馬場翁(原作) 輝竜司(キャラクター原案)</t>
+          <t>むちまろ</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第78話その1</t>
+          <t>第145話	男3人寄ればえっちじゃん</t>
         </is>
       </c>
     </row>
@@ -28773,7 +29815,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第７４話『半球停止』⓵</t>
+          <t>第７４話『半球停止』②</t>
         </is>
       </c>
     </row>
@@ -28783,17 +29825,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>勇者パーティーをクビになったので故郷に帰ったら、メンバー全員がついてきたんだが</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>絶叫あいす。(漫画) 木の芽(原作) 希(キャラクター原案)</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第7話 後編</t>
+          <t>第７３話　合評の戦いが始まった（２）</t>
         </is>
       </c>
     </row>
@@ -28803,17 +29845,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>王子様の友達</t>
+          <t>帰ってください！ 阿久津さん</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>すけろく(著者)</t>
+          <t>長岡太一(著者)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>第34話</t>
+          <t>番外編㉖</t>
         </is>
       </c>
     </row>
@@ -28823,17 +29865,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第７３話　合評の戦いが始まった（１）</t>
+          <t>第16話-1</t>
         </is>
       </c>
     </row>
@@ -28843,17 +29885,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>立ち飲み居酒屋でクーデレダウナー系女子大生が隣に来る話</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>原作:剃り残し 漫画:大窪太一</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>第1話</t>
+          <t>胃腸がぶっ壊れたため休載イラスト</t>
         </is>
       </c>
     </row>
@@ -28863,17 +29905,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
+          <t>ダンジョンの幼なじみ</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
+          <t>久真やすひさ(著者)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第83話その1</t>
+          <t>第61話</t>
         </is>
       </c>
     </row>
@@ -28883,17 +29925,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>女友達は頼めば意外とヤらせてくれる</t>
+          <t>金属スライムを倒しまくった俺が【黒鋼の王】と呼ばれるまで</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ろくろ(漫画) 鏡遊(原作)</t>
+          <t>藤屋いずこ(著者) 温泉カピバラ(原作) 山椒魚(キャラクター原案)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第29話①</t>
+          <t>第17章-2</t>
         </is>
       </c>
     </row>
@@ -28903,12 +29945,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
+          <t>クセ強彼女は床にいざなう</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
+          <t>須河篤志(著者)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -28933,7 +29975,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第５７話　和解する器用貧乏（１）</t>
+          <t>第５７話　和解する器用貧乏（２）</t>
         </is>
       </c>
     </row>
@@ -28953,7 +29995,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第138話　わたくしと戦いませんか？・前編</t>
+          <t>第138話　わたくしと戦いませんか？・後編</t>
         </is>
       </c>
     </row>
@@ -28963,17 +30005,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>田舎で恋は難しい!?</t>
+          <t>魔のものたちは企てる</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ねこうめ(著者)</t>
+          <t>加藤拓弐(原作) ガしガし(作画)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第4話</t>
+          <t>第34話</t>
         </is>
       </c>
     </row>
@@ -28993,7 +30035,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第133話　王都に戻ってみるⅡ（前編）</t>
+          <t>第133話　王都に戻ってみるⅡ（中編）</t>
         </is>
       </c>
     </row>
@@ -29003,17 +30045,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>まんきつしたい常連さん</t>
+          <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>しんみりん(著者)</t>
+          <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第53話前編</t>
+          <t>第4話前編：大聖堂からの来訪者</t>
         </is>
       </c>
     </row>
@@ -29023,17 +30065,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>貞操逆転世界で頼めばヤれると噂の俺</t>
+          <t>淫獄団地</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>澄田佑貴(漫画) aaa168（スリーエー）(原作)</t>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>休載イラスト</t>
+          <t>第54話</t>
         </is>
       </c>
     </row>
@@ -29043,17 +30085,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
+          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>板垣恵介 猪原賽 陸井栄史</t>
+          <t>夜州 nini 藻</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第89話　天罰</t>
+          <t>第72話(後編)</t>
         </is>
       </c>
     </row>
@@ -29063,17 +30105,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>クセ強彼女は床にいざなう</t>
+          <t>宇崎ちゃんは遊びたい！</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>須河篤志(著者)</t>
+          <t>丈(著者)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>休載イラストその２</t>
+          <t>第131話</t>
         </is>
       </c>
     </row>
@@ -29083,17 +30125,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
+          <t>望まぬ不死の冒険者</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>モリタ Ｕ４ nima</t>
+          <t>中曽根ハイジ（漫画） 丘野 優（原作） じゃいあん（キャラクター原案）</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第15話（１）　お嬢様と宰相と、とびきりの滋養食（１）</t>
+          <t>第63話　一角獣</t>
         </is>
       </c>
     </row>
@@ -29103,17 +30145,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>せっかく農家に転生したので勇者は目指しません</t>
+          <t>美人女上司滝沢さん</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>マツオカヨシノリ(漫画) 月見里嘉助(原作) ゆーにっと(キャラクター原案)</t>
+          <t>やんBARU(著者)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第2話④</t>
+          <t>第213話</t>
         </is>
       </c>
     </row>
@@ -29123,17 +30165,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>リビルドワールド</t>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第77話④</t>
+          <t>第37話 独身貴族は新しい喫茶店に呼ばれる（1）</t>
         </is>
       </c>
     </row>
@@ -29153,7 +30195,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第２７食　コカトリスのフライドチキン、パクパクですわ！（２）</t>
+          <t>第２７食　コカトリスのフライドチキン、パクパクですわ！（３）</t>
         </is>
       </c>
     </row>
@@ -29163,17 +30205,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ぽんドロイド！ はまさん</t>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>はれやまはれぞう(著者)</t>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第16話</t>
+          <t>第45話　奴は巡る（後編）</t>
         </is>
       </c>
     </row>
@@ -29183,17 +30225,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>せっかく農家に転生したので勇者は目指しません</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>マツオカヨシノリ(漫画) 月見里嘉助(原作) ゆーにっと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第36話 独身貴族は生ハムの原木を買う（4）</t>
+          <t>第3話①</t>
         </is>
       </c>
     </row>
@@ -29203,17 +30245,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>聖者無双</t>
+          <t>田舎で恋は難しい!?</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
+          <t>ねこうめ(著者)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>第96話　戦闘準備・消えた魔物の死体①</t>
+          <t>4話おまけ</t>
         </is>
       </c>
     </row>
@@ -29223,17 +30265,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第147話 よくわからないけれど滾るみたいです（２）</t>
+          <t>第61話①　期間限定イベントに参加してみた</t>
         </is>
       </c>
     </row>
@@ -29243,17 +30285,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>悪友の俺がポンコツ騎士を見てられないんだが、どう世話を焼きゃいい？ ～まどめ外伝～</t>
+          <t>路地裏で拾った女の子がバッドエンド後の乙女ゲームのヒロインだった件</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>原作：手島史詞 漫画：双葉もも キャラクター原案：COMTA 構成：板垣ハコ</t>
+          <t>カボチャマスク(原作) 樋乃えなが(作画) へいろー(キャラクター原案)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第19話</t>
+          <t>第6話-1</t>
         </is>
       </c>
     </row>
@@ -29263,17 +30305,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>小林さんちのメイドラゴン</t>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>クール教信者</t>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第159話</t>
+          <t>第11話-2：普通の高校生</t>
         </is>
       </c>
     </row>
@@ -29283,17 +30325,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>板垣恵介 林たかあき</t>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第63話 同類の香り</t>
+          <t>第7話前編</t>
         </is>
       </c>
     </row>
@@ -29303,17 +30345,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>六志麻あさ 業務用餅 kisui</t>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第８０話</t>
+          <t>第50話 養殖場見学と蜜の酒④</t>
         </is>
       </c>
     </row>
@@ -29323,17 +30365,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第85話その2</t>
+          <t>第148話 よくわからないけれど海難事故が起こったようです（１）</t>
         </is>
       </c>
     </row>
@@ -29343,17 +30385,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>北斗の拳 世紀末ドラマ撮影伝</t>
+          <t>アザミヤコを好きになる</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>原案/武論尊・原哲夫 漫画/倉尾宏</t>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第80話 映画北斗、観客の反応!!（後）</t>
+          <t>第13話後編</t>
         </is>
       </c>
     </row>
@@ -29363,17 +30405,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>経験値貯蓄でのんびり傷心旅行 ～勇者と恋人に追放された戦士の無自覚ざまぁ～</t>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>奏ヨシキ(著者) 徳川レモン(原作) riritto(キャラクターデザイン)</t>
+          <t>はぐはぐ(著者)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第43話-2</t>
+          <t>第93話</t>
         </is>
       </c>
     </row>
@@ -29383,17 +30425,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>村上よしゆき 茨木野 あるてら</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第４５話　エリーゼ、死す（１）</t>
+          <t>第85話その3</t>
         </is>
       </c>
     </row>
@@ -29403,17 +30445,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>アイドル辞めるけど結婚してくれますか!?</t>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>三吉汐美(著者)</t>
+          <t>村上よしゆき 茨木野 あるてら</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第20話後半</t>
+          <t>第４５話　エリーゼ、死す（２）</t>
         </is>
       </c>
     </row>
@@ -29423,17 +30465,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ヴァージン・キラー忍法帖</t>
+          <t>お気楽領主の楽しい領地防衛 ～生産系魔術で名もなき村を最強の城塞都市に～</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>成田芋虫</t>
+          <t>青色まろ（漫画） 赤池宗（原作） 転（原作イラスト）</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>一之巻</t>
+          <t>第37話　初めての戦争（前編）</t>
         </is>
       </c>
     </row>
@@ -29443,17 +30485,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>淫獄団地</t>
+          <t>バーサス</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>コミックス告知</t>
+          <t>第31話　小粒との対話（1）</t>
         </is>
       </c>
     </row>
@@ -29473,7 +30515,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>拷問169</t>
+          <t>拷問170</t>
         </is>
       </c>
     </row>
@@ -29483,17 +30525,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
+          <t>立ち飲み居酒屋でクーデレダウナー系女子大生が隣に来る話</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>KAKERU</t>
+          <t>原作:剃り残し 漫画:大窪太一</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第73話「弓王2」(前半)</t>
+          <t>第2話</t>
         </is>
       </c>
     </row>
@@ -29503,17 +30545,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ハズレ枠の【状態異常スキル】で最強になった俺がすべてを蹂躙するまで</t>
+          <t>くらいあの子としたいこと</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>鵜吉しょう（作画） 内々けやき（構成） 篠崎 芳（原作） KWKM（キャラクター原案）</t>
+          <t>碇マナツ(著者)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第61話　勇の剣</t>
+          <t>第91話</t>
         </is>
       </c>
     </row>
@@ -29523,17 +30565,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>陰キャの俺が席替えでS級美少女に囲まれたら秘密の関係が始まった。</t>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>星野 星野(原作) バラマツヒトミ(漫画) 黒兎 ゆう(キャラクター原案)</t>
+          <t>FUNA 東西 モトエ恵介</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第10話</t>
+          <t>第127話　襲撃［その６］</t>
         </is>
       </c>
     </row>
@@ -29543,17 +30585,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
+          <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
+          <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第38話</t>
+          <t>第8話①「1st ハイスクール・イベント」</t>
         </is>
       </c>
     </row>
@@ -29563,17 +30605,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ライブダンジョン！</t>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第93話後半</t>
+          <t>第22話③</t>
         </is>
       </c>
     </row>
@@ -29583,17 +30625,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>三枝さんはメガネ先輩と恋を描く</t>
+          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>セレビィ量産型(著者)</t>
+          <t>三部べべ(漫画) ねうしとら(原作)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>第25話</t>
+          <t>コミックス１巻発売！</t>
         </is>
       </c>
     </row>
@@ -29603,17 +30645,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>魔王になったので、ダンジョン造って人外娘とほのぼのする</t>
+          <t>乙女ゲー世界はモブに厳しい世界です【共和国編】</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>遠野ノオト(作画) 流優(原作) だぶ竜(キャラクター原案)</t>
+          <t>三嶋与夢(原作) 行々狸(作画) 孟達(キャラクター原案) マツリセイシロウ(構成) FTops(制作)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第86話後半</t>
+          <t>第6話</t>
         </is>
       </c>
     </row>
@@ -29623,17 +30665,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>黄金の経験値</t>
+          <t>俺は星間国家の悪徳領主！</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>原純(原作) 霜月汐(作画) fixro2n(キャラクター原案)</t>
+          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第22話（後編）</t>
+          <t>第45話　暇すぎる!!</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ranking data for 2026-02-23
</commit_message>
<xml_diff>
--- a/ranking_weekly.xlsx
+++ b/ranking_weekly.xlsx
@@ -42,6 +42,7 @@
     <sheet name="2026-02-02" sheetId="34" state="visible" r:id="rId34"/>
     <sheet name="2026-02-09" sheetId="35" state="visible" r:id="rId35"/>
     <sheet name="2026-02-16" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="2026-02-23" sheetId="37" state="visible" r:id="rId37"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -29680,22 +29681,1063 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>転生したらスライムだった件</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>原作：伏瀬 漫画：川上泰樹 キャラクター原案：みっつばー</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>第132話　視察と研究成果</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>魔術師クノンは見えている</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>第44話➁</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>不徳のギルド</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>河添太一</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>第１０３話：Let's school</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>第36話：クソガキ②</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>第20話-3「パーフェクトB級冒険者」</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>生徒会にも穴はある！</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>むちまろ</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>第145話	男3人寄ればえっちじゃん</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>光永康則</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>第７４話『半球停止』②</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>マツモトケンゴ</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>第７３話　合評の戦いが始まった（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>帰ってください！ 阿久津さん</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>長岡太一(著者)</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>番外編㉖</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>第16話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>いとこのこ</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>いぬちく(著者)</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>胃腸がぶっ壊れたため休載イラスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>ダンジョンの幼なじみ</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>久真やすひさ(著者)</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>第61話</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>金属スライムを倒しまくった俺が【黒鋼の王】と呼ばれるまで</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>藤屋いずこ(著者) 温泉カピバラ(原作) 山椒魚(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>第17章-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>クセ強彼女は床にいざなう</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>須河篤志(著者)</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>第19話前半</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>第５７話　和解する器用貧乏（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>実は俺、最強でした？</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>原作：澄守 彩 漫画：高橋 愛</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>第138話　わたくしと戦いませんか？・後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>魔のものたちは企てる</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>加藤拓弐(原作) ガしガし(作画)</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>第34話</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>第133話　王都に戻ってみるⅡ（中編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>第4話前編：大聖堂からの来訪者</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>淫獄団地</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>第54話</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>夜州 nini 藻</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>第72話(後編)</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>宇崎ちゃんは遊びたい！</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>丈(著者)</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>第131話</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>望まぬ不死の冒険者</t>
+        </is>
+      </c>
+      <c r="C24" s="0" t="inlineStr">
+        <is>
+          <t>中曽根ハイジ（漫画） 丘野 優（原作） じゃいあん（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>第63話　一角獣</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>美人女上司滝沢さん</t>
+        </is>
+      </c>
+      <c r="C25" s="0" t="inlineStr">
+        <is>
+          <t>やんBARU(著者)</t>
+        </is>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>第213話</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+        </is>
+      </c>
+      <c r="C26" s="0" t="inlineStr">
+        <is>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+        </is>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>第37話 独身貴族は新しい喫茶店に呼ばれる（1）</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+        </is>
+      </c>
+      <c r="C27" s="0" t="inlineStr">
+        <is>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
+        </is>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>第２７食　コカトリスのフライドチキン、パクパクですわ！（３）</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+        </is>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>第45話　奴は巡る（後編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>せっかく農家に転生したので勇者は目指しません</t>
+        </is>
+      </c>
+      <c r="C29" s="0" t="inlineStr">
+        <is>
+          <t>マツオカヨシノリ(漫画) 月見里嘉助(原作) ゆーにっと(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>第3話①</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>田舎で恋は難しい!?</t>
+        </is>
+      </c>
+      <c r="C30" s="0" t="inlineStr">
+        <is>
+          <t>ねこうめ(著者)</t>
+        </is>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>4話おまけ</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
+          <t>戸賀 環 坂木持丸 riritto</t>
+        </is>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>第61話①　期間限定イベントに参加してみた</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>路地裏で拾った女の子がバッドエンド後の乙女ゲームのヒロインだった件</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
+          <t>カボチャマスク(原作) 樋乃えなが(作画) へいろー(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>第6話-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
+          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>第11話-2：普通の高校生</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
+          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>第7話前編</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
+          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+        </is>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>第50話 養殖場見学と蜜の酒④</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>よくわからないけれど異世界に転生していたようです</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
+          <t>内々けやき あし カオミン</t>
+        </is>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>第148話 よくわからないけれど海難事故が起こったようです（１）</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>アザミヤコを好きになる</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
+          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+        </is>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>第13話後編</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>サーシャちゃんとクラスメイトオタクくん</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
+          <t>はぐはぐ(著者)</t>
+        </is>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>第93話</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>第85話その3</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>落ちこぼれだった兄が実は最強 ～史上最強の勇者は転生し、学園で無自覚に無双する～</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
+          <t>村上よしゆき 茨木野 あるてら</t>
+        </is>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>第４５話　エリーゼ、死す（２）</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>お気楽領主の楽しい領地防衛 ～生産系魔術で名もなき村を最強の城塞都市に～</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>青色まろ（漫画） 赤池宗（原作） 転（原作イラスト）</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>第37話　初めての戦争（前編）</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>バーサス</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
+          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+        </is>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>第31話　小粒との対話（1）</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>姫様“拷問”の時間です</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+        </is>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>拷問170</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>立ち飲み居酒屋でクーデレダウナー系女子大生が隣に来る話</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
+          <t>原作:剃り残し 漫画:大窪太一</t>
+        </is>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>第2話</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>くらいあの子としたいこと</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
+          <t>碇マナツ(著者)</t>
+        </is>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>第91話</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>FUNA 東西 モトエ恵介</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>第127話　襲撃［その６］</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
+          <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
+        </is>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>第8話①「1st ハイスクール・イベント」</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
+          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+        </is>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>第22話③</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
+          <t>三部べべ(漫画) ねうしとら(原作)</t>
+        </is>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>コミックス１巻発売！</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>乙女ゲー世界はモブに厳しい世界です【共和国編】</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
+          <t>三嶋与夢(原作) 行々狸(作画) 孟達(キャラクター原案) マツリセイシロウ(構成) FTops(制作)</t>
+        </is>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>第6話</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>俺は星間国家の悪徳領主！</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
+          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
+        </is>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>第45話　暇すぎる!!</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>latest_episode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>転生したらスライムだった件</t>
+          <t>ワンパンマン</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>原作：伏瀬 漫画：川上泰樹 キャラクター原案：みっつばー</t>
+          <t>原作/ＯＮＥ 作画/村田雄介</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>第132話　視察と研究成果</t>
+          <t>221撃目</t>
         </is>
       </c>
     </row>
@@ -29705,17 +30747,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>魔術師クノンは見えている</t>
+          <t>異種族レビュアーズ</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>La-na(作画) 南野海風(原作) Ｌａｒｕｈａ(キャラクター原案)</t>
+          <t>天原(原作) masha(作画)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>第44話➁</t>
+          <t>第90話</t>
         </is>
       </c>
     </row>
@@ -29725,17 +30767,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>不徳のギルド</t>
+          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>河添太一</t>
+          <t>zunta(作画) はらわたさいぞう(原作)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>第１０３話：Let's school</t>
+          <t>第36話：クソガキ③</t>
         </is>
       </c>
     </row>
@@ -29745,17 +30787,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>転生コロシアム～最弱スキルで最強の女たちを攻略して奴隷ハーレム作ります～</t>
+          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>zunta(作画) はらわたさいぞう(原作)</t>
+          <t>光永康則</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>第36話：クソガキ②</t>
+          <t>第７４話『半球停止』③</t>
         </is>
       </c>
     </row>
@@ -29765,17 +30807,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>悪人面したＢ級冒険者 主人公とその幼馴染たちのパパになる</t>
+          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>こげめ(著者) えんじ(原作) ハラカズヒロ(キャラクター原案)</t>
+          <t>マツモトケンゴ</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>第20話-3「パーフェクトB級冒険者」</t>
+          <t>第７４話　黒板アートの戦いが始まった（１）</t>
         </is>
       </c>
     </row>
@@ -29785,17 +30827,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>生徒会にも穴はある！</t>
+          <t>クラスで２番目に可愛い女の子と友だちになった</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>むちまろ</t>
+          <t>尾野凛(漫画) たかた(原作) 日向あずり(キャラクター原案)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>第145話	男3人寄ればえっちじゃん</t>
+          <t>第38話②</t>
         </is>
       </c>
     </row>
@@ -29805,17 +30847,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>時間停止勇者―余命３日の設定じゃ世界を救うには短すぎる―</t>
+          <t>いとこのこ</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>光永康則</t>
+          <t>いぬちく(著者)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>第７４話『半球停止』②</t>
+          <t>第46話</t>
         </is>
       </c>
     </row>
@@ -29825,17 +30867,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>地元のいじめっ子達に仕返ししようとしたら、別の戦いが始まった。</t>
+          <t>元・世界１位のサブキャラ育成日記 ～廃プレイヤー、異世界を攻略中！～</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>マツモトケンゴ</t>
+          <t>沢村治太郎(原作) 前田理想(漫画) まろ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>第７３話　合評の戦いが始まった（２）</t>
+          <t>第83話その2</t>
         </is>
       </c>
     </row>
@@ -29845,17 +30887,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>帰ってください！ 阿久津さん</t>
+          <t>貞操逆転世界で頼めばヤれると噂の俺</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>長岡太一(著者)</t>
+          <t>澄田佑貴(漫画) aaa168（スリーエー）(原作)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>番外編㉖</t>
+          <t>第6話</t>
         </is>
       </c>
     </row>
@@ -29865,17 +30907,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>男女比1：5の世界でも普通に生きられると思った？　～激重感情な彼女たちが無自覚男子に翻弄されたら～</t>
+          <t>このヒーラー、めんどくさい</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>三藤 孝太郎(原作) 桃季憂(漫画) jimmy(キャラクター原案)</t>
+          <t>丹念に発酵(著者)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>第16話-1</t>
+          <t>第94話：審査</t>
         </is>
       </c>
     </row>
@@ -29885,17 +30927,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>いとこのこ</t>
+          <t>怠惰な悪辱貴族に転生した俺、シナリオをぶっ壊したら規格外の魔力で最凶になった</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>いぬちく(著者)</t>
+          <t>菊池快晴(原作) 小田童馬(作画) 桑島黎音(キャラクター原案)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>胃腸がぶっ壊れたため休載イラスト</t>
+          <t>第19話後半</t>
         </is>
       </c>
     </row>
@@ -29905,17 +30947,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ダンジョンの幼なじみ</t>
+          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>久真やすひさ(著者)</t>
+          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>第61話</t>
+          <t>第５７話　和解する器用貧乏（３）</t>
         </is>
       </c>
     </row>
@@ -29925,17 +30967,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>金属スライムを倒しまくった俺が【黒鋼の王】と呼ばれるまで</t>
+          <t>バキ外伝 烈海王は異世界転生しても一向にかまわんッッ</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>藤屋いずこ(著者) 温泉カピバラ(原作) 山椒魚(キャラクター原案)</t>
+          <t>板垣恵介 猪原賽 陸井栄史</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>第17章-2</t>
+          <t>第90話　初体験(はじめて)</t>
         </is>
       </c>
     </row>
@@ -29945,17 +30987,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>クセ強彼女は床にいざなう</t>
+          <t>辺境モブ貴族のウチに嫁いできた悪役令嬢が、めちゃくちゃできる良い嫁なんだが？</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>須河篤志(著者)</t>
+          <t>tera(原作) 朝倉はやて(作画) 徹田(キャラクター原案)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>第19話前半</t>
+          <t>第14話-2</t>
         </is>
       </c>
     </row>
@@ -29965,17 +31007,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>勇者パーティを追い出された器用貧乏　～パーティ事情で付与術士をやっていた剣士、万能へと至る～</t>
+          <t>不純な彼女達は懺悔しない</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>漫画：よねぞう 原作：都神樹 キャラクター原案：きさらぎゆり</t>
+          <t>ポロロッカ(著者)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>第５７話　和解する器用貧乏（２）</t>
+          <t>第35話</t>
         </is>
       </c>
     </row>
@@ -29995,7 +31037,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>第138話　わたくしと戦いませんか？・後編</t>
+          <t>第139話　イリスVS.フレイ・前編</t>
         </is>
       </c>
     </row>
@@ -30005,17 +31047,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>魔のものたちは企てる</t>
+          <t>異世界魔王と召喚少女の奴隷魔術</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>加藤拓弐(原作) ガしガし(作画)</t>
+          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>第34話</t>
+          <t>第133話　王都に戻ってみるⅡ（後編）</t>
         </is>
       </c>
     </row>
@@ -30025,17 +31067,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>異世界魔王と召喚少女の奴隷魔術</t>
+          <t>異世界のんびり農家</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>原作：むらさきゆきや 漫画：福田直叶 キャラクター原案：鶴崎貴大</t>
+          <t>剣康之(作画) 内藤騎之介(原作) やすも(キャラクター原案)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>第133話　王都に戻ってみるⅡ（中編）</t>
+          <t>第317話</t>
         </is>
       </c>
     </row>
@@ -30045,17 +31087,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>全滅エンドを死に物狂いで回避した。パーティが病んだ。</t>
+          <t>女友達は頼めば意外とヤらせてくれる</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>縞(漫画) 雨糸雀(原作) kodamazon(キャラクター原案)</t>
+          <t>ろくろ(漫画) 鏡遊(原作)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>第4話前編：大聖堂からの来訪者</t>
+          <t>第29話②</t>
         </is>
       </c>
     </row>
@@ -30065,17 +31107,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>淫獄団地</t>
+          <t>まんきつしたい常連さん</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>搾精研究所(原作) 丈山雄為(漫画)</t>
+          <t>しんみりん(著者)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>第54話</t>
+          <t>第53話後編</t>
         </is>
       </c>
     </row>
@@ -30085,17 +31127,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>転生貴族の異世界冒険録 ～自重を知らない神々の使徒～</t>
+          <t>え、社内システム全てワンオペしている私を解雇ですか？</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>夜州 nini 藻</t>
+          <t>漫画：伊於 原作：下城米雪 キャラクター原案：icchi</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>第72話(後編)</t>
+          <t>第36話</t>
         </is>
       </c>
     </row>
@@ -30105,17 +31147,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>宇崎ちゃんは遊びたい！</t>
+          <t>ダークサモナーとデキている</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>丈(著者)</t>
+          <t>車王(著者)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>第131話</t>
+          <t>重大告知！</t>
         </is>
       </c>
     </row>
@@ -30125,17 +31167,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>望まぬ不死の冒険者</t>
+          <t>Ｓ級ギルドを追放されたけど、実は俺だけドラゴンの言葉がわかるので、気付いたときには竜騎士の頂点を極めてました。</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>中曽根ハイジ（漫画） 丘野 優（原作） じゃいあん（キャラクター原案）</t>
+          <t>ひそな(漫画) 三木なずな(原作) 白狼(キャラクター原案)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>第63話　一角獣</t>
+          <t>第42話-2</t>
         </is>
       </c>
     </row>
@@ -30145,17 +31187,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>美人女上司滝沢さん</t>
+          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>やんBARU(著者)</t>
+          <t>島知宏 音速炒飯 有都あらゆる</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>第213話</t>
+          <t>第２７食　コカトリスのフライドチキン、パクパクですわ！（３）</t>
         </is>
       </c>
     </row>
@@ -30165,17 +31207,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
+          <t>リビルドワールド</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
+          <t>綾村切人(漫画) ナフセ(原作) 吟(キャラクターデザイン) わいっしゅ(世界観デザイン) cell(メカニックデザイン)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>第37話 独身貴族は新しい喫茶店に呼ばれる（1）</t>
+          <t>第78話①</t>
         </is>
       </c>
     </row>
@@ -30185,17 +31227,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>【パクパクですわ】追放されたお嬢様の『モンスターを食べるほど強くなる』スキルは、１食で１レベルアップする前代未聞の最強スキルでした。３日で人類最強になりましたわ～！</t>
+          <t>独身貴族は異世界を謳歌する ～結婚しない男の優雅なおひとりさまライフ～</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>島知宏 音速炒飯 有都あらゆる</t>
+          <t>漫画：駒鳥 ひわ 原作：錬金王 キャラクター原案：三登 いつき</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>第２７食　コカトリスのフライドチキン、パクパクですわ！（３）</t>
+          <t>第37話 独身貴族は新しい喫茶店に呼ばれる（2）</t>
         </is>
       </c>
     </row>
@@ -30205,17 +31247,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>「ククク……。奴は四天王の中でも最弱」と解雇された俺、なぜか勇者と聖女の師匠になる</t>
+          <t>せっかく農家に転生したので勇者は目指しません</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>漫画：芳橋アツシ 原作：延野正行 キャラクター原案：坂野杏梨</t>
+          <t>マツオカヨシノリ(漫画) 月見里嘉助(原作) ゆーにっと(キャラクター原案)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>第45話　奴は巡る（後編）</t>
+          <t>第3話②</t>
         </is>
       </c>
     </row>
@@ -30225,17 +31267,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>せっかく農家に転生したので勇者は目指しません</t>
+          <t>異世界メイドの三ツ星グルメ ～現代ごはん作ったら王宮で大バズリしました～</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>マツオカヨシノリ(漫画) 月見里嘉助(原作) ゆーにっと(キャラクター原案)</t>
+          <t>モリタ Ｕ４ nima</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>第3話①</t>
+          <t>第15話（２）　お嬢様と宰相と、とびきりの滋養食（２）</t>
         </is>
       </c>
     </row>
@@ -30245,17 +31287,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>田舎で恋は難しい!?</t>
+          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ねこうめ(著者)</t>
+          <t>戸賀 環 坂木持丸 riritto</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>4話おまけ</t>
+          <t>第61話②　期間限定イベントに参加してみた</t>
         </is>
       </c>
     </row>
@@ -30265,17 +31307,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>世界最強の魔女、始めました 〜私だけ『攻略サイト』を見れる世界で自由に生きます〜</t>
+          <t>勇者の元仲間夫婦は田舎でのんびり幸せに暮らす</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>戸賀 環 坂木持丸 riritto</t>
+          <t>薊マスラオ(漫画) 相野仁(原作) nima(キャラクター原案)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>第61話①　期間限定イベントに参加してみた</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -30285,17 +31327,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>路地裏で拾った女の子がバッドエンド後の乙女ゲームのヒロインだった件</t>
+          <t>骸骨騎士様、只今異世界へお出掛け中</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>カボチャマスク(原作) 樋乃えなが(作画) へいろー(キャラクター原案)</t>
+          <t>サワノアキラ（漫画） 秤猿鬼（原作） KeG（キャラクター原案）</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>第6話-1</t>
+          <t>第66話　エルフ族の決断Ⅴ</t>
         </is>
       </c>
     </row>
@@ -30305,17 +31347,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>願ってもない追放後からのスローライフ？ 〜引退したはずが成り行きで美少女ギャルの師匠になったらなぜかめちゃくちゃ懐かれた〜</t>
+          <t>姫様“拷問”の時間です</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ヤミーゴ(漫画) シュガースプーン。（GA文庫/SBクリエイティブ）(原作) なたーしゃ(キャラクター原案)</t>
+          <t>原作:春原ロビンソン　漫画:ひらけい</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>第11話-2：普通の高校生</t>
+          <t>拷問171</t>
         </is>
       </c>
     </row>
@@ -30325,17 +31367,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>配信に致命的に向いていない女の子が迷宮で黙々と人助けする配信</t>
+          <t>聖者無双</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>下田将也(漫画) 佐藤悪糖(原作) 福きつね(キャラクター原案)</t>
+          <t>漫画：秋風緋色 原作：ブロッコリーライオン キャラクター原案：sime</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>第7話前編</t>
+          <t>第96話　戦闘準備・消えた魔物の死体②</t>
         </is>
       </c>
     </row>
@@ -30345,17 +31387,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>魔導具師ダリヤはうつむかない ～Dahliya Wilts No More～</t>
+          <t>よくわからないけれど異世界に転生していたようです</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>漫画：住川惠 原作：甘岸久弥(｢魔導具師ダリヤはうつむかない ～今日から自由な職人ライフ～｣MFブックス刊) キャラクター原案：景、駒田ハチ</t>
+          <t>内々けやき あし カオミン</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>第50話 養殖場見学と蜜の酒④</t>
+          <t>第148話 よくわからないけれど海難事故が起こったようです（２）</t>
         </is>
       </c>
     </row>
@@ -30365,17 +31407,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>よくわからないけれど異世界に転生していたようです</t>
+          <t>バキ外伝　ガイアとシコルスキー　～ときどきノムラ 二人だけど三人暮らし～</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>内々けやき あし カオミン</t>
+          <t>板垣恵介 林たかあき</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>第148話 よくわからないけれど海難事故が起こったようです（１）</t>
+          <t>第64話 十字傷</t>
         </is>
       </c>
     </row>
@@ -30385,17 +31427,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>アザミヤコを好きになる</t>
+          <t>お気楽領主の楽しい領地防衛 ～生産系魔術で名もなき村を最強の城塞都市に～</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>ユニティコング(原作) ツノニガウ(作画)</t>
+          <t>青色まろ（漫画） 赤池宗（原作） 転（原作イラスト）</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>第13話後編</t>
+          <t>第37話　初めての戦争（後編）</t>
         </is>
       </c>
     </row>
@@ -30405,17 +31447,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>サーシャちゃんとクラスメイトオタクくん</t>
+          <t>ふかふかダンジョン攻略記～俺の異世界転生冒険譚～</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>はぐはぐ(著者)</t>
+          <t>KAKERU</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>第93話</t>
+          <t>第73話「弓王2」（後半）</t>
         </is>
       </c>
     </row>
@@ -30425,17 +31467,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
+          <t>小林さんちのメイドラゴン</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
+          <t>クール教信者</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>第85話その3</t>
+          <t>第160話</t>
         </is>
       </c>
     </row>
@@ -30455,7 +31497,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>第４５話　エリーゼ、死す（２）</t>
+          <t>第４５話　エリーゼ、死す（３）</t>
         </is>
       </c>
     </row>
@@ -30465,17 +31507,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>お気楽領主の楽しい領地防衛 ～生産系魔術で名もなき村を最強の城塞都市に～</t>
+          <t>治癒魔法の間違った使い方 ~戦場を駆ける回復要員~</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>青色まろ（漫画） 赤池宗（原作） 転（原作イラスト）</t>
+          <t>九我山レキ(漫画) くろかた(原作) ＫｅＧ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>第37話　初めての戦争（前編）</t>
+          <t>第85話その4</t>
         </is>
       </c>
     </row>
@@ -30485,17 +31527,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>バーサス</t>
+          <t>アイドル辞めるけど結婚してくれますか!?</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>原作：ONE 漫画：あずま京太郎 構成：bose</t>
+          <t>三吉汐美(著者)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>第31話　小粒との対話（1）</t>
+          <t>第21話前半</t>
         </is>
       </c>
     </row>
@@ -30505,17 +31547,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>姫様“拷問”の時間です</t>
+          <t>追放されたチート付与魔術師は 気ままなセカンドライフを謳歌する。</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>原作:春原ロビンソン　漫画:ひらけい</t>
+          <t>六志麻あさ 業務用餅 kisui</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>拷問170</t>
+          <t>第８１話</t>
         </is>
       </c>
     </row>
@@ -30525,17 +31567,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>立ち飲み居酒屋でクーデレダウナー系女子大生が隣に来る話</t>
+          <t>北斗の拳 世紀末ドラマ撮影伝</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>原作:剃り残し 漫画:大窪太一</t>
+          <t>原案/武論尊・原哲夫 漫画/倉尾宏</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>第2話</t>
+          <t>第81話 テレビドラマ、撮影再開!!</t>
         </is>
       </c>
     </row>
@@ -30545,17 +31587,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>くらいあの子としたいこと</t>
+          <t>遊び人な少女たちは今日も放課後ヤっている</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>碇マナツ(著者)</t>
+          <t>逢上おかき(著者)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>第91話</t>
+          <t>第1話</t>
         </is>
       </c>
     </row>
@@ -30565,17 +31607,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>老後に備えて異世界で８万枚の金貨を貯めます</t>
+          <t>異世界のすみっこで快適ものづくり生活 ～女神さまのくれた工房はちょっとやりすぎ性能だった～</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>FUNA 東西 モトエ恵介</t>
+          <t>西山アラタ(漫画) 長田信織(原作) 東上文(キャラクター原案)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>第127話　襲撃［その６］</t>
+          <t>EP.24②</t>
         </is>
       </c>
     </row>
@@ -30585,17 +31627,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>彼女にしたい女子一位、の隣で見つけたあまりちゃん</t>
+          <t>ゲーム悪役貴族に転生した俺は、チート筋肉で無双する</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>寝巻ネルゾ(漫画) 裕時悠示(原作) たん旦(キャラクター原案)</t>
+          <t>昼行燈（原作） しいたけ元帥（漫画）</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>第8話①「1st ハイスクール・イベント」</t>
+          <t>第39話</t>
         </is>
       </c>
     </row>
@@ -30605,17 +31647,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>十年目、帰還を諦めた転移者はいまさら主人公になる</t>
+          <t>モブ司祭だけど、この世界が乙女ゲームだと気づいたのでヒロインを育成します</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>原作：氷純（「十年目、帰還を諦めた転移者はいまさら主人公になる」MFブックス刊） 漫画：しゅーかま キャラクター原案：あんべよしろう</t>
+          <t>井冬良(漫画) レオナールＤ(原作) りいちゅ(キャラクター原案)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>第22話③</t>
+          <t>第6話-2：聖務のお手伝い</t>
         </is>
       </c>
     </row>
@@ -30625,17 +31667,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ゲーム世界で魔物に転生してしまった俺、前世で推しだったヒロインを拾ってしまう</t>
+          <t>ライブダンジョン！</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>三部べべ(漫画) ねうしとら(原作)</t>
+          <t>ことりりょう(作画) dy冷凍(原作) Mika Pikazo(キャラクター原案)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>コミックス１巻発売！</t>
+          <t>第94話前半</t>
         </is>
       </c>
     </row>
@@ -30645,17 +31687,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>乙女ゲー世界はモブに厳しい世界です【共和国編】</t>
+          <t>婚約者に裏切られた錬金術師は、独立して『ざまぁ』します　コミック版</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>三嶋与夢(原作) 行々狸(作画) 孟達(キャラクター原案) マツリセイシロウ(構成) FTops(制作)</t>
+          <t>漫画/すたひろ 原作/Y.A</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>第6話</t>
+          <t>chapter80【42話①】</t>
         </is>
       </c>
     </row>
@@ -30665,17 +31707,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>俺は星間国家の悪徳領主！</t>
+          <t>最弱貴族に転生したので悪役たちを集めてみた</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>灘島かい（漫画） 三嶋与夢（原作） 高峰ナダレ（キャラクター原案）</t>
+          <t>空野進 sorani ファルまろ</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>第45話　暇すぎる!!</t>
+          <t>第17話　最弱貴族、魔王を住まわせる（２）</t>
         </is>
       </c>
     </row>

</xml_diff>